<commit_message>
updated myodds for weekend matches
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitboyzorro5\FDAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard.000\gitboyzorro5\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -553,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F35"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0.69168651753599997</v>
+        <v>1.35759955878</v>
       </c>
       <c r="B1" s="1">
-        <v>0.67126455536000007</v>
+        <v>1.0979737029000001</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
@@ -585,10 +585,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.0306989692999999</v>
+        <v>1.0182663357300001</v>
       </c>
       <c r="B2" s="1">
-        <v>1.3760679743999997</v>
+        <v>0.18299561715000004</v>
       </c>
       <c r="C2" s="3">
         <f t="shared" ref="C2:C4" si="0">ROUND(A2,0)</f>
@@ -596,58 +596,58 @@
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2:D4" si="1">ROUND(B2,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2:E4" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(E2,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.15787144852199997</v>
+        <v>1.368983621678</v>
       </c>
       <c r="B3" s="1">
-        <v>1.113598953216</v>
+        <v>1.171961887136</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
+        <v>1</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
         <v>1</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>0-1</v>
+        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
+        <v>1-1</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.75944222323199995</v>
+        <v>1.116715328388</v>
       </c>
       <c r="B4" s="1">
-        <v>0.97134217194799988</v>
+        <v>0.66578103801599997</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E4" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1-1</v>
       </c>
       <c r="F4" s="2" t="str">
@@ -657,22 +657,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2.6688411925560001</v>
+        <v>1.5861402179199999</v>
       </c>
       <c r="B5" s="1">
-        <v>0.41377048157699997</v>
+        <v>1.0999469951359999</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" ref="C5:C7" si="3">ROUND(A5,0)</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D7" si="4">ROUND(B5,0)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="E5" s="4" t="str">
-        <f t="shared" ref="E5:E35" si="5">CONCATENATE(C5,"-",D5)</f>
-        <v>3-0</v>
+        <f t="shared" si="5"/>
+        <v>2-1</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -681,70 +681,70 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1.012663620738</v>
+        <v>2.0355953287640003</v>
       </c>
       <c r="B6" s="1">
-        <v>1.9310713363469998</v>
+        <v>0.64014843471999994</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ref="C6:C35" si="6">ROUND(A6,0)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ref="D6:D35" si="7">ROUND(B6,0)</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>2-1</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.50206813826399999</v>
+        <v>1.2110463756000001</v>
       </c>
       <c r="B7" s="1">
-        <v>1.8193280665049998</v>
+        <v>0.48230499668999999</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-0</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1.3117519356480001</v>
+        <v>0.28718364396000007</v>
       </c>
       <c r="B8" s="1">
-        <v>1.1676005337599997</v>
+        <v>0.29790773050500002</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-0</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -753,46 +753,46 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>3.7169066721599995</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1">
-        <v>1.4296706222399995</v>
+        <v>0.49650454992600002</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>4-1</v>
+        <v>0-0</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>VLOOKUP(E9,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2.3685370243919994</v>
+        <v>2.440538582301</v>
       </c>
       <c r="B10" s="1">
-        <v>0.55602746639999989</v>
+        <v>0.37215979945600003</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>2-0</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -801,46 +801,46 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.6053164430919997</v>
+        <v>0.13560769936799999</v>
       </c>
       <c r="B11" s="1">
-        <v>0.56295638009999993</v>
+        <v>0.93033282723199995</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-1</v>
+        <v>0-1</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>VLOOKUP(E11,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.02028880448</v>
+        <v>2.0337488194229998</v>
       </c>
       <c r="B12" s="1">
-        <v>2.3349820204999996</v>
+        <v>3.3490381786000003</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>2-3</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -849,41 +849,41 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.6836715803</v>
+        <v>0.65705341415999996</v>
       </c>
       <c r="B13" s="1">
-        <v>1.011821166856</v>
+        <v>0.86802068320000003</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>VLOOKUP(E13,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.1099830658400001</v>
+        <v>0.51190794143999996</v>
       </c>
       <c r="B14" s="1">
-        <v>1.2642132247360001</v>
+        <v>0.93267412731199995</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E14" s="4" t="str">
@@ -897,17 +897,17 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2.046454112028</v>
+        <v>2.1236991131199998</v>
       </c>
       <c r="B15" s="1">
-        <v>1.1129232818680002</v>
+        <v>1.271754113456</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E15" s="4" t="str">
@@ -921,41 +921,41 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>0.93025853503200018</v>
+        <v>0.71308630847999999</v>
       </c>
       <c r="B16" s="1">
-        <v>2.0859781864000002</v>
+        <v>0.8287412704999999</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>VLOOKUP(E16,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>0.87462510101999991</v>
+        <v>1.4559720447999998</v>
       </c>
       <c r="B17" s="1">
-        <v>1.5726491135999996</v>
+        <v>1.5041424908249998</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E17" s="4" t="str">
@@ -969,41 +969,41 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.147926992256</v>
+        <v>1.7680160534400002</v>
       </c>
       <c r="B18" s="1">
-        <v>1.3552812332999997</v>
+        <v>1.0505185652</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E18" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F18" s="2" t="str">
         <f>VLOOKUP(E18,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.3742129114999999</v>
+        <v>1.0696794617599998</v>
       </c>
       <c r="B19" s="1">
-        <v>0.64334606543999984</v>
+        <v>1.074330348975</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E19" s="4" t="str">
@@ -1017,89 +1017,89 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1.052161447392</v>
+        <v>0.46216890262899996</v>
       </c>
       <c r="B20" s="1">
-        <v>0.89390040863999998</v>
+        <v>0.76402158299999989</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-1</v>
       </c>
       <c r="F20" s="2" t="str">
         <f>VLOOKUP(E20,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1.2239408674499996</v>
+        <v>0.79233716664199993</v>
       </c>
       <c r="B21" s="1">
-        <v>1.4619228064000001</v>
+        <v>0.40928933987499999</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F21" s="2" t="str">
         <f>VLOOKUP(E21,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.482775474488</v>
+        <v>0.576712865706</v>
       </c>
       <c r="B22" s="1">
-        <v>1.2530338363200002</v>
+        <v>1.7605344776320002</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="E22" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F22" s="2" t="str">
         <f>VLOOKUP(E22,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1.2709789776599998</v>
+        <v>1.4765451456000001</v>
       </c>
       <c r="B23" s="1">
-        <v>0.78324197952000019</v>
+        <v>0.97046481486000025</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E23" s="4" t="str">
@@ -1113,41 +1113,41 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>0.41447504709999994</v>
+        <v>2.1118918950000003</v>
       </c>
       <c r="B24" s="1">
-        <v>3.2478755175980005</v>
+        <v>0.83598609731999995</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="7"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-3</v>
+        <v>2-1</v>
       </c>
       <c r="F24" s="2" t="str">
         <f>VLOOKUP(E24,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0.78761823272600007</v>
+        <v>0.8348066784</v>
       </c>
       <c r="B25" s="1">
-        <v>1.2916387626450001</v>
+        <v>1.238049235344</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E25" s="4" t="str">
@@ -1161,46 +1161,46 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>0.90443064624000002</v>
+        <v>0.93705474869999994</v>
       </c>
       <c r="B26" s="1">
-        <v>0.60706017362599995</v>
+        <v>1.6124270327450001</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="E26" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F26" s="2" t="str">
         <f>VLOOKUP(E26,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1.3604523346560002</v>
+        <v>1.7633965244999998</v>
       </c>
       <c r="B27" s="1">
-        <v>0.34768636415599996</v>
+        <v>0.79622631909699992</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>2-1</v>
       </c>
       <c r="F27" s="2" t="str">
         <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1209,41 +1209,41 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>0.5396673929400001</v>
+        <v>0.96904108560000002</v>
       </c>
       <c r="B28" s="1">
-        <v>0.85360535979600005</v>
+        <v>1.75207740989</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F28" s="2" t="str">
         <f>VLOOKUP(E28,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>1.877891167824</v>
+        <v>1.9149011342100002</v>
       </c>
       <c r="B29" s="1">
-        <v>0.57945394050400001</v>
+        <v>0.89746854262499998</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E29" s="4" t="str">
@@ -1257,41 +1257,41 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>0.92376368462400016</v>
+        <v>0.50885599863599995</v>
       </c>
       <c r="B30" s="1">
-        <v>1.5580437071440001</v>
+        <v>1.1367465216799999</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="E30" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F30" s="2" t="str">
         <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>1.2275841885119998</v>
+        <v>1.0100948956739999</v>
       </c>
       <c r="B31" s="1">
-        <v>0.76623785027999991</v>
+        <v>0.75017223417500001</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E31" s="4" t="str">
@@ -1305,70 +1305,70 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>0.398589563988</v>
+        <v>0.65892967531199997</v>
       </c>
       <c r="B32" s="1">
-        <v>0.54732703662000004</v>
+        <v>1.43648473995</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E32" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-1</v>
+        <v>1-1</v>
       </c>
       <c r="F32" s="2" t="str">
         <f>VLOOKUP(E32,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>1.4055934004639998</v>
+        <v>1.7553957668909999</v>
       </c>
       <c r="B33" s="1">
-        <v>0.7148924567999998</v>
+        <v>0.54416314677600008</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E33" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F33" s="2" t="str">
         <f>VLOOKUP(E33,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>0.51785254634400002</v>
+        <v>1.6797884125230003</v>
       </c>
       <c r="B34" s="1">
-        <v>1.3575644308800001</v>
+        <v>2.1768275873119998</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="E34" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F34" s="2" t="str">
         <f>VLOOKUP(E34,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1377,22 +1377,22 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1.0894176941760001</v>
+        <v>0.45951341740000001</v>
       </c>
       <c r="B35" s="1">
-        <v>0.92304233336000008</v>
+        <v>0</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E35" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-0</v>
       </c>
       <c r="F35" s="2" t="str">
         <f>VLOOKUP(E35,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1400,648 +1400,1948 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="2"/>
+      <c r="A36" s="1">
+        <v>1.5507452804400002</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2.0491196725800003</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-2</v>
+      </c>
+      <c r="F36" s="2" t="str">
+        <f>VLOOKUP(E36,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="2"/>
+      <c r="A37" s="1">
+        <v>2.0676603739200003</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.60716878992000001</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F37" s="2" t="str">
+        <f>VLOOKUP(E37,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="2"/>
+      <c r="A38" s="1">
+        <v>0.68922012464000015</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.68306488866000015</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F38" s="2" t="str">
+        <f>VLOOKUP(E38,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="2"/>
+      <c r="A39" s="1">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.4893386473350001</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-1</v>
+      </c>
+      <c r="F39" s="2" t="str">
+        <f>VLOOKUP(E39,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="2"/>
+      <c r="A40" s="1">
+        <v>0.19147798617600004</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.5886412241700003</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E40" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-2</v>
+      </c>
+      <c r="F40" s="2" t="str">
+        <f>VLOOKUP(E40,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="2"/>
+      <c r="A41" s="1">
+        <v>2.0983843039679999</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1.0322352393080001</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F41" s="2" t="str">
+        <f>VLOOKUP(E41,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="2"/>
+      <c r="A42" s="1">
+        <v>2.6229803799600004</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.77422643118800005</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F42" s="2" t="str">
+        <f>VLOOKUP(E42,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="2"/>
+      <c r="A43" s="1">
+        <v>1.1803911706079999</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.51611761965400005</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E43" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F43" s="2" t="str">
+        <f>VLOOKUP(E43,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="2"/>
+      <c r="A44" s="1">
+        <v>2.0033906126399996</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1.4328897643440004</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F44" s="2" t="str">
+        <f>VLOOKUP(E44,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="2"/>
+      <c r="A45" s="1">
+        <v>1.545489185034</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.20519461473</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-0</v>
+      </c>
+      <c r="F45" s="2" t="str">
+        <f>VLOOKUP(E45,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="2"/>
+      <c r="A46" s="1">
+        <v>0.8695499023440002</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.86480383430700003</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E46" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F46" s="2" t="str">
+        <f>VLOOKUP(E46,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="2"/>
+      <c r="A47" s="1">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-0</v>
+      </c>
+      <c r="F47" s="2" t="str">
+        <f>VLOOKUP(E47,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="2"/>
+      <c r="A48" s="1">
+        <v>1.0788028911840002</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.96031854445999998</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F48" s="2" t="str">
+        <f>VLOOKUP(E48,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="2"/>
+      <c r="A49" s="1">
+        <v>1.8462049478160003</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1.2260430360360002</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F49" s="2" t="str">
+        <f>VLOOKUP(E49,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="2"/>
+      <c r="A50" s="1">
+        <v>2.3989084303180004</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1.2004431814440002</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F50" s="2" t="str">
+        <f>VLOOKUP(E50,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="2"/>
+      <c r="A51" s="1">
+        <v>1.618204336776</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.97807777781999994</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F51" s="2" t="str">
+        <f>VLOOKUP(E51,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="2"/>
+      <c r="A52" s="1">
+        <v>2.2374270338939999</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.74425292750400007</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E52" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F52" s="2" t="str">
+        <f>VLOOKUP(E52,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="2"/>
+      <c r="A53" s="1">
+        <v>1.016957739582</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1.395332574272</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F53" s="2" t="str">
+        <f>VLOOKUP(E53,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="2"/>
+      <c r="A54" s="1">
+        <v>3.2541181080569999</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1.1164127269599999</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E54" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F54" s="2" t="str">
+        <f>VLOOKUP(E54,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="2"/>
+      <c r="A55" s="1">
+        <v>1.6686494624799997</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.95387447372000012</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F55" s="2" t="str">
+        <f>VLOOKUP(E55,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="2"/>
+      <c r="A56" s="1">
+        <v>0.81110421167999991</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.41216043800400004</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E56" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-0</v>
+      </c>
+      <c r="F56" s="2" t="str">
+        <f>VLOOKUP(E56,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="2"/>
+      <c r="A57" s="1">
+        <v>1.2893716042399999</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.582880080272</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F57" s="2" t="str">
+        <f>VLOOKUP(E57,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="2"/>
+      <c r="A58" s="1">
+        <v>1.0132947451199998</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2.9450562464000001</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E58" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-3</v>
+      </c>
+      <c r="F58" s="2" t="str">
+        <f>VLOOKUP(E58,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="2"/>
+      <c r="A59" s="1">
+        <v>0.27304245735999999</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.61050597592400002</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E59" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-1</v>
+      </c>
+      <c r="F59" s="2" t="str">
+        <f>VLOOKUP(E59,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="2"/>
+      <c r="A60" s="1">
+        <v>0.57273731140500006</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1.0979737029000001</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E60" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F60" s="2" t="str">
+        <f>VLOOKUP(E60,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="2"/>
+      <c r="A61" s="1">
+        <v>0.25461658719000002</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1.6470272194200002</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E61" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-2</v>
+      </c>
+      <c r="F61" s="2" t="str">
+        <f>VLOOKUP(E61,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="2"/>
+      <c r="A62" s="1">
+        <v>2.5455991726799998</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1.0979737029000001</v>
+      </c>
+      <c r="C62" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E62" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F62" s="2" t="str">
+        <f>VLOOKUP(E62,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="2"/>
+      <c r="A63" s="1">
+        <v>1.1926095408000001</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.85745674610900002</v>
+      </c>
+      <c r="C63" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F63" s="2" t="str">
+        <f>VLOOKUP(E63,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="2"/>
+      <c r="A64" s="1">
+        <v>1.5450787949999998</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1.254126697904</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D64" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E64" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F64" s="2" t="str">
+        <f>VLOOKUP(E64,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="2"/>
+      <c r="A65" s="1">
+        <v>1.265348767968</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1.55134930701</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D65" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E65" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F65" s="2" t="str">
+        <f>VLOOKUP(E65,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="2"/>
+      <c r="A66" s="1">
+        <v>2.8617555419370002</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1.0529878612499999</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D66" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E66" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F66" s="2" t="str">
+        <f>VLOOKUP(E66,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="2"/>
+      <c r="A67" s="1">
+        <v>1.3414604096519998</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.82661352644499997</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" ref="C67:C116" si="6">ROUND(A67,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D67" s="3">
+        <f t="shared" ref="D67:D116" si="7">ROUND(B67,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E67" s="4" t="str">
+        <f t="shared" ref="E67:E116" si="8">CONCATENATE(C67,"-",D67)</f>
+        <v>1-1</v>
+      </c>
+      <c r="F67" s="2" t="str">
+        <f>VLOOKUP(E67,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="4"/>
+      <c r="A68" s="1">
+        <v>3.4841944898280004</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.73713897047699994</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F68" s="2" t="str">
+        <f>VLOOKUP(E68,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="4"/>
+      <c r="A69" s="1">
+        <v>2.150209170603</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.63490075462399997</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E69" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F69" s="2" t="str">
+        <f>VLOOKUP(E69,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="2"/>
+      <c r="A70" s="1">
+        <v>2.2676331110940002</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1.049497676219</v>
+      </c>
+      <c r="C70" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F70" s="2" t="str">
+        <f>VLOOKUP(E70,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="2"/>
+      <c r="A71" s="1">
+        <v>0.98547364773000012</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1.646887078375</v>
+      </c>
+      <c r="C71" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E71" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F71" s="2" t="str">
+        <f>VLOOKUP(E71,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="2"/>
+      <c r="A72" s="1">
+        <v>2.074601816235</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.38869867554299997</v>
+      </c>
+      <c r="C72" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E72" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F72" s="2" t="str">
+        <f>VLOOKUP(E72,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="2"/>
+      <c r="A73" s="1">
+        <v>2.0905478055540003</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.92144871441800003</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E73" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F73" s="2" t="str">
+        <f>VLOOKUP(E73,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="2"/>
+      <c r="A74" s="1">
+        <v>5.6282810125100005</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" s="3">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="D74" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E74" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>6-0</v>
+      </c>
+      <c r="F74" s="2" t="str">
+        <f>VLOOKUP(E74,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="2"/>
+      <c r="A75" s="1">
+        <v>1.5314558315400004</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.40482364031999996</v>
+      </c>
+      <c r="C75" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E75" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F75" s="2" t="str">
+        <f>VLOOKUP(E75,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="2"/>
+      <c r="A76" s="1">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0</v>
+      </c>
+      <c r="C76" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E76" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-0</v>
+      </c>
+      <c r="F76" s="2" t="str">
+        <f>VLOOKUP(E76,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="2"/>
+      <c r="A77" s="1">
+        <v>1.7232268711500001</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.79432061208500016</v>
+      </c>
+      <c r="C77" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E77" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F77" s="2" t="str">
+        <f>VLOOKUP(E77,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="2"/>
+      <c r="A78" s="1">
+        <v>3.350464746039</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E78" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-0</v>
+      </c>
+      <c r="F78" s="2" t="str">
+        <f>VLOOKUP(E78,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="2"/>
+      <c r="A79" s="1">
+        <v>1.049192151984</v>
+      </c>
+      <c r="B79" s="1">
+        <v>1.720347622422</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E79" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F79" s="2" t="str">
+        <f>VLOOKUP(E79,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="2"/>
+      <c r="A80" s="1">
+        <v>1.9672852845959998</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D80" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E80" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F80" s="2" t="str">
+        <f>VLOOKUP(E80,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="2"/>
+      <c r="A81" s="1">
+        <v>1.1803911706079999</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1.0322352393080001</v>
+      </c>
+      <c r="C81" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E81" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F81" s="2" t="str">
+        <f>VLOOKUP(E81,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="2"/>
+      <c r="A82" s="1">
+        <v>1.7838626729040001</v>
+      </c>
+      <c r="B82" s="1">
+        <v>1.0030417238400002</v>
+      </c>
+      <c r="C82" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D82" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E82" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F82" s="2" t="str">
+        <f>VLOOKUP(E82,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="2"/>
+      <c r="A83" s="1">
+        <v>1.127725581</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0.52109425747799998</v>
+      </c>
+      <c r="C83" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E83" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F83" s="2" t="str">
+        <f>VLOOKUP(E83,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="2"/>
+      <c r="A84" s="1">
+        <v>1.017584649504</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1.0537538209200001</v>
+      </c>
+      <c r="C84" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E84" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F84" s="2" t="str">
+        <f>VLOOKUP(E84,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="2"/>
+      <c r="A85" s="1">
+        <v>1.5652598297700002</v>
+      </c>
+      <c r="B85" s="1">
+        <v>1.4595720992999999</v>
+      </c>
+      <c r="C85" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E85" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F85" s="2" t="str">
+        <f>VLOOKUP(E85,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="2"/>
+      <c r="A86" s="1">
+        <v>2.7391672018620001</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1.2972307501259999</v>
+      </c>
+      <c r="C86" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E86" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F86" s="2" t="str">
+        <f>VLOOKUP(E86,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="2"/>
+      <c r="A87" s="1">
+        <v>0.52166994486300011</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1.94604612993</v>
+      </c>
+      <c r="C87" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D87" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E87" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F87" s="2" t="str">
+        <f>VLOOKUP(E87,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="2"/>
+      <c r="A88" s="1">
+        <v>1.8575813413679998</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1.0669721221999999</v>
+      </c>
+      <c r="C88" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D88" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E88" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F88" s="2" t="str">
+        <f>VLOOKUP(E88,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="2"/>
+      <c r="A89" s="1">
+        <v>1.6500044220000003</v>
+      </c>
+      <c r="B89" s="1">
+        <v>1.0078109422680002</v>
+      </c>
+      <c r="C89" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D89" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E89" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F89" s="2" t="str">
+        <f>VLOOKUP(E89,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="2"/>
+      <c r="A90" s="1">
+        <v>1.1106029764080001</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.8669950754400001</v>
+      </c>
+      <c r="C90" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E90" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F90" s="2" t="str">
+        <f>VLOOKUP(E90,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="2"/>
+      <c r="A91" s="1">
+        <v>1.0740208266819999</v>
+      </c>
+      <c r="B91" s="1">
+        <v>1.1703933521280001</v>
+      </c>
+      <c r="C91" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E91" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F91" s="2" t="str">
+        <f>VLOOKUP(E91,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="2"/>
+      <c r="A92" s="1">
+        <v>1.1538243024519999</v>
+      </c>
+      <c r="B92" s="1">
+        <v>1.1855932657920001</v>
+      </c>
+      <c r="C92" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E92" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F92" s="2" t="str">
+        <f>VLOOKUP(E92,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="2"/>
+      <c r="A93" s="1">
+        <v>1.4160632970879998</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.88919494934400001</v>
+      </c>
+      <c r="C93" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E93" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F93" s="2" t="str">
+        <f>VLOOKUP(E93,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="2"/>
+      <c r="A94" s="1">
+        <v>0.99996328499999998</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.70734598225200007</v>
+      </c>
+      <c r="C94" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E94" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F94" s="2" t="str">
+        <f>VLOOKUP(E94,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="2"/>
+      <c r="A95" s="1">
+        <v>2.1922058750960005</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.64666299360000001</v>
+      </c>
+      <c r="C95" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E95" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F95" s="2" t="str">
+        <f>VLOOKUP(E95,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="2"/>
+      <c r="A96" s="1">
+        <v>1.8034534888439997</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1.21886058969</v>
+      </c>
+      <c r="C96" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E96" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F96" s="2" t="str">
+        <f>VLOOKUP(E96,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="2"/>
+      <c r="A97" s="1">
+        <v>0.67631005809599998</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.58041694768000007</v>
+      </c>
+      <c r="C97" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E97" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F97" s="2" t="str">
+        <f>VLOOKUP(E97,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="2"/>
+      <c r="A98" s="1">
+        <v>1.8034534888439997</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0</v>
+      </c>
+      <c r="C98" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E98" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F98" s="2" t="str">
+        <f>VLOOKUP(E98,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="2"/>
+      <c r="A99" s="1">
+        <v>0.187878072132</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0.58041694768000007</v>
+      </c>
+      <c r="C99" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E99" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-1</v>
+      </c>
+      <c r="F99" s="2" t="str">
+        <f>VLOOKUP(E99,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="2"/>
+      <c r="A100" s="1">
+        <v>1.0341709247999999</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.69372749614399998</v>
+      </c>
+      <c r="C100" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D100" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E100" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F100" s="2" t="str">
+        <f>VLOOKUP(E100,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="2"/>
+      <c r="A101" s="1">
+        <v>0.7637497550550002</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0</v>
+      </c>
+      <c r="C101" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E101" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-0</v>
+      </c>
+      <c r="F101" s="2" t="str">
+        <f>VLOOKUP(E101,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="4"/>
-      <c r="F102" s="2"/>
+      <c r="A102" s="1">
+        <v>1.7676137165759997</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.73477424526000001</v>
+      </c>
+      <c r="C102" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E102" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F102" s="2" t="str">
+        <f>VLOOKUP(E102,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="2"/>
+      <c r="A103" s="1">
+        <v>0.91902683480000003</v>
+      </c>
+      <c r="B103" s="1">
+        <v>2.4285751648200002</v>
+      </c>
+      <c r="C103" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D103" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E103" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F103" s="2" t="str">
+        <f>VLOOKUP(E103,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="2"/>
+      <c r="A104" s="1">
+        <v>1.8378536637600005</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.30361773024000005</v>
+      </c>
+      <c r="C104" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D104" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E104" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F104" s="2" t="str">
+        <f>VLOOKUP(E104,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="2"/>
+      <c r="A105" s="1">
+        <v>3.4462037391270002</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0</v>
+      </c>
+      <c r="C105" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D105" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E105" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-0</v>
+      </c>
+      <c r="F105" s="2" t="str">
+        <f>VLOOKUP(E105,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="2"/>
+      <c r="A106" s="1">
+        <v>1.2922264035150002</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.39712697324300006</v>
+      </c>
+      <c r="C106" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D106" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E106" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-0</v>
+      </c>
+      <c r="F106" s="2" t="str">
+        <f>VLOOKUP(E106,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="2"/>
+      <c r="A107" s="1">
+        <v>1.5738548941439996</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0</v>
+      </c>
+      <c r="C107" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D107" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E107" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F107" s="2" t="str">
+        <f>VLOOKUP(E107,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="2"/>
+      <c r="A108" s="1">
+        <v>1.3114901899800002</v>
+      </c>
+      <c r="B108" s="1">
+        <v>4.644858582975</v>
+      </c>
+      <c r="C108" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D108" s="3">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E108" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-5</v>
+      </c>
+      <c r="F108" s="2" t="str">
+        <f>VLOOKUP(E108,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="2"/>
+      <c r="A109" s="1">
+        <v>1.3114901899800002</v>
+      </c>
+      <c r="B109" s="1">
+        <v>4.644858582975</v>
+      </c>
+      <c r="C109" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D109" s="3">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E109" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-5</v>
+      </c>
+      <c r="F109" s="2" t="str">
+        <f>VLOOKUP(E109,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="2"/>
+      <c r="A110" s="1">
+        <v>1.7637548740290001</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1.042088516058</v>
+      </c>
+      <c r="C110" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D110" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E110" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F110" s="2" t="str">
+        <f>VLOOKUP(E110,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="2"/>
+      <c r="A111" s="1">
+        <v>0.37851163737599997</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0.86131091554200012</v>
+      </c>
+      <c r="C111" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D111" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E111" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-1</v>
+      </c>
+      <c r="F111" s="2" t="str">
+        <f>VLOOKUP(E111,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="2"/>
+      <c r="A112" s="1">
+        <v>0.77265709292700002</v>
+      </c>
+      <c r="B112" s="1">
+        <v>1.6120166100480002</v>
+      </c>
+      <c r="C112" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D112" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E112" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F112" s="2" t="str">
+        <f>VLOOKUP(E112,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="2"/>
+      <c r="A113" s="1">
+        <v>2.0676772085519999</v>
+      </c>
+      <c r="B113" s="1">
+        <v>1.763598316038</v>
+      </c>
+      <c r="C113" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D113" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E113" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F113" s="2" t="str">
+        <f>VLOOKUP(E113,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="2"/>
+      <c r="A114" s="1">
+        <v>0.75137228836799996</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0.17413008445000003</v>
+      </c>
+      <c r="C114" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D114" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E114" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-0</v>
+      </c>
+      <c r="F114" s="2" t="str">
+        <f>VLOOKUP(E114,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="4"/>
+      <c r="A115" s="1">
+        <v>0.20472184248</v>
+      </c>
+      <c r="B115" s="1">
+        <v>0.9920422096</v>
+      </c>
+      <c r="C115" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D115" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E115" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-1</v>
+      </c>
+      <c r="F115" s="2" t="str">
+        <f>VLOOKUP(E115,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="4"/>
+      <c r="A116" s="1">
+        <v>1.6607564626590001</v>
+      </c>
+      <c r="B116" s="1">
+        <v>1.0392166704000001</v>
+      </c>
+      <c r="C116" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D116" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E116" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F116" s="2" t="str">
+        <f>VLOOKUP(E116,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>

</xml_diff>

<commit_message>
14/09/2021 fixtures and odds
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard.000\gitboyzorro5\FDAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitboyzorro5\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -553,317 +553,317 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K106" sqref="K106"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1.35759955878</v>
+        <v>1.8033834887639999</v>
       </c>
       <c r="B1" s="1">
-        <v>1.0979737029000001</v>
+        <v>0</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3">
         <f>ROUND(B1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>VLOOKUP(E1,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.0182663357300001</v>
+        <v>0.96177252692399984</v>
       </c>
       <c r="B2" s="1">
-        <v>0.18299561715000004</v>
+        <v>1.1143045388100001</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C4" si="0">ROUND(A2,0)</f>
+        <f t="shared" ref="C2:C23" si="0">ROUND(A2,0)</f>
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D4" si="1">ROUND(B2,0)</f>
-        <v>0</v>
+        <f t="shared" ref="D2:D23" si="1">ROUND(B2,0)</f>
+        <v>1</v>
       </c>
       <c r="E2" s="4" t="str">
-        <f t="shared" ref="E2:E4" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>1-0</v>
+        <f t="shared" ref="E2:E23" si="2">CONCATENATE(C2,"-",D2)</f>
+        <v>1-1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(E2,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.368983621678</v>
+        <v>2.4046713204359995</v>
       </c>
       <c r="B3" s="1">
-        <v>1.171961887136</v>
+        <v>2.7857613470250002</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
-        <v>1-1</v>
+        <f t="shared" si="2"/>
+        <v>2-3</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.116715328388</v>
+        <v>0.305604336611</v>
       </c>
       <c r="B4" s="1">
-        <v>0.66578103801599997</v>
+        <v>1.10503121625</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E4" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
+        <f t="shared" si="2"/>
+        <v>0-1</v>
       </c>
       <c r="F4" s="2" t="str">
         <f>VLOOKUP(E4,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1.5861402179199999</v>
+        <v>0.29711929519999997</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0999469951359999</v>
+        <v>1.4734416235500001</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E5" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
+        <f t="shared" si="2"/>
+        <v>0-1</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2.0355953287640003</v>
+        <v>1.4605526026599998</v>
       </c>
       <c r="B6" s="1">
-        <v>0.64014843471999994</v>
+        <v>0.8511416684319999</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
+        <f t="shared" si="2"/>
+        <v>1-1</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1.2110463756000001</v>
+        <v>0.225441685404</v>
       </c>
       <c r="B7" s="1">
-        <v>0.48230499668999999</v>
+        <v>0.17415508518</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
+        <f t="shared" si="2"/>
+        <v>0-0</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.28718364396000007</v>
+        <v>1.6832219236799999</v>
       </c>
       <c r="B8" s="1">
-        <v>0.29790773050500002</v>
+        <v>1.48573938508</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-0</v>
+        <f t="shared" si="2"/>
+        <v>2-1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0</v>
+        <v>1.502899575012</v>
       </c>
       <c r="B9" s="1">
-        <v>0.49650454992600002</v>
+        <v>0.69647033634</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-0</v>
+        <f t="shared" si="2"/>
+        <v>2-1</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>VLOOKUP(E9,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2.440538582301</v>
+        <v>0.78904090175999997</v>
       </c>
       <c r="B10" s="1">
-        <v>0.37215979945600003</v>
+        <v>2.0892910106850002</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D10" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="E10" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-0</v>
+        <f t="shared" si="2"/>
+        <v>1-2</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0.13560769936799999</v>
+        <v>1.8633404491440002</v>
       </c>
       <c r="B11" s="1">
-        <v>0.93033282723199995</v>
+        <v>1.293392653488</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-1</v>
+        <f t="shared" si="2"/>
+        <v>2-1</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>VLOOKUP(E11,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2.0337488194229998</v>
+        <v>3.1250477700000001</v>
       </c>
       <c r="B12" s="1">
-        <v>3.3490381786000003</v>
+        <v>0.75447904786800024</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-3</v>
+        <f t="shared" si="2"/>
+        <v>3-1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.65705341415999996</v>
+        <v>0.76143870941800007</v>
       </c>
       <c r="B13" s="1">
-        <v>0.86802068320000003</v>
+        <v>0.96817227852799992</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1-1</v>
       </c>
       <c r="F13" s="2" t="str">
@@ -873,117 +873,117 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>0.51190794143999996</v>
+        <v>1.5028445730479996</v>
       </c>
       <c r="B14" s="1">
-        <v>0.93267412731199995</v>
+        <v>2.8438680402450003</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
+        <f t="shared" si="2"/>
+        <v>2-3</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>VLOOKUP(E14,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2.1236991131199998</v>
+        <v>1.4278038265040001</v>
       </c>
       <c r="B15" s="1">
-        <v>1.271754113456</v>
+        <v>1.0003693178700002</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
+        <f t="shared" si="2"/>
+        <v>1-1</v>
       </c>
       <c r="F15" s="2" t="str">
         <f>VLOOKUP(E15,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>0.71308630847999999</v>
+        <v>2.2846061227280008</v>
       </c>
       <c r="B16" s="1">
-        <v>0.8287412704999999</v>
+        <v>0.47426397283200006</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
+        <f t="shared" si="2"/>
+        <v>2-0</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>VLOOKUP(E16,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1.4559720447999998</v>
+        <v>1.2956451363600001</v>
       </c>
       <c r="B17" s="1">
-        <v>1.5041424908249998</v>
+        <v>0.55574684334000002</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
+        <f t="shared" si="2"/>
+        <v>1-1</v>
       </c>
       <c r="F17" s="2" t="str">
         <f>VLOOKUP(E17,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.7680160534400002</v>
+        <v>1.8633404491440002</v>
       </c>
       <c r="B18" s="1">
-        <v>1.0505185652</v>
+        <v>1.1639497539999999</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E18" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2-1</v>
       </c>
       <c r="F18" s="2" t="str">
@@ -993,21 +993,21 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.0696794617599998</v>
+        <v>1.243707335648</v>
       </c>
       <c r="B19" s="1">
-        <v>1.074330348975</v>
+        <v>1.2004431814440002</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E19" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1-1</v>
       </c>
       <c r="F19" s="2" t="str">
@@ -1017,22 +1017,22 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.46216890262899996</v>
+        <v>1.0788028911840002</v>
       </c>
       <c r="B20" s="1">
-        <v>0.76402158299999989</v>
+        <v>1.576341046332</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-1</v>
+        <f t="shared" si="2"/>
+        <v>1-2</v>
       </c>
       <c r="F20" s="2" t="str">
         <f>VLOOKUP(E20,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1041,22 +1041,22 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>0.79233716664199993</v>
+        <v>1.8508966244300002</v>
       </c>
       <c r="B21" s="1">
-        <v>0.40928933987499999</v>
+        <v>0.95094459860400016</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="E21" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
+        <f t="shared" si="2"/>
+        <v>2-1</v>
       </c>
       <c r="F21" s="2" t="str">
         <f>VLOOKUP(E21,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1065,21 +1065,21 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>0.576712865706</v>
+        <v>1.27497978</v>
       </c>
       <c r="B22" s="1">
-        <v>1.7605344776320002</v>
+        <v>1.6976576312039997</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1-2</v>
       </c>
       <c r="F22" s="2" t="str">
@@ -1089,21 +1089,21 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1.4765451456000001</v>
+        <v>1.4110829215919998</v>
       </c>
       <c r="B23" s="1">
-        <v>0.97046481486000025</v>
+        <v>1.1866452595949999</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1-1</v>
       </c>
       <c r="F23" s="2" t="str">
@@ -1112,2236 +1112,746 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>2.1118918950000003</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0.83598609731999995</v>
-      </c>
-      <c r="C24" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E24" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F24" s="2" t="str">
-        <f>VLOOKUP(E24,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.8348066784</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.238049235344</v>
-      </c>
-      <c r="C25" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F25" s="2" t="str">
-        <f>VLOOKUP(E25,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>0.93705474869999994</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1.6124270327450001</v>
-      </c>
-      <c r="C26" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E26" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F26" s="2" t="str">
-        <f>VLOOKUP(E26,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>1.7633965244999998</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0.79622631909699992</v>
-      </c>
-      <c r="C27" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E27" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F27" s="2" t="str">
-        <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>0.96904108560000002</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1.75207740989</v>
-      </c>
-      <c r="C28" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D28" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E28" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F28" s="2" t="str">
-        <f>VLOOKUP(E28,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>1.9149011342100002</v>
-      </c>
-      <c r="B29" s="1">
-        <v>0.89746854262499998</v>
-      </c>
-      <c r="C29" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E29" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F29" s="2" t="str">
-        <f>VLOOKUP(E29,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>0.50885599863599995</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1.1367465216799999</v>
-      </c>
-      <c r="C30" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E30" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F30" s="2" t="str">
-        <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>1.0100948956739999</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.75017223417500001</v>
-      </c>
-      <c r="C31" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E31" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F31" s="2" t="str">
-        <f>VLOOKUP(E31,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>0.65892967531199997</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1.43648473995</v>
-      </c>
-      <c r="C32" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F32" s="2" t="str">
-        <f>VLOOKUP(E32,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>1.7553957668909999</v>
-      </c>
-      <c r="B33" s="1">
-        <v>0.54416314677600008</v>
-      </c>
-      <c r="C33" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E33" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F33" s="2" t="str">
-        <f>VLOOKUP(E33,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>1.6797884125230003</v>
-      </c>
-      <c r="B34" s="1">
-        <v>2.1768275873119998</v>
-      </c>
-      <c r="C34" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E34" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-2</v>
-      </c>
-      <c r="F34" s="2" t="str">
-        <f>VLOOKUP(E34,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>0.45951341740000001</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-0</v>
-      </c>
-      <c r="F35" s="2" t="str">
-        <f>VLOOKUP(E35,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>1.5507452804400002</v>
-      </c>
-      <c r="B36" s="1">
-        <v>2.0491196725800003</v>
-      </c>
-      <c r="C36" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E36" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-2</v>
-      </c>
-      <c r="F36" s="2" t="str">
-        <f>VLOOKUP(E36,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>2.0676603739200003</v>
-      </c>
-      <c r="B37" s="1">
-        <v>0.60716878992000001</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E37" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F37" s="2" t="str">
-        <f>VLOOKUP(E37,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>0.68922012464000015</v>
-      </c>
-      <c r="B38" s="1">
-        <v>0.68306488866000015</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E38" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F38" s="2" t="str">
-        <f>VLOOKUP(E38,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1.4893386473350001</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E39" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-1</v>
-      </c>
-      <c r="F39" s="2" t="str">
-        <f>VLOOKUP(E39,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>0.19147798617600004</v>
-      </c>
-      <c r="B40" s="1">
-        <v>1.5886412241700003</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E40" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-2</v>
-      </c>
-      <c r="F40" s="2" t="str">
-        <f>VLOOKUP(E40,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>2.0983843039679999</v>
-      </c>
-      <c r="B41" s="1">
-        <v>1.0322352393080001</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E41" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F41" s="2" t="str">
-        <f>VLOOKUP(E41,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>2.6229803799600004</v>
-      </c>
-      <c r="B42" s="1">
-        <v>0.77422643118800005</v>
-      </c>
-      <c r="C42" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E42" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-1</v>
-      </c>
-      <c r="F42" s="2" t="str">
-        <f>VLOOKUP(E42,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>1.1803911706079999</v>
-      </c>
-      <c r="B43" s="1">
-        <v>0.51611761965400005</v>
-      </c>
-      <c r="C43" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E43" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F43" s="2" t="str">
-        <f>VLOOKUP(E43,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>2.0033906126399996</v>
-      </c>
-      <c r="B44" s="1">
-        <v>1.4328897643440004</v>
-      </c>
-      <c r="C44" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E44" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F44" s="2" t="str">
-        <f>VLOOKUP(E44,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>1.545489185034</v>
-      </c>
-      <c r="B45" s="1">
-        <v>0.20519461473</v>
-      </c>
-      <c r="C45" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D45" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-0</v>
-      </c>
-      <c r="F45" s="2" t="str">
-        <f>VLOOKUP(E45,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>0.8695499023440002</v>
-      </c>
-      <c r="B46" s="1">
-        <v>0.86480383430700003</v>
-      </c>
-      <c r="C46" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D46" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E46" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F46" s="2" t="str">
-        <f>VLOOKUP(E46,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>0</v>
-      </c>
-      <c r="B47" s="1">
-        <v>0</v>
-      </c>
-      <c r="C47" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D47" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E47" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-0</v>
-      </c>
-      <c r="F47" s="2" t="str">
-        <f>VLOOKUP(E47,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>1.0788028911840002</v>
-      </c>
-      <c r="B48" s="1">
-        <v>0.96031854445999998</v>
-      </c>
-      <c r="C48" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D48" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E48" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F48" s="2" t="str">
-        <f>VLOOKUP(E48,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>1.8462049478160003</v>
-      </c>
-      <c r="B49" s="1">
-        <v>1.2260430360360002</v>
-      </c>
-      <c r="C49" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D49" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E49" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F49" s="2" t="str">
-        <f>VLOOKUP(E49,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>2.3989084303180004</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1.2004431814440002</v>
-      </c>
-      <c r="C50" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D50" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E50" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F50" s="2" t="str">
-        <f>VLOOKUP(E50,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>1.618204336776</v>
-      </c>
-      <c r="B51" s="1">
-        <v>0.97807777781999994</v>
-      </c>
-      <c r="C51" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D51" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E51" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F51" s="2" t="str">
-        <f>VLOOKUP(E51,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>2.2374270338939999</v>
-      </c>
-      <c r="B52" s="1">
-        <v>0.74425292750400007</v>
-      </c>
-      <c r="C52" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D52" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E52" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F52" s="2" t="str">
-        <f>VLOOKUP(E52,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>1.016957739582</v>
-      </c>
-      <c r="B53" s="1">
-        <v>1.395332574272</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E53" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F53" s="2" t="str">
-        <f>VLOOKUP(E53,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>3.2541181080569999</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1.1164127269599999</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E54" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-1</v>
-      </c>
-      <c r="F54" s="2" t="str">
-        <f>VLOOKUP(E54,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>1.6686494624799997</v>
-      </c>
-      <c r="B55" s="1">
-        <v>0.95387447372000012</v>
-      </c>
-      <c r="C55" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E55" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F55" s="2" t="str">
-        <f>VLOOKUP(E55,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>0.81110421167999991</v>
-      </c>
-      <c r="B56" s="1">
-        <v>0.41216043800400004</v>
-      </c>
-      <c r="C56" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E56" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F56" s="2" t="str">
-        <f>VLOOKUP(E56,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>1.2893716042399999</v>
-      </c>
-      <c r="B57" s="1">
-        <v>0.582880080272</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E57" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F57" s="2" t="str">
-        <f>VLOOKUP(E57,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>1.0132947451199998</v>
-      </c>
-      <c r="B58" s="1">
-        <v>2.9450562464000001</v>
-      </c>
-      <c r="C58" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D58" s="3">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E58" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-3</v>
-      </c>
-      <c r="F58" s="2" t="str">
-        <f>VLOOKUP(E58,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>0.27304245735999999</v>
-      </c>
-      <c r="B59" s="1">
-        <v>0.61050597592400002</v>
-      </c>
-      <c r="C59" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D59" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E59" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-1</v>
-      </c>
-      <c r="F59" s="2" t="str">
-        <f>VLOOKUP(E59,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>0.57273731140500006</v>
-      </c>
-      <c r="B60" s="1">
-        <v>1.0979737029000001</v>
-      </c>
-      <c r="C60" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D60" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E60" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F60" s="2" t="str">
-        <f>VLOOKUP(E60,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>0.25461658719000002</v>
-      </c>
-      <c r="B61" s="1">
-        <v>1.6470272194200002</v>
-      </c>
-      <c r="C61" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D61" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E61" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-2</v>
-      </c>
-      <c r="F61" s="2" t="str">
-        <f>VLOOKUP(E61,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>2.5455991726799998</v>
-      </c>
-      <c r="B62" s="1">
-        <v>1.0979737029000001</v>
-      </c>
-      <c r="C62" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D62" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E62" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-1</v>
-      </c>
-      <c r="F62" s="2" t="str">
-        <f>VLOOKUP(E62,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>1.1926095408000001</v>
-      </c>
-      <c r="B63" s="1">
-        <v>0.85745674610900002</v>
-      </c>
-      <c r="C63" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D63" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E63" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F63" s="2" t="str">
-        <f>VLOOKUP(E63,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>1.5450787949999998</v>
-      </c>
-      <c r="B64" s="1">
-        <v>1.254126697904</v>
-      </c>
-      <c r="C64" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D64" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E64" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F64" s="2" t="str">
-        <f>VLOOKUP(E64,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>1.265348767968</v>
-      </c>
-      <c r="B65" s="1">
-        <v>1.55134930701</v>
-      </c>
-      <c r="C65" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D65" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E65" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F65" s="2" t="str">
-        <f>VLOOKUP(E65,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>2.8617555419370002</v>
-      </c>
-      <c r="B66" s="1">
-        <v>1.0529878612499999</v>
-      </c>
-      <c r="C66" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D66" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E66" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-1</v>
-      </c>
-      <c r="F66" s="2" t="str">
-        <f>VLOOKUP(E66,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>1.3414604096519998</v>
-      </c>
-      <c r="B67" s="1">
-        <v>0.82661352644499997</v>
-      </c>
-      <c r="C67" s="3">
-        <f t="shared" ref="C67:C116" si="6">ROUND(A67,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D67" s="3">
-        <f t="shared" ref="D67:D116" si="7">ROUND(B67,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E67" s="4" t="str">
-        <f t="shared" ref="E67:E116" si="8">CONCATENATE(C67,"-",D67)</f>
-        <v>1-1</v>
-      </c>
-      <c r="F67" s="2" t="str">
-        <f>VLOOKUP(E67,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>3.4841944898280004</v>
-      </c>
-      <c r="B68" s="1">
-        <v>0.73713897047699994</v>
-      </c>
-      <c r="C68" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D68" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E68" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F68" s="2" t="str">
-        <f>VLOOKUP(E68,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="4"/>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>2.150209170603</v>
-      </c>
-      <c r="B69" s="1">
-        <v>0.63490075462399997</v>
-      </c>
-      <c r="C69" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D69" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E69" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F69" s="2" t="str">
-        <f>VLOOKUP(E69,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="4"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>2.2676331110940002</v>
-      </c>
-      <c r="B70" s="1">
-        <v>1.049497676219</v>
-      </c>
-      <c r="C70" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D70" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E70" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F70" s="2" t="str">
-        <f>VLOOKUP(E70,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>0.98547364773000012</v>
-      </c>
-      <c r="B71" s="1">
-        <v>1.646887078375</v>
-      </c>
-      <c r="C71" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D71" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E71" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F71" s="2" t="str">
-        <f>VLOOKUP(E71,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>2.074601816235</v>
-      </c>
-      <c r="B72" s="1">
-        <v>0.38869867554299997</v>
-      </c>
-      <c r="C72" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D72" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E72" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F72" s="2" t="str">
-        <f>VLOOKUP(E72,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>2.0905478055540003</v>
-      </c>
-      <c r="B73" s="1">
-        <v>0.92144871441800003</v>
-      </c>
-      <c r="C73" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D73" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E73" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F73" s="2" t="str">
-        <f>VLOOKUP(E73,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>5.6282810125100005</v>
-      </c>
-      <c r="B74" s="1">
-        <v>0</v>
-      </c>
-      <c r="C74" s="3">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="D74" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E74" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>6-0</v>
-      </c>
-      <c r="F74" s="2" t="str">
-        <f>VLOOKUP(E74,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>1.5314558315400004</v>
-      </c>
-      <c r="B75" s="1">
-        <v>0.40482364031999996</v>
-      </c>
-      <c r="C75" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D75" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E75" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F75" s="2" t="str">
-        <f>VLOOKUP(E75,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>0</v>
-      </c>
-      <c r="B76" s="1">
-        <v>0</v>
-      </c>
-      <c r="C76" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D76" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E76" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-0</v>
-      </c>
-      <c r="F76" s="2" t="str">
-        <f>VLOOKUP(E76,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>1.7232268711500001</v>
-      </c>
-      <c r="B77" s="1">
-        <v>0.79432061208500016</v>
-      </c>
-      <c r="C77" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D77" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E77" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F77" s="2" t="str">
-        <f>VLOOKUP(E77,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>3.350464746039</v>
-      </c>
-      <c r="B78" s="1">
-        <v>0</v>
-      </c>
-      <c r="C78" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D78" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E78" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-0</v>
-      </c>
-      <c r="F78" s="2" t="str">
-        <f>VLOOKUP(E78,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>1.049192151984</v>
-      </c>
-      <c r="B79" s="1">
-        <v>1.720347622422</v>
-      </c>
-      <c r="C79" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D79" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E79" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F79" s="2" t="str">
-        <f>VLOOKUP(E79,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>1.9672852845959998</v>
-      </c>
-      <c r="B80" s="1">
-        <v>0</v>
-      </c>
-      <c r="C80" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D80" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E80" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F80" s="2" t="str">
-        <f>VLOOKUP(E80,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>1.1803911706079999</v>
-      </c>
-      <c r="B81" s="1">
-        <v>1.0322352393080001</v>
-      </c>
-      <c r="C81" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D81" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E81" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F81" s="2" t="str">
-        <f>VLOOKUP(E81,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>1.7838626729040001</v>
-      </c>
-      <c r="B82" s="1">
-        <v>1.0030417238400002</v>
-      </c>
-      <c r="C82" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D82" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E82" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F82" s="2" t="str">
-        <f>VLOOKUP(E82,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>1.127725581</v>
-      </c>
-      <c r="B83" s="1">
-        <v>0.52109425747799998</v>
-      </c>
-      <c r="C83" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D83" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E83" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F83" s="2" t="str">
-        <f>VLOOKUP(E83,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>1.017584649504</v>
-      </c>
-      <c r="B84" s="1">
-        <v>1.0537538209200001</v>
-      </c>
-      <c r="C84" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D84" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E84" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F84" s="2" t="str">
-        <f>VLOOKUP(E84,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>1.5652598297700002</v>
-      </c>
-      <c r="B85" s="1">
-        <v>1.4595720992999999</v>
-      </c>
-      <c r="C85" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D85" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E85" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F85" s="2" t="str">
-        <f>VLOOKUP(E85,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>2.7391672018620001</v>
-      </c>
-      <c r="B86" s="1">
-        <v>1.2972307501259999</v>
-      </c>
-      <c r="C86" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D86" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E86" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F86" s="2" t="str">
-        <f>VLOOKUP(E86,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>0.52166994486300011</v>
-      </c>
-      <c r="B87" s="1">
-        <v>1.94604612993</v>
-      </c>
-      <c r="C87" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D87" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E87" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F87" s="2" t="str">
-        <f>VLOOKUP(E87,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>1.8575813413679998</v>
-      </c>
-      <c r="B88" s="1">
-        <v>1.0669721221999999</v>
-      </c>
-      <c r="C88" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D88" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E88" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F88" s="2" t="str">
-        <f>VLOOKUP(E88,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>1.6500044220000003</v>
-      </c>
-      <c r="B89" s="1">
-        <v>1.0078109422680002</v>
-      </c>
-      <c r="C89" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D89" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E89" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F89" s="2" t="str">
-        <f>VLOOKUP(E89,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>1.1106029764080001</v>
-      </c>
-      <c r="B90" s="1">
-        <v>0.8669950754400001</v>
-      </c>
-      <c r="C90" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D90" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E90" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F90" s="2" t="str">
-        <f>VLOOKUP(E90,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>1.0740208266819999</v>
-      </c>
-      <c r="B91" s="1">
-        <v>1.1703933521280001</v>
-      </c>
-      <c r="C91" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D91" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E91" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F91" s="2" t="str">
-        <f>VLOOKUP(E91,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>1.1538243024519999</v>
-      </c>
-      <c r="B92" s="1">
-        <v>1.1855932657920001</v>
-      </c>
-      <c r="C92" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D92" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E92" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F92" s="2" t="str">
-        <f>VLOOKUP(E92,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>1.4160632970879998</v>
-      </c>
-      <c r="B93" s="1">
-        <v>0.88919494934400001</v>
-      </c>
-      <c r="C93" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D93" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E93" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F93" s="2" t="str">
-        <f>VLOOKUP(E93,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>0.99996328499999998</v>
-      </c>
-      <c r="B94" s="1">
-        <v>0.70734598225200007</v>
-      </c>
-      <c r="C94" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D94" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E94" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F94" s="2" t="str">
-        <f>VLOOKUP(E94,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <v>2.1922058750960005</v>
-      </c>
-      <c r="B95" s="1">
-        <v>0.64666299360000001</v>
-      </c>
-      <c r="C95" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D95" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E95" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F95" s="2" t="str">
-        <f>VLOOKUP(E95,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>1.8034534888439997</v>
-      </c>
-      <c r="B96" s="1">
-        <v>1.21886058969</v>
-      </c>
-      <c r="C96" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D96" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E96" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F96" s="2" t="str">
-        <f>VLOOKUP(E96,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>0.67631005809599998</v>
-      </c>
-      <c r="B97" s="1">
-        <v>0.58041694768000007</v>
-      </c>
-      <c r="C97" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D97" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E97" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F97" s="2" t="str">
-        <f>VLOOKUP(E97,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>1.8034534888439997</v>
-      </c>
-      <c r="B98" s="1">
-        <v>0</v>
-      </c>
-      <c r="C98" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D98" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E98" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F98" s="2" t="str">
-        <f>VLOOKUP(E98,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>0.187878072132</v>
-      </c>
-      <c r="B99" s="1">
-        <v>0.58041694768000007</v>
-      </c>
-      <c r="C99" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D99" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E99" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-1</v>
-      </c>
-      <c r="F99" s="2" t="str">
-        <f>VLOOKUP(E99,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>1.0341709247999999</v>
-      </c>
-      <c r="B100" s="1">
-        <v>0.69372749614399998</v>
-      </c>
-      <c r="C100" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D100" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E100" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F100" s="2" t="str">
-        <f>VLOOKUP(E100,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>0.7637497550550002</v>
-      </c>
-      <c r="B101" s="1">
-        <v>0</v>
-      </c>
-      <c r="C101" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D101" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E101" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F101" s="2" t="str">
-        <f>VLOOKUP(E101,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>1.7676137165759997</v>
-      </c>
-      <c r="B102" s="1">
-        <v>0.73477424526000001</v>
-      </c>
-      <c r="C102" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D102" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E102" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F102" s="2" t="str">
-        <f>VLOOKUP(E102,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>0.91902683480000003</v>
-      </c>
-      <c r="B103" s="1">
-        <v>2.4285751648200002</v>
-      </c>
-      <c r="C103" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D103" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E103" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F103" s="2" t="str">
-        <f>VLOOKUP(E103,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>1.8378536637600005</v>
-      </c>
-      <c r="B104" s="1">
-        <v>0.30361773024000005</v>
-      </c>
-      <c r="C104" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D104" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E104" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F104" s="2" t="str">
-        <f>VLOOKUP(E104,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>3.4462037391270002</v>
-      </c>
-      <c r="B105" s="1">
-        <v>0</v>
-      </c>
-      <c r="C105" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D105" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E105" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-0</v>
-      </c>
-      <c r="F105" s="2" t="str">
-        <f>VLOOKUP(E105,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>1.2922264035150002</v>
-      </c>
-      <c r="B106" s="1">
-        <v>0.39712697324300006</v>
-      </c>
-      <c r="C106" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D106" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E106" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F106" s="2" t="str">
-        <f>VLOOKUP(E106,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>1.5738548941439996</v>
-      </c>
-      <c r="B107" s="1">
-        <v>0</v>
-      </c>
-      <c r="C107" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D107" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E107" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F107" s="2" t="str">
-        <f>VLOOKUP(E107,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="2"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <v>1.3114901899800002</v>
-      </c>
-      <c r="B108" s="1">
-        <v>4.644858582975</v>
-      </c>
-      <c r="C108" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D108" s="3">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="E108" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-5</v>
-      </c>
-      <c r="F108" s="2" t="str">
-        <f>VLOOKUP(E108,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="2"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <v>1.3114901899800002</v>
-      </c>
-      <c r="B109" s="1">
-        <v>4.644858582975</v>
-      </c>
-      <c r="C109" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D109" s="3">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="E109" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-5</v>
-      </c>
-      <c r="F109" s="2" t="str">
-        <f>VLOOKUP(E109,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>1.7637548740290001</v>
-      </c>
-      <c r="B110" s="1">
-        <v>1.042088516058</v>
-      </c>
-      <c r="C110" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D110" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E110" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F110" s="2" t="str">
-        <f>VLOOKUP(E110,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>0.37851163737599997</v>
-      </c>
-      <c r="B111" s="1">
-        <v>0.86131091554200012</v>
-      </c>
-      <c r="C111" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D111" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E111" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-1</v>
-      </c>
-      <c r="F111" s="2" t="str">
-        <f>VLOOKUP(E111,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>0.77265709292700002</v>
-      </c>
-      <c r="B112" s="1">
-        <v>1.6120166100480002</v>
-      </c>
-      <c r="C112" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D112" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E112" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F112" s="2" t="str">
-        <f>VLOOKUP(E112,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>2.0676772085519999</v>
-      </c>
-      <c r="B113" s="1">
-        <v>1.763598316038</v>
-      </c>
-      <c r="C113" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D113" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E113" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-2</v>
-      </c>
-      <c r="F113" s="2" t="str">
-        <f>VLOOKUP(E113,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <v>0.75137228836799996</v>
-      </c>
-      <c r="B114" s="1">
-        <v>0.17413008445000003</v>
-      </c>
-      <c r="C114" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D114" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E114" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F114" s="2" t="str">
-        <f>VLOOKUP(E114,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="2"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <v>0.20472184248</v>
-      </c>
-      <c r="B115" s="1">
-        <v>0.9920422096</v>
-      </c>
-      <c r="C115" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D115" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E115" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-1</v>
-      </c>
-      <c r="F115" s="2" t="str">
-        <f>VLOOKUP(E115,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>1.6607564626590001</v>
-      </c>
-      <c r="B116" s="1">
-        <v>1.0392166704000001</v>
-      </c>
-      <c r="C116" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D116" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E116" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F116" s="2" t="str">
-        <f>VLOOKUP(E116,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>

</xml_diff>

<commit_message>
updated fixtures on 09/10/2021
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -553,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F122"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1.7198329140720001</v>
+        <v>1.5635056786320001</v>
       </c>
       <c r="B1" s="1">
-        <v>1.0215139019119999</v>
+        <v>1.67145456863</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
@@ -572,58 +572,58 @@
       </c>
       <c r="D1" s="3">
         <f>ROUND(B1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>2-1</v>
+        <v>2-2</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>VLOOKUP(E1,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2.169663341613</v>
+        <v>0.80416958740000011</v>
       </c>
       <c r="B2" s="1">
-        <v>0.63284540972799996</v>
+        <v>0.742826475496</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C65" si="0">ROUND(A2,0)</f>
-        <v>2</v>
+        <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D65" si="1">ROUND(B2,0)</f>
+        <f t="shared" ref="D2" si="1">ROUND(B2,0)</f>
         <v>1</v>
       </c>
       <c r="E2" s="4" t="str">
-        <f t="shared" ref="E2:E65" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>2-1</v>
+        <f t="shared" ref="E2" si="2">CONCATENATE(C2,"-",D2)</f>
+        <v>1-1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(E2,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.5758327516719999</v>
+        <v>1.715536897872</v>
       </c>
       <c r="B3" s="1">
-        <v>1.3359184354199998</v>
+        <v>0.59427717924399992</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
+        <f t="shared" ref="C3:C29" si="3">ROUND(A3,0)</f>
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
+        <f t="shared" ref="D3:D29" si="4">ROUND(B3,0)</f>
         <v>1</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
+        <f t="shared" ref="E3:E29" si="5">CONCATENATE(C3,"-",D3)</f>
         <v>2-1</v>
       </c>
       <c r="F3" s="2" t="str">
@@ -633,10 +633,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.05552877293</v>
+        <v>0.61580268427999996</v>
       </c>
       <c r="B4" s="1">
-        <v>1.2422779499999999</v>
+        <v>2.0142277959600001</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="3"/>
@@ -644,23 +644,23 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F4" s="2" t="str">
         <f>VLOOKUP(E4,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1.4428476135359998</v>
+        <v>1.179371616696</v>
       </c>
       <c r="B5" s="1">
-        <v>0.83611844339999997</v>
+        <v>0.40864222673399997</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="3"/>
@@ -668,35 +668,35 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.69338786592000001</v>
+        <v>0.48249975024400005</v>
       </c>
       <c r="B6" s="1">
-        <v>1.4707209445</v>
+        <v>0.14856596096999999</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-0</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -705,14 +705,14 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2.640813045552</v>
+        <v>1.3401715341520002</v>
       </c>
       <c r="B7" s="1">
-        <v>0.76575939728400011</v>
+        <v>1.0834066645639999</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="4"/>
@@ -720,55 +720,55 @@
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-1</v>
+        <v>1-1</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2.8882642679549999</v>
+        <v>0.22333414448000005</v>
       </c>
       <c r="B8" s="1">
-        <v>2.7568038319520003</v>
+        <v>0.55718485530399997</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-3</v>
+        <v>0-1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0.118674724674</v>
+        <v>0.64328633630800003</v>
       </c>
       <c r="B9" s="1">
-        <v>1.7085927555359999</v>
+        <v>3.9223373886899995</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-2</v>
+        <v>1-4</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>VLOOKUP(E9,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -777,38 +777,38 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1.4240966960880002</v>
+        <v>2.3576334448880001</v>
       </c>
       <c r="B10" s="1">
-        <v>0.54914767160400002</v>
+        <v>0.23860484835200005</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1.9556249964999999</v>
+        <v>1.036361072816</v>
       </c>
       <c r="B11" s="1">
-        <v>1.1255225100000001</v>
+        <v>0.85891745284800014</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="4"/>
@@ -816,23 +816,23 @@
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>VLOOKUP(E11,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.1487541722600001</v>
+        <v>7.1370871779999998E-2</v>
       </c>
       <c r="B12" s="1">
-        <v>0.53057129168400008</v>
+        <v>0.63895347991800011</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="4"/>
@@ -840,19 +840,19 @@
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.6081872690600001</v>
+        <v>1.9345433386019999</v>
       </c>
       <c r="B13" s="1">
-        <v>0.63678983507999998</v>
+        <v>1.0498213319360004</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="3"/>
@@ -873,10 +873,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.0051703174320001</v>
+        <v>0.97887657152399987</v>
       </c>
       <c r="B14" s="1">
-        <v>1.0834066645639999</v>
+        <v>1.633112071422</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="3"/>
@@ -884,23 +884,23 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>VLOOKUP(E14,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.493306373776</v>
+        <v>1.3420984317479998</v>
       </c>
       <c r="B15" s="1">
-        <v>0.13265115528000002</v>
+        <v>0.77801913573999992</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
@@ -908,23 +908,23 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>1-1</v>
       </c>
       <c r="F15" s="2" t="str">
         <f>VLOOKUP(E15,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.2635731611360002</v>
+        <v>0.63586012561200012</v>
       </c>
       <c r="B16" s="1">
-        <v>0.42454084332800002</v>
+        <v>0.5264025207980001</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="3"/>
@@ -932,23 +932,23 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>1-1</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>VLOOKUP(E16,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>0.93505449180000011</v>
+        <v>0.51456506841600003</v>
       </c>
       <c r="B17" s="1">
-        <v>0.44999999999999996</v>
+        <v>1.3372236550679999</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="3"/>
@@ -956,27 +956,27 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>1-1</v>
       </c>
       <c r="F17" s="2" t="str">
         <f>VLOOKUP(E17,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>3.1167316485759997</v>
+        <v>1.2561491813219998</v>
       </c>
       <c r="B18" s="1">
-        <v>0.75</v>
+        <v>1.0150597182179999</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="4"/>
@@ -984,19 +984,19 @@
       </c>
       <c r="E18" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-1</v>
+        <v>1-1</v>
       </c>
       <c r="F18" s="2" t="str">
         <f>VLOOKUP(E18,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.363616970976</v>
+        <v>1.427417458758</v>
       </c>
       <c r="B19" s="1">
-        <v>2.25</v>
+        <v>2.1454700410000003</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="3"/>
@@ -1017,10 +1017,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1.6331059347539996</v>
+        <v>1.6017034783320001</v>
       </c>
       <c r="B20" s="1">
-        <v>1.1712019835879999</v>
+        <v>1.1451896360840002</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="3"/>
@@ -1041,14 +1041,14 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1.7619098275919998</v>
+        <v>1.0555603516640002</v>
       </c>
       <c r="B21" s="1">
-        <v>0.66811357579200015</v>
+        <v>0.52063785282600006</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="4"/>
@@ -1056,19 +1056,19 @@
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F21" s="2" t="str">
         <f>VLOOKUP(E21,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>0.58887788091600002</v>
+        <v>0.69370277985900008</v>
       </c>
       <c r="B22" s="1">
-        <v>1.0932331214220001</v>
+        <v>1.2131274004250001</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="3"/>
@@ -1089,14 +1089,14 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1.2154287319199999</v>
+        <v>1.5145132882229999</v>
       </c>
       <c r="B23" s="1">
-        <v>1.04032163824</v>
+        <v>0.85746003314999997</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="4"/>
@@ -1104,43 +1104,43 @@
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F23" s="2" t="str">
         <f>VLOOKUP(E23,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>2.1391371129599994</v>
+        <v>0.84198030393599999</v>
       </c>
       <c r="B24" s="1">
-        <v>0.32007029471999993</v>
+        <v>0.63335797994700005</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-0</v>
+        <v>1-1</v>
       </c>
       <c r="F24" s="2" t="str">
         <f>VLOOKUP(E24,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0.56294867889599998</v>
+        <v>0.96497283770400011</v>
       </c>
       <c r="B25" s="1">
-        <v>1.3063704095700002</v>
+        <v>1.560057596482</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="3"/>
@@ -1148,35 +1148,35 @@
       </c>
       <c r="D25" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F25" s="2" t="str">
         <f>VLOOKUP(E25,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1.6474923583279999</v>
+        <v>1.2865860040080002</v>
       </c>
       <c r="B26" s="1">
-        <v>0.55979650125000013</v>
+        <v>0.44574121835599995</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-0</v>
       </c>
       <c r="F26" s="2" t="str">
         <f>VLOOKUP(E26,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1185,2307 +1185,817 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1.3349849218320002</v>
+        <v>1.6081658418320002</v>
       </c>
       <c r="B27" s="1">
-        <v>0.934105034226</v>
+        <v>7.4274648126000001E-2</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F27" s="2" t="str">
         <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1.032980224248</v>
+        <v>2.5731453452320001</v>
       </c>
       <c r="B28" s="1">
-        <v>0.52987407548400001</v>
+        <v>0.22289394157799999</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>3-0</v>
       </c>
       <c r="F28" s="2" t="str">
         <f>VLOOKUP(E28,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>4.0146284771499996</v>
+        <v>1.4460161464549999</v>
       </c>
       <c r="B29" s="1">
-        <v>0.49705995201399999</v>
+        <v>1.084476583476</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>4-0</v>
+        <v>1-1</v>
       </c>
       <c r="F29" s="2" t="str">
         <f>VLOOKUP(E29,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>1.7650115431</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1.3806235677760001</v>
-      </c>
-      <c r="C30" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E30" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F30" s="2" t="str">
-        <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>1.7184573924839999</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.72535379886999984</v>
-      </c>
-      <c r="C31" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E31" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F31" s="2" t="str">
-        <f>VLOOKUP(E31,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>0.81057162959999995</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1.03248940212</v>
-      </c>
-      <c r="C32" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F32" s="2" t="str">
-        <f>VLOOKUP(E32,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>0.88582052467799999</v>
-      </c>
-      <c r="B33" s="1">
-        <v>1.0684692176249999</v>
-      </c>
-      <c r="C33" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E33" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F33" s="2" t="str">
-        <f>VLOOKUP(E33,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>0.68739618394799995</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1.44486242873</v>
-      </c>
-      <c r="C34" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E34" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F34" s="2" t="str">
-        <f>VLOOKUP(E34,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>2.5251330406499997</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0.85477003925999995</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-1</v>
-      </c>
-      <c r="F35" s="2" t="str">
-        <f>VLOOKUP(E35,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>0.90593773514999998</v>
-      </c>
-      <c r="B36" s="1">
-        <v>1.2875386766950001</v>
-      </c>
-      <c r="C36" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E36" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F36" s="2" t="str">
-        <f>VLOOKUP(E36,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>2.7681864146159998</v>
-      </c>
-      <c r="B37" s="1">
-        <v>1.6954175150880002</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E37" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-2</v>
-      </c>
-      <c r="F37" s="2" t="str">
-        <f>VLOOKUP(E37,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>0.9903048920819999</v>
-      </c>
-      <c r="B38" s="1">
-        <v>0.22972115287200001</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F38" s="2" t="str">
-        <f>VLOOKUP(E38,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>1.9254511808730002</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1.1486807631040001</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E39" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F39" s="2" t="str">
-        <f>VLOOKUP(E39,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>1.320406522776</v>
-      </c>
-      <c r="B40" s="1">
-        <v>0.321657947512</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F40" s="2" t="str">
-        <f>VLOOKUP(E40,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>1.1139430066380001</v>
-      </c>
-      <c r="B41" s="1">
-        <v>1.148639095926</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E41" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F41" s="2" t="str">
-        <f>VLOOKUP(E41,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>0.55384871506799993</v>
-      </c>
-      <c r="B42" s="1">
-        <v>1.464443790732</v>
-      </c>
-      <c r="C42" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E42" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F42" s="2" t="str">
-        <f>VLOOKUP(E42,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>0.31649926572000003</v>
-      </c>
-      <c r="B43" s="1">
-        <v>2.135690944632</v>
-      </c>
-      <c r="C43" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E43" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-2</v>
-      </c>
-      <c r="F43" s="2" t="str">
-        <f>VLOOKUP(E43,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>1.2659281915930001</v>
-      </c>
-      <c r="B44" s="1">
-        <v>1.1566457897940001</v>
-      </c>
-      <c r="C44" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E44" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F44" s="2" t="str">
-        <f>VLOOKUP(E44,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>1.4065146580869998</v>
-      </c>
-      <c r="B45" s="1">
-        <v>1.0281407024789999</v>
-      </c>
-      <c r="C45" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D45" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E45" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F45" s="2" t="str">
-        <f>VLOOKUP(E45,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>1.977987799696</v>
-      </c>
-      <c r="B46" s="1">
-        <v>1.3494534227459998</v>
-      </c>
-      <c r="C46" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D46" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E46" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F46" s="2" t="str">
-        <f>VLOOKUP(E46,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>1.054868493531</v>
-      </c>
-      <c r="B47" s="1">
-        <v>0.69388747510499993</v>
-      </c>
-      <c r="C47" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D47" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E47" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F47" s="2" t="str">
-        <f>VLOOKUP(E47,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>1.7479099312500002</v>
-      </c>
-      <c r="B48" s="1">
-        <v>0.83115116700000002</v>
-      </c>
-      <c r="C48" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D48" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E48" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F48" s="2" t="str">
-        <f>VLOOKUP(E48,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>0.94124353050000009</v>
-      </c>
-      <c r="B49" s="1">
-        <v>0.1058332275</v>
-      </c>
-      <c r="C49" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D49" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E49" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F49" s="2" t="str">
-        <f>VLOOKUP(E49,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>1.918952772128</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1.1405882386080002</v>
-      </c>
-      <c r="C50" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D50" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E50" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F50" s="2" t="str">
-        <f>VLOOKUP(E50,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>1.2593127567090001</v>
-      </c>
-      <c r="B51" s="1">
-        <v>0.80187610337999993</v>
-      </c>
-      <c r="C51" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D51" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E51" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F51" s="2" t="str">
-        <f>VLOOKUP(E51,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>1.7876231822970001</v>
-      </c>
-      <c r="B52" s="1">
-        <v>2.5332652575999997</v>
-      </c>
-      <c r="C52" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D52" s="3">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E52" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-3</v>
-      </c>
-      <c r="F52" s="2" t="str">
-        <f>VLOOKUP(E52,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>1.435921881916</v>
-      </c>
-      <c r="B53" s="1">
-        <v>0.636782691776</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E53" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F53" s="2" t="str">
-        <f>VLOOKUP(E53,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>1.1486708386240001</v>
-      </c>
-      <c r="B54" s="1">
-        <v>0.39799632566400001</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F54" s="2" t="str">
-        <f>VLOOKUP(E54,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>0.68926393204000003</v>
-      </c>
-      <c r="B55" s="1">
-        <v>0.47758701883200005</v>
-      </c>
-      <c r="C55" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F55" s="2" t="str">
-        <f>VLOOKUP(E55,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>0.98469541344000011</v>
-      </c>
-      <c r="B56" s="1">
-        <v>0.72775981152000013</v>
-      </c>
-      <c r="C56" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E56" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F56" s="2" t="str">
-        <f>VLOOKUP(E56,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>0.41562422116800002</v>
-      </c>
-      <c r="B57" s="1">
-        <v>2.8444888875000003</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E57" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-3</v>
-      </c>
-      <c r="F57" s="2" t="str">
-        <f>VLOOKUP(E57,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>2.727233941952</v>
-      </c>
-      <c r="B58" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="C58" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D58" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E58" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-1</v>
-      </c>
-      <c r="F58" s="2" t="str">
-        <f>VLOOKUP(E58,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>1.51935105465</v>
-      </c>
-      <c r="B59" s="1">
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="C59" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D59" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E59" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-0</v>
-      </c>
-      <c r="F59" s="2" t="str">
-        <f>VLOOKUP(E59,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>1.9783793252240001</v>
-      </c>
-      <c r="B60" s="1">
-        <v>0.60736234135199996</v>
-      </c>
-      <c r="C60" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D60" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E60" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F60" s="2" t="str">
-        <f>VLOOKUP(E60,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>0.61172702267000001</v>
-      </c>
-      <c r="B61" s="1">
-        <v>1.3519708076160002</v>
-      </c>
-      <c r="C61" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D61" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E61" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F61" s="2" t="str">
-        <f>VLOOKUP(E61,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>1.6331059347539998</v>
-      </c>
-      <c r="B62" s="1">
-        <v>1.3535311389860001</v>
-      </c>
-      <c r="C62" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D62" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E62" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F62" s="2" t="str">
-        <f>VLOOKUP(E62,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>1.884314678712</v>
-      </c>
-      <c r="B63" s="1">
-        <v>1.1105534754599999</v>
-      </c>
-      <c r="C63" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D63" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E63" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F63" s="2" t="str">
-        <f>VLOOKUP(E63,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>1.4464005603390002</v>
-      </c>
-      <c r="B64" s="1">
-        <v>0.10545756709200001</v>
-      </c>
-      <c r="C64" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D64" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E64" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F64" s="2" t="str">
-        <f>VLOOKUP(E64,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>1.2959837028000001</v>
-      </c>
-      <c r="B65" s="1">
-        <v>0.81001012500000014</v>
-      </c>
-      <c r="C65" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D65" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E65" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F65" s="2" t="str">
-        <f>VLOOKUP(E65,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>1.9285340804520001</v>
-      </c>
-      <c r="B66" s="1">
-        <v>0.31642270486399998</v>
-      </c>
-      <c r="C66" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D66" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E66" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-0</v>
-      </c>
-      <c r="F66" s="2" t="str">
-        <f>VLOOKUP(E66,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>1.8514567176389998</v>
-      </c>
-      <c r="B67" s="1">
-        <v>1.4174577180000001</v>
-      </c>
-      <c r="C67" s="3">
-        <f t="shared" ref="C67:C122" si="6">ROUND(A67,0)</f>
-        <v>2</v>
-      </c>
-      <c r="D67" s="3">
-        <f t="shared" ref="D67:D122" si="7">ROUND(B67,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E67" s="4" t="str">
-        <f t="shared" ref="E67:E122" si="8">CONCATENATE(C67,"-",D67)</f>
-        <v>2-1</v>
-      </c>
-      <c r="F67" s="2" t="str">
-        <f>VLOOKUP(E67,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>2.221792062774</v>
-      </c>
-      <c r="B68" s="1">
-        <v>1.1811447670880002</v>
-      </c>
-      <c r="C68" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D68" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E68" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F68" s="2" t="str">
-        <f>VLOOKUP(E68,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="4"/>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>2.0796166368</v>
-      </c>
-      <c r="B69" s="1">
-        <v>0.79231647983999987</v>
-      </c>
-      <c r="C69" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D69" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E69" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F69" s="2" t="str">
-        <f>VLOOKUP(E69,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="4"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>1.4037412298399998</v>
-      </c>
-      <c r="B70" s="1">
-        <v>0.8642088873599999</v>
-      </c>
-      <c r="C70" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D70" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E70" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F70" s="2" t="str">
-        <f>VLOOKUP(E70,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>0.49507669007999999</v>
-      </c>
-      <c r="B71" s="1">
-        <v>0.88024457247999988</v>
-      </c>
-      <c r="C71" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D71" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E71" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-1</v>
-      </c>
-      <c r="F71" s="2" t="str">
-        <f>VLOOKUP(E71,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>1.5152221216799999</v>
-      </c>
-      <c r="B72" s="1">
-        <v>0.39214179263999993</v>
-      </c>
-      <c r="C72" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D72" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E72" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F72" s="2" t="str">
-        <f>VLOOKUP(E72,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>0.53403778049999995</v>
-      </c>
-      <c r="B73" s="1">
-        <v>0.98907970171400006</v>
-      </c>
-      <c r="C73" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D73" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E73" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F73" s="2" t="str">
-        <f>VLOOKUP(E73,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>0.62300407441999994</v>
-      </c>
-      <c r="B74" s="1">
-        <v>1.0687467207899999</v>
-      </c>
-      <c r="C74" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D74" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E74" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F74" s="2" t="str">
-        <f>VLOOKUP(E74,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>0.78909582457999994</v>
-      </c>
-      <c r="B75" s="1">
-        <v>1.3490941527140001</v>
-      </c>
-      <c r="C75" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D75" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E75" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F75" s="2" t="str">
-        <f>VLOOKUP(E75,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>2.5365605939189999</v>
-      </c>
-      <c r="B76" s="1">
-        <v>0.85886160749999996</v>
-      </c>
-      <c r="C76" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D76" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E76" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F76" s="2" t="str">
-        <f>VLOOKUP(E76,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>0.82284471917999991</v>
-      </c>
-      <c r="B77" s="1">
-        <v>0.89216872838999994</v>
-      </c>
-      <c r="C77" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D77" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E77" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F77" s="2" t="str">
-        <f>VLOOKUP(E77,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>3.0782617458659995</v>
-      </c>
-      <c r="B78" s="1">
-        <v>0.85727550876000003</v>
-      </c>
-      <c r="C78" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D78" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E78" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F78" s="2" t="str">
-        <f>VLOOKUP(E78,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>1.5739755479100002</v>
-      </c>
-      <c r="B79" s="1">
-        <v>0.67120278875000006</v>
-      </c>
-      <c r="C79" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D79" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E79" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F79" s="2" t="str">
-        <f>VLOOKUP(E79,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>1.4235821575919998</v>
-      </c>
-      <c r="B80" s="1">
-        <v>1.1125677457259999</v>
-      </c>
-      <c r="C80" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D80" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E80" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F80" s="2" t="str">
-        <f>VLOOKUP(E80,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>1.5100362249000001</v>
-      </c>
-      <c r="B81" s="1">
-        <v>1.8543240193659998</v>
-      </c>
-      <c r="C81" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D81" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E81" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-2</v>
-      </c>
-      <c r="F81" s="2" t="str">
-        <f>VLOOKUP(E81,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>0.65911581180900014</v>
-      </c>
-      <c r="B82" s="1">
-        <v>2.3349767515059998</v>
-      </c>
-      <c r="C82" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D82" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E82" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F82" s="2" t="str">
-        <f>VLOOKUP(E82,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>1.2583168542000001</v>
-      </c>
-      <c r="B83" s="1">
-        <v>2.0661401008619995</v>
-      </c>
-      <c r="C83" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D83" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E83" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F83" s="2" t="str">
-        <f>VLOOKUP(E83,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>2.0492647178850003</v>
-      </c>
-      <c r="B84" s="1">
-        <v>0.63578156815800002</v>
-      </c>
-      <c r="C84" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D84" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E84" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F84" s="2" t="str">
-        <f>VLOOKUP(E84,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>1.6178388110220001</v>
-      </c>
-      <c r="B85" s="1">
-        <v>1.08083666614</v>
-      </c>
-      <c r="C85" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D85" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E85" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F85" s="2" t="str">
-        <f>VLOOKUP(E85,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>1.320406522776</v>
-      </c>
-      <c r="B86" s="1">
-        <v>2.7568038319520003</v>
-      </c>
-      <c r="C86" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D86" s="3">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="E86" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-3</v>
-      </c>
-      <c r="F86" s="2" t="str">
-        <f>VLOOKUP(E86,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>2.640813045552</v>
-      </c>
-      <c r="B87" s="1">
-        <v>0.22976282005000004</v>
-      </c>
-      <c r="C87" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D87" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E87" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-0</v>
-      </c>
-      <c r="F87" s="2" t="str">
-        <f>VLOOKUP(E87,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>1.4440446373319999</v>
-      </c>
-      <c r="B88" s="1">
-        <v>0.34461922868000006</v>
-      </c>
-      <c r="C88" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D88" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E88" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F88" s="2" t="str">
-        <f>VLOOKUP(E88,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>1.1394293585399999</v>
-      </c>
-      <c r="B89" s="1">
-        <v>0.14645137838800001</v>
-      </c>
-      <c r="C89" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D89" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E89" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F89" s="2" t="str">
-        <f>VLOOKUP(E89,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>2.373594493248</v>
-      </c>
-      <c r="B90" s="1">
-        <v>0.54914767160400002</v>
-      </c>
-      <c r="C90" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D90" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E90" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F90" s="2" t="str">
-        <f>VLOOKUP(E90,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>0.35602417402200004</v>
-      </c>
-      <c r="B91" s="1">
-        <v>2.562889133304</v>
-      </c>
-      <c r="C91" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D91" s="3">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="E91" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-3</v>
-      </c>
-      <c r="F91" s="2" t="str">
-        <f>VLOOKUP(E91,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>0.69229839386400005</v>
-      </c>
-      <c r="B92" s="1">
-        <v>0.45764805956399995</v>
-      </c>
-      <c r="C92" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D92" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E92" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F92" s="2" t="str">
-        <f>VLOOKUP(E92,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>2.6257051388699999</v>
-      </c>
-      <c r="B93" s="1">
-        <v>0</v>
-      </c>
-      <c r="C93" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D93" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E93" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-0</v>
-      </c>
-      <c r="F93" s="2" t="str">
-        <f>VLOOKUP(E93,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>1.6410365450700002</v>
-      </c>
-      <c r="B94" s="1">
-        <v>0.77113052784899994</v>
-      </c>
-      <c r="C94" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D94" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E94" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F94" s="2" t="str">
-        <f>VLOOKUP(E94,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <v>0.65937093297499993</v>
-      </c>
-      <c r="B95" s="1">
-        <v>0.57824789517000008</v>
-      </c>
-      <c r="C95" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D95" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E95" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F95" s="2" t="str">
-        <f>VLOOKUP(E95,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>2.461454815378</v>
-      </c>
-      <c r="B96" s="1">
-        <v>0.8674468424820001</v>
-      </c>
-      <c r="C96" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D96" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E96" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F96" s="2" t="str">
-        <f>VLOOKUP(E96,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>0.95072174662500009</v>
-      </c>
-      <c r="B97" s="1">
-        <v>0.57722164499999995</v>
-      </c>
-      <c r="C97" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D97" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E97" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F97" s="2" t="str">
-        <f>VLOOKUP(E97,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>1.5401785035</v>
-      </c>
-      <c r="B98" s="1">
-        <v>1.0476209520000002</v>
-      </c>
-      <c r="C98" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D98" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E98" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F98" s="2" t="str">
-        <f>VLOOKUP(E98,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>0.88005524774999999</v>
-      </c>
-      <c r="B99" s="1">
-        <v>1.4545636349999997</v>
-      </c>
-      <c r="C99" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D99" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E99" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F99" s="2" t="str">
-        <f>VLOOKUP(E99,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>1.9678564709999999</v>
-      </c>
-      <c r="B100" s="1">
-        <v>1.0389989610000001</v>
-      </c>
-      <c r="C100" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D100" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E100" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F100" s="2" t="str">
-        <f>VLOOKUP(E100,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>1.9917476845000002</v>
-      </c>
-      <c r="B101" s="1">
-        <v>1.1287633140000002</v>
-      </c>
-      <c r="C101" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D101" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E101" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F101" s="2" t="str">
-        <f>VLOOKUP(E101,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>3.358167351224</v>
-      </c>
-      <c r="B102" s="1">
-        <v>0.85537450908000001</v>
-      </c>
-      <c r="C102" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D102" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E102" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F102" s="2" t="str">
-        <f>VLOOKUP(E102,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>5.0372510268360005</v>
-      </c>
-      <c r="B103" s="1">
-        <v>0.85537450908000001</v>
-      </c>
-      <c r="C103" s="3">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="D103" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E103" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>5-1</v>
-      </c>
-      <c r="F103" s="2" t="str">
-        <f>VLOOKUP(E103,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>2.4285246007049999</v>
-      </c>
-      <c r="B104" s="1">
-        <v>2.3523799047840002</v>
-      </c>
-      <c r="C104" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D104" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E104" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-2</v>
-      </c>
-      <c r="F104" s="2" t="str">
-        <f>VLOOKUP(E104,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>1.804885001865</v>
-      </c>
-      <c r="B105" s="1">
-        <v>1.2665909632530001</v>
-      </c>
-      <c r="C105" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D105" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E105" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F105" s="2" t="str">
-        <f>VLOOKUP(E105,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>0.80546100574500012</v>
-      </c>
-      <c r="B106" s="1">
-        <v>1.283090519865</v>
-      </c>
-      <c r="C106" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D106" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E106" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F106" s="2" t="str">
-        <f>VLOOKUP(E106,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>2.2001131471050002</v>
-      </c>
-      <c r="B107" s="1">
-        <v>1.2408237985439998</v>
-      </c>
-      <c r="C107" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D107" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E107" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F107" s="2" t="str">
-        <f>VLOOKUP(E107,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="2"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <v>1.804885001865</v>
-      </c>
-      <c r="B108" s="1">
-        <v>0.86861665974800006</v>
-      </c>
-      <c r="C108" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D108" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E108" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F108" s="2" t="str">
-        <f>VLOOKUP(E108,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="2"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <v>1.21155217209</v>
-      </c>
-      <c r="B109" s="1">
-        <v>1.2471085380100002</v>
-      </c>
-      <c r="C109" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D109" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E109" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F109" s="2" t="str">
-        <f>VLOOKUP(E109,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>1.3658801690160001</v>
-      </c>
-      <c r="B110" s="1">
-        <v>0.94095668409000011</v>
-      </c>
-      <c r="C110" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D110" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E110" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F110" s="2" t="str">
-        <f>VLOOKUP(E110,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>1.1068376247180001</v>
-      </c>
-      <c r="B111" s="1">
-        <v>0.42951208315200001</v>
-      </c>
-      <c r="C111" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D111" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E111" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F111" s="2" t="str">
-        <f>VLOOKUP(E111,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>2.0234272229820003</v>
-      </c>
-      <c r="B112" s="1">
-        <v>0.74015147421199989</v>
-      </c>
-      <c r="C112" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D112" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E112" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F112" s="2" t="str">
-        <f>VLOOKUP(E112,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>1.6485879471660001</v>
-      </c>
-      <c r="B113" s="1">
-        <v>0.63171211600600008</v>
-      </c>
-      <c r="C113" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D113" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E113" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F113" s="2" t="str">
-        <f>VLOOKUP(E113,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <v>0.89022053870100015</v>
-      </c>
-      <c r="B114" s="1">
-        <v>0.94756817400900006</v>
-      </c>
-      <c r="C114" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D114" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E114" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F114" s="2" t="str">
-        <f>VLOOKUP(E114,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="2"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <v>0.68929488524400007</v>
-      </c>
-      <c r="B115" s="1">
-        <v>0.63669221590800007</v>
-      </c>
-      <c r="C115" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D115" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E115" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F115" s="2" t="str">
-        <f>VLOOKUP(E115,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>1.6848165952800001</v>
-      </c>
-      <c r="B116" s="1">
-        <v>1.8572852351060003</v>
-      </c>
-      <c r="C116" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D116" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E116" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-2</v>
-      </c>
-      <c r="F116" s="2" t="str">
-        <f>VLOOKUP(E116,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>0.84792360470700001</v>
-      </c>
-      <c r="B117" s="1">
-        <v>0.36443831470799998</v>
-      </c>
-      <c r="C117" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D117" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E117" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F117" s="2" t="str">
-        <f>VLOOKUP(E117,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>1.5816122732159998</v>
-      </c>
-      <c r="B118" s="1">
-        <v>0.92813179513999999</v>
-      </c>
-      <c r="C118" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D118" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E118" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F118" s="2" t="str">
-        <f>VLOOKUP(E118,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="2"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>0.72692480321099995</v>
-      </c>
-      <c r="B119" s="1">
-        <v>1.1367465216799999</v>
-      </c>
-      <c r="C119" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D119" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E119" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F119" s="2" t="str">
-        <f>VLOOKUP(E119,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="2"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>1.422823638816</v>
-      </c>
-      <c r="B120" s="1">
-        <v>1.002219222196</v>
-      </c>
-      <c r="C120" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D120" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E120" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F120" s="2" t="str">
-        <f>VLOOKUP(E120,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="2"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>0.98444094465599985</v>
-      </c>
-      <c r="B121" s="1">
-        <v>0.91872531135000002</v>
-      </c>
-      <c r="C121" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D121" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E121" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F121" s="2" t="str">
-        <f>VLOOKUP(E121,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>0.57438779974400012</v>
-      </c>
-      <c r="B122" s="1">
-        <v>0.63678269177600011</v>
-      </c>
-      <c r="C122" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D122" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E122" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F122" s="2" t="str">
-        <f>VLOOKUP(E122,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="2"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>

</xml_diff>

<commit_message>
updated myodds and myoddsnewleagues
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -553,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E35"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0.9988674929400001</v>
+        <v>1.028171600456</v>
       </c>
       <c r="B1" s="1">
-        <v>1.4494357566980001</v>
+        <v>2.2792454277119996</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
@@ -572,27 +572,27 @@
       </c>
       <c r="D1" s="3">
         <f>ROUND(B1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>VLOOKUP(E1,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.62439932565</v>
+        <v>1.846070717106</v>
       </c>
       <c r="B2" s="1">
-        <v>1.054126004647</v>
+        <v>0.65846984070000003</v>
       </c>
       <c r="C2" s="3">
         <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2" si="1">ROUND(B2,0)</f>
@@ -600,43 +600,43 @@
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(E2,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.42814167975000006</v>
+        <v>2.373594493248</v>
       </c>
       <c r="B3" s="1">
-        <v>0.37642357320999997</v>
+        <v>0.71839209613499999</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C35" si="3">ROUND(A3,0)</f>
-        <v>0</v>
+        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
+        <v>2</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D35" si="4">ROUND(B3,0)</f>
-        <v>0</v>
+        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
+        <v>1</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3:E35" si="5">CONCATENATE(C3,"-",D3)</f>
-        <v>0-0</v>
+        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
+        <v>2-1</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.3747923678959999</v>
+        <v>1.1720964119939998</v>
       </c>
       <c r="B4" s="1">
-        <v>1.3645521707699999</v>
+        <v>0.67668433462799993</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="3"/>
@@ -657,86 +657,86 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0.85623335755200003</v>
+        <v>2.1504000000000003</v>
       </c>
       <c r="B5" s="1">
-        <v>1.1293189325639998</v>
+        <v>0.41510691334199995</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.85628335950000012</v>
+        <v>3.9822111093750006</v>
       </c>
       <c r="B6" s="1">
-        <v>0.67766314576999997</v>
+        <v>0.192266162928</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>4-0</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1.9082518951500003</v>
+        <v>0.48766095000000004</v>
       </c>
       <c r="B7" s="1">
-        <v>1.5488708631499999</v>
+        <v>0.78766769250000013</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>0-1</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.39145606635000002</v>
+        <v>1.2800600006249998</v>
       </c>
       <c r="B8" s="1">
-        <v>0.96798714689599996</v>
+        <v>0.98462461499999998</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="4"/>
@@ -744,23 +744,23 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-1</v>
+        <v>1-1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2.5115407136820003</v>
+        <v>1.5973612907219998</v>
       </c>
       <c r="B9" s="1">
-        <v>0.56470678743799996</v>
+        <v>0.67051402685999995</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="4"/>
@@ -768,7 +768,7 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-1</v>
+        <v>2-1</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>VLOOKUP(E9,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -777,10 +777,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>0.97266751181999989</v>
+        <v>0.53819084847999998</v>
       </c>
       <c r="B10" s="1">
-        <v>0.922986646036</v>
+        <v>0.17247217169699999</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="3"/>
@@ -788,23 +788,23 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1.860171101793</v>
+        <v>2.1090294416399997</v>
       </c>
       <c r="B11" s="1">
-        <v>1.0559291681249998</v>
+        <v>1.4948356808759999</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="3"/>
@@ -825,14 +825,14 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.7171733232980002</v>
+        <v>2.9063513178</v>
       </c>
       <c r="B12" s="1">
-        <v>0.67120278875000006</v>
+        <v>0.5338934137350001</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="4"/>
@@ -840,7 +840,7 @@
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>3-1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -849,14 +849,14 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.48778321118399998</v>
+        <v>1.7155712637</v>
       </c>
       <c r="B13" s="1">
-        <v>1.1301553692000001</v>
+        <v>0.61802941680000001</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="4"/>
@@ -864,19 +864,19 @@
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-1</v>
+        <v>2-1</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>VLOOKUP(E13,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.1417444806320001</v>
+        <v>1.4800474300950002</v>
       </c>
       <c r="B14" s="1">
-        <v>1.183127147372</v>
+        <v>1.8127529495999999</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="3"/>
@@ -884,23 +884,23 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>VLOOKUP(E14,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.1416694777100003</v>
+        <v>1.2809751669000002</v>
       </c>
       <c r="B15" s="1">
-        <v>0.67766314576999997</v>
+        <v>0.60988697840000006</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
@@ -921,22 +921,22 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2.2263867366480001</v>
+        <v>1.2916529821200002</v>
       </c>
       <c r="B16" s="1">
-        <v>1.844645506282</v>
+        <v>0.72821966139999994</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>VLOOKUP(E16,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -945,10 +945,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1.1417444806320001</v>
+        <v>0.51670939500000002</v>
       </c>
       <c r="B17" s="1">
-        <v>0.67766314576999997</v>
+        <v>2.0164813669999999</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="3"/>
@@ -956,23 +956,23 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F17" s="2" t="str">
         <f>VLOOKUP(E17,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.3491376123499998</v>
+        <v>1.4117958693600003</v>
       </c>
       <c r="B18" s="1">
-        <v>0.64105490930000009</v>
+        <v>1.1096299591999998</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="3"/>
@@ -993,14 +993,14 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>2.0271157302959995</v>
+        <v>1.0908717108299999</v>
       </c>
       <c r="B19" s="1">
-        <v>0.85727550876000003</v>
+        <v>0.93125128751200004</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="4"/>
@@ -1008,19 +1008,19 @@
       </c>
       <c r="E19" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F19" s="2" t="str">
         <f>VLOOKUP(E19,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1.004202947232</v>
+        <v>0.76918432519500013</v>
       </c>
       <c r="B20" s="1">
-        <v>1.4206176238349999</v>
+        <v>0.40243156778999994</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="3"/>
@@ -1028,23 +1028,23 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F20" s="2" t="str">
         <f>VLOOKUP(E20,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1.0520939496869999</v>
+        <v>1.4025073503209999</v>
       </c>
       <c r="B21" s="1">
-        <v>1.250357644795</v>
+        <v>1.3569378494</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="3"/>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.3196771779879999</v>
+        <v>0.77410948272500013</v>
       </c>
       <c r="B22" s="1">
-        <v>0.74572153703999999</v>
+        <v>1.0805812699919999</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="3"/>
@@ -1089,34 +1089,34 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1.6802090628050002</v>
+        <v>0.31788389403000006</v>
       </c>
       <c r="B23" s="1">
-        <v>1.4490489279300001</v>
+        <v>2.1687451735679999</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>0-2</v>
       </c>
       <c r="F23" s="2" t="str">
         <f>VLOOKUP(E23,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1.0204884680899999</v>
+        <v>1.1191654803499997</v>
       </c>
       <c r="B24" s="1">
-        <v>0.58705667405999995</v>
+        <v>1.8636306285239999</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="3"/>
@@ -1124,35 +1124,35 @@
       </c>
       <c r="D24" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F24" s="2" t="str">
         <f>VLOOKUP(E24,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1.7450428355099998</v>
+        <v>1.438798474872</v>
       </c>
       <c r="B25" s="1">
-        <v>1.83081412098</v>
+        <v>0.53030836900799994</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
       <c r="F25" s="2" t="str">
         <f>VLOOKUP(E25,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1161,34 +1161,34 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1.4139530968680001</v>
+        <v>0.42968221328799988</v>
       </c>
       <c r="B26" s="1">
-        <v>0.94908065734200009</v>
+        <v>1.567561804875</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-2</v>
       </c>
       <c r="F26" s="2" t="str">
         <f>VLOOKUP(E26,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1.256821802548</v>
+        <v>1.3519993487399997</v>
       </c>
       <c r="B27" s="1">
-        <v>0.88125856927500013</v>
+        <v>0.40397483095199993</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="3"/>
@@ -1196,23 +1196,23 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F27" s="2" t="str">
         <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1.0354590145639999</v>
+        <v>0.80930070586199998</v>
       </c>
       <c r="B28" s="1">
-        <v>0.77868083370600016</v>
+        <v>1.122224530392</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="3"/>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>1.7312377484220001</v>
+        <v>2.2049410759199999</v>
       </c>
       <c r="B29" s="1">
-        <v>1.3060417499039998</v>
+        <v>0.99416580956</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="3"/>
@@ -1257,14 +1257,14 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1.8967978642859999</v>
+        <v>1.116180661122</v>
       </c>
       <c r="B30" s="1">
-        <v>0.56694977971500005</v>
+        <v>1.1667946057499998</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="4"/>
@@ -1272,19 +1272,19 @@
       </c>
       <c r="E30" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F30" s="2" t="str">
         <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>0.85609416882600009</v>
+        <v>1.4686613967239999</v>
       </c>
       <c r="B31" s="1">
-        <v>1.1778644570399999</v>
+        <v>0.696118291</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="3"/>
@@ -1305,10 +1305,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>2.1116777702280003</v>
+        <v>1.7293495913279999</v>
       </c>
       <c r="B32" s="1">
-        <v>1.288083953778</v>
+        <v>2.1750187035840001</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="3"/>
@@ -1316,23 +1316,23 @@
       </c>
       <c r="D32" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>2-2</v>
       </c>
       <c r="F32" s="2" t="str">
         <f>VLOOKUP(E32,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>1.3133902115879998</v>
+        <v>0.74300035663999997</v>
       </c>
       <c r="B33" s="1">
-        <v>0.69598581552000005</v>
+        <v>2.4241023559260002</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="3"/>
@@ -1340,23 +1340,23 @@
       </c>
       <c r="D33" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F33" s="2" t="str">
         <f>VLOOKUP(E33,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1.3699676611500002</v>
+        <v>1.4933000000000001</v>
       </c>
       <c r="B34" s="1">
-        <v>0.64542000142800005</v>
+        <v>0.57666515579999988</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="3"/>
@@ -1377,735 +1377,2163 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1.437514168104</v>
+        <v>2.56</v>
       </c>
       <c r="B35" s="1">
-        <v>1.7283938379049999</v>
+        <v>0.77837795833200008</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D35" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>3-1</v>
       </c>
       <c r="F35" s="2" t="str">
         <f>VLOOKUP(E35,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="2"/>
+      <c r="A36" s="1">
+        <v>2.3039999999999998</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.38918897916600004</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-0</v>
+      </c>
+      <c r="F36" s="2" t="str">
+        <f>VLOOKUP(E36,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="2"/>
+      <c r="A37" s="1">
+        <v>1.4336000000000002</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.210896827442</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F37" s="2" t="str">
+        <f>VLOOKUP(E37,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="2"/>
+      <c r="A38" s="1">
+        <v>0.63497936249999998</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.71796794874999992</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F38" s="2" t="str">
+        <f>VLOOKUP(E38,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="2"/>
+      <c r="A39" s="1">
+        <v>0.10159269750000001</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.3127794874999998</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-1</v>
+      </c>
+      <c r="F39" s="2" t="str">
+        <f>VLOOKUP(E39,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="2"/>
+      <c r="A40" s="1">
+        <v>0.91428428437500009</v>
+      </c>
+      <c r="B40" s="1">
+        <v>3.6923656412499994</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E40" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-4</v>
+      </c>
+      <c r="F40" s="2" t="str">
+        <f>VLOOKUP(E40,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="2"/>
+      <c r="A41" s="1">
+        <v>0.73951911607500009</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2.2627073396200004</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E41" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F41" s="2" t="str">
+        <f>VLOOKUP(E41,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="2"/>
+      <c r="A42" s="1">
+        <v>1.7748458785800001</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2.8159229097840002</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E42" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-3</v>
+      </c>
+      <c r="F42" s="2" t="str">
+        <f>VLOOKUP(E42,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="2"/>
+      <c r="A43" s="1">
+        <v>0.98602548810000012</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.33520701238399997</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-0</v>
+      </c>
+      <c r="F43" s="2" t="str">
+        <f>VLOOKUP(E43,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="2"/>
+      <c r="A44" s="1">
+        <v>1.6787997481799999</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1.1325463211800002</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F44" s="2" t="str">
+        <f>VLOOKUP(E44,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="2"/>
+      <c r="A45" s="1">
+        <v>1.678680051458</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.75509552909000011</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F45" s="2" t="str">
+        <f>VLOOKUP(E45,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="2"/>
+      <c r="A46" s="1">
+        <v>1.805259643808</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.26137457735400005</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-0</v>
+      </c>
+      <c r="F46" s="2" t="str">
+        <f>VLOOKUP(E46,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="2"/>
+      <c r="A47" s="1">
+        <v>2.7233259780440005</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1.6464468283199998</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E47" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-2</v>
+      </c>
+      <c r="F47" s="2" t="str">
+        <f>VLOOKUP(E47,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="2"/>
+      <c r="A48" s="1">
+        <v>1.2965115266400002</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1.1177587564920002</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F48" s="2" t="str">
+        <f>VLOOKUP(E48,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="2"/>
+      <c r="A49" s="1">
+        <v>1.6123089311999999</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1.3882318760880001</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F49" s="2" t="str">
+        <f>VLOOKUP(E49,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="2"/>
+      <c r="A50" s="1">
+        <v>0.7414291009959999</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1.1642277894539999</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F50" s="2" t="str">
+        <f>VLOOKUP(E50,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="2"/>
+      <c r="A51" s="1">
+        <v>0.9226503815999999</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.207417708188</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F51" s="2" t="str">
+        <f>VLOOKUP(E51,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="2"/>
+      <c r="A52" s="1">
+        <v>0.82026330303600004</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.63879919791299988</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E52" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F52" s="2" t="str">
+        <f>VLOOKUP(E52,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="2"/>
+      <c r="A53" s="1">
+        <v>0.95684422093199994</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.51102824781300005</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F53" s="2" t="str">
+        <f>VLOOKUP(E53,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="2"/>
+      <c r="A54" s="1">
+        <v>1.3562972816400001</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1.1865764756550001</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E54" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F54" s="2" t="str">
+        <f>VLOOKUP(E54,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="2"/>
+      <c r="A55" s="1">
+        <v>0.72658782945</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.66732177109500013</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F55" s="2" t="str">
+        <f>VLOOKUP(E55,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="2"/>
+      <c r="A56" s="1">
+        <v>2.32508105424</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1.1567590639650001</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E56" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F56" s="2" t="str">
+        <f>VLOOKUP(E56,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="2"/>
+      <c r="A57" s="1">
+        <v>1.2520064977200003</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.48258936080000009</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E57" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-0</v>
+      </c>
+      <c r="F57" s="2" t="str">
+        <f>VLOOKUP(E57,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="2"/>
+      <c r="A58" s="1">
+        <v>0.91349916761999994</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.82151119040000009</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E58" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F58" s="2" t="str">
+        <f>VLOOKUP(E58,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="2"/>
+      <c r="A59" s="1">
+        <v>1.5777920184000001</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.99750440640000015</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E59" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F59" s="2" t="str">
+        <f>VLOOKUP(E59,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="2"/>
+      <c r="A60" s="1">
+        <v>0.50477333291000004</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2.3720853752959998</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E60" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F60" s="2" t="str">
+        <f>VLOOKUP(E60,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="2"/>
+      <c r="A61" s="1">
+        <v>1.8691604797249999</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.81399955718399986</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E61" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F61" s="2" t="str">
+        <f>VLOOKUP(E61,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="2"/>
+      <c r="A62" s="1">
+        <v>1.2561091726259999</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.39072445420799995</v>
+      </c>
+      <c r="C62" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E62" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-0</v>
+      </c>
+      <c r="F62" s="2" t="str">
+        <f>VLOOKUP(E62,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="2"/>
+      <c r="A63" s="1">
+        <v>2.8038240526449996</v>
+      </c>
+      <c r="B63" s="1">
+        <v>6.9746629680000005E-2</v>
+      </c>
+      <c r="C63" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E63" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-0</v>
+      </c>
+      <c r="F63" s="2" t="str">
+        <f>VLOOKUP(E63,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="2"/>
+      <c r="A64" s="1">
+        <v>1.480532169303</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1.1707183490309998</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D64" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E64" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F64" s="2" t="str">
+        <f>VLOOKUP(E64,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="2"/>
+      <c r="A65" s="1">
+        <v>1.1514931229190002</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1.0968041897759999</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D65" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F65" s="2" t="str">
+        <f>VLOOKUP(E65,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="2"/>
+      <c r="A66" s="1">
+        <v>1.3099478295929998</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1.381139323884</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D66" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E66" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F66" s="2" t="str">
+        <f>VLOOKUP(E66,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="2"/>
+      <c r="A67" s="1">
+        <v>1.0791801044389999</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.94956258301200003</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" ref="C67:C124" si="6">ROUND(A67,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D67" s="3">
+        <f t="shared" ref="D67:D124" si="7">ROUND(B67,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E67" s="4" t="str">
+        <f t="shared" ref="E67:E124" si="8">CONCATENATE(C67,"-",D67)</f>
+        <v>1-1</v>
+      </c>
+      <c r="F67" s="2" t="str">
+        <f>VLOOKUP(E67,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="4"/>
+      <c r="A68" s="1">
+        <v>2.0773970160960005</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.78732947943000009</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F68" s="2" t="str">
+        <f>VLOOKUP(E68,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="4"/>
+      <c r="A69" s="1">
+        <v>1.1960651382159999</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2.430830713158</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E69" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F69" s="2" t="str">
+        <f>VLOOKUP(E69,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="2"/>
+      <c r="A70" s="1">
+        <v>1.2801801120930001</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1.0363143692500001</v>
+      </c>
+      <c r="C70" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F70" s="2" t="str">
+        <f>VLOOKUP(E70,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="2"/>
+      <c r="A71" s="1">
+        <v>0.71060202932399985</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1.0735623703199999</v>
+      </c>
+      <c r="C71" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E71" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F71" s="2" t="str">
+        <f>VLOOKUP(E71,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="2"/>
+      <c r="A72" s="1">
+        <v>1.8939146966639997</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.42790147236499992</v>
+      </c>
+      <c r="C72" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E72" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F72" s="2" t="str">
+        <f>VLOOKUP(E72,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="2"/>
+      <c r="A73" s="1">
+        <v>2.3643019607039997</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.48488956326600002</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E73" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F73" s="2" t="str">
+        <f>VLOOKUP(E73,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="2"/>
+      <c r="A74" s="1">
+        <v>3.1901778939200005</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1.251727786464</v>
+      </c>
+      <c r="C74" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D74" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E74" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F74" s="2" t="str">
+        <f>VLOOKUP(E74,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="2"/>
+      <c r="A75" s="1">
+        <v>1.1145378078720001</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1.1334273085319999</v>
+      </c>
+      <c r="C75" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E75" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F75" s="2" t="str">
+        <f>VLOOKUP(E75,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="2"/>
+      <c r="A76" s="1">
+        <v>1.4267243221920003</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1.3332290239260001</v>
+      </c>
+      <c r="C76" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E76" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F76" s="2" t="str">
+        <f>VLOOKUP(E76,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="2"/>
+      <c r="A77" s="1">
+        <v>2.1751043474079998</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1.0504728374130001</v>
+      </c>
+      <c r="C77" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E77" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F77" s="2" t="str">
+        <f>VLOOKUP(E77,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="2"/>
+      <c r="A78" s="1">
+        <v>2.1646501306080004</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1.3852055962080001</v>
+      </c>
+      <c r="C78" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E78" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F78" s="2" t="str">
+        <f>VLOOKUP(E78,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="2"/>
+      <c r="A79" s="1">
+        <v>1.70672</v>
+      </c>
+      <c r="B79" s="1">
+        <v>1.383863040936</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E79" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F79" s="2" t="str">
+        <f>VLOOKUP(E79,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="2"/>
+      <c r="A80" s="1">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="B80" s="1">
+        <v>1.2455007372419999</v>
+      </c>
+      <c r="C80" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D80" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E80" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F80" s="2" t="str">
+        <f>VLOOKUP(E80,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="2"/>
+      <c r="A81" s="1">
+        <v>1.70672</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1.3837963744439998</v>
+      </c>
+      <c r="C81" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E81" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F81" s="2" t="str">
+        <f>VLOOKUP(E81,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="2"/>
+      <c r="A82" s="1">
+        <v>1.98098761875</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.16413076874999999</v>
+      </c>
+      <c r="C82" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D82" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E82" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F82" s="2" t="str">
+        <f>VLOOKUP(E82,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="2"/>
+      <c r="A83" s="1">
+        <v>1.23256519432</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1.3968292210559998</v>
+      </c>
+      <c r="C83" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E83" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F83" s="2" t="str">
+        <f>VLOOKUP(E83,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="2"/>
+      <c r="A84" s="1">
+        <v>1.2941334524850001</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0.29329613682</v>
+      </c>
+      <c r="C84" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E84" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-0</v>
+      </c>
+      <c r="F84" s="2" t="str">
+        <f>VLOOKUP(E84,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="2"/>
+      <c r="A85" s="1">
+        <v>0.88742293929000005</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.60336062347200015</v>
+      </c>
+      <c r="C85" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E85" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F85" s="2" t="str">
+        <f>VLOOKUP(E85,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="2"/>
+      <c r="A86" s="1">
+        <v>2.4044475544199999</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1.1247461169400002</v>
+      </c>
+      <c r="C86" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E86" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F86" s="2" t="str">
+        <f>VLOOKUP(E86,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="2"/>
+      <c r="A87" s="1">
+        <v>2.5279996207999997</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.23962923565000002</v>
+      </c>
+      <c r="C87" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D87" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E87" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-0</v>
+      </c>
+      <c r="F87" s="2" t="str">
+        <f>VLOOKUP(E87,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="2"/>
+      <c r="A88" s="1">
+        <v>1.0191998471200001</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.39600274031999999</v>
+      </c>
+      <c r="C88" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D88" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E88" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-0</v>
+      </c>
+      <c r="F88" s="2" t="str">
+        <f>VLOOKUP(E88,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="2"/>
+      <c r="A89" s="1">
+        <v>1.7312372384189998</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.63895775656000009</v>
+      </c>
+      <c r="C89" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D89" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E89" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F89" s="2" t="str">
+        <f>VLOOKUP(E89,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="2"/>
+      <c r="A90" s="1">
+        <v>0.65949990107499989</v>
+      </c>
+      <c r="B90" s="1">
+        <v>1.9007404257600002</v>
+      </c>
+      <c r="C90" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E90" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F90" s="2" t="str">
+        <f>VLOOKUP(E90,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="2"/>
+      <c r="A91" s="1">
+        <v>2.475821794572</v>
+      </c>
+      <c r="B91" s="1">
+        <v>2.1952624377599999</v>
+      </c>
+      <c r="C91" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E91" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F91" s="2" t="str">
+        <f>VLOOKUP(E91,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="2"/>
+      <c r="A92" s="1">
+        <v>2.4758317987800003</v>
+      </c>
+      <c r="B92" s="1">
+        <v>1.1432325224339999</v>
+      </c>
+      <c r="C92" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E92" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F92" s="2" t="str">
+        <f>VLOOKUP(E92,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="2"/>
+      <c r="A93" s="1">
+        <v>3.5075158844960006</v>
+      </c>
+      <c r="B93" s="1">
+        <v>1.7247462019200002</v>
+      </c>
+      <c r="C93" s="3">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E93" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>4-2</v>
+      </c>
+      <c r="F93" s="2" t="str">
+        <f>VLOOKUP(E93,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="2"/>
+      <c r="A94" s="1">
+        <v>2.5520367488</v>
+      </c>
+      <c r="B94" s="1">
+        <v>1.066960241376</v>
+      </c>
+      <c r="C94" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E94" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F94" s="2" t="str">
+        <f>VLOOKUP(E94,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="2"/>
+      <c r="A95" s="1">
+        <v>0.64536643599999999</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.55044581529600001</v>
+      </c>
+      <c r="C95" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E95" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F95" s="2" t="str">
+        <f>VLOOKUP(E95,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="2"/>
+      <c r="A96" s="1">
+        <v>1.1314448639999999</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1.4289118027140002</v>
+      </c>
+      <c r="C96" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E96" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F96" s="2" t="str">
+        <f>VLOOKUP(E96,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="2"/>
+      <c r="A97" s="1">
+        <v>1.8755270072000001</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1.5719022692520002</v>
+      </c>
+      <c r="C97" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E97" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F97" s="2" t="str">
+        <f>VLOOKUP(E97,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="2"/>
+      <c r="A98" s="1">
+        <v>1.8949201436000001</v>
+      </c>
+      <c r="B98" s="1">
+        <v>2.4937552012320001</v>
+      </c>
+      <c r="C98" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E98" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F98" s="2" t="str">
+        <f>VLOOKUP(E98,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="2"/>
+      <c r="A99" s="1">
+        <v>1.1314448640000001</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0.58972357843199996</v>
+      </c>
+      <c r="C99" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E99" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F99" s="2" t="str">
+        <f>VLOOKUP(E99,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="2"/>
+      <c r="A100" s="1">
+        <v>1.82162623104</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.83835835314000007</v>
+      </c>
+      <c r="C100" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D100" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E100" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F100" s="2" t="str">
+        <f>VLOOKUP(E100,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="2"/>
+      <c r="A101" s="1">
+        <v>2.1025902768639999</v>
+      </c>
+      <c r="B101" s="1">
+        <v>1.2763902459780001</v>
+      </c>
+      <c r="C101" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E101" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F101" s="2" t="str">
+        <f>VLOOKUP(E101,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="4"/>
-      <c r="F102" s="2"/>
+      <c r="A102" s="1">
+        <v>1.4331634944</v>
+      </c>
+      <c r="B102" s="1">
+        <v>1.4969450181840003</v>
+      </c>
+      <c r="C102" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E102" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F102" s="2" t="str">
+        <f>VLOOKUP(E102,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="2"/>
+      <c r="A103" s="1">
+        <v>1.6866065108099999</v>
+      </c>
+      <c r="B103" s="1">
+        <v>1.272488582949</v>
+      </c>
+      <c r="C103" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D103" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E103" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F103" s="2" t="str">
+        <f>VLOOKUP(E103,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="2"/>
+      <c r="A104" s="1">
+        <v>1.230217173592</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1.0731737656259999</v>
+      </c>
+      <c r="C104" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D104" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E104" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F104" s="2" t="str">
+        <f>VLOOKUP(E104,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="2"/>
+      <c r="A105" s="1">
+        <v>1.5379492479520003</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.23004715695600003</v>
+      </c>
+      <c r="C105" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D105" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E105" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F105" s="2" t="str">
+        <f>VLOOKUP(E105,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="2"/>
+      <c r="A106" s="1">
+        <v>1.31811006828</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.71869076571599999</v>
+      </c>
+      <c r="C106" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D106" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E106" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F106" s="2" t="str">
+        <f>VLOOKUP(E106,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="2"/>
+      <c r="A107" s="1">
+        <v>1.5378575789519999</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.70427514478499997</v>
+      </c>
+      <c r="C107" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D107" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E107" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F107" s="2" t="str">
+        <f>VLOOKUP(E107,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="2"/>
+      <c r="A108" s="1">
+        <v>1.7574356473799999</v>
+      </c>
+      <c r="B108" s="1">
+        <v>1.5331625209259998</v>
+      </c>
+      <c r="C108" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D108" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E108" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F108" s="2" t="str">
+        <f>VLOOKUP(E108,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="2"/>
+      <c r="A109" s="1">
+        <v>1.3278876734799998</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.53658688281299993</v>
+      </c>
+      <c r="C109" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D109" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E109" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F109" s="2" t="str">
+        <f>VLOOKUP(E109,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="2"/>
+      <c r="A110" s="1">
+        <v>1.8568074097500002</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1.4812617872000002</v>
+      </c>
+      <c r="C110" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D110" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E110" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F110" s="2" t="str">
+        <f>VLOOKUP(E110,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="2"/>
+      <c r="A111" s="1">
+        <v>2.2429925756699998</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0.44652509032799997</v>
+      </c>
+      <c r="C111" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D111" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E111" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F111" s="2" t="str">
+        <f>VLOOKUP(E111,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="2"/>
+      <c r="A112" s="1">
+        <v>2.46611020948</v>
+      </c>
+      <c r="B112" s="1">
+        <v>0.88726605491599997</v>
+      </c>
+      <c r="C112" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D112" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E112" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F112" s="2" t="str">
+        <f>VLOOKUP(E112,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="2"/>
+      <c r="A113" s="1">
+        <v>1.854696380652</v>
+      </c>
+      <c r="B113" s="1">
+        <v>0.79601866614599992</v>
+      </c>
+      <c r="C113" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D113" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E113" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F113" s="2" t="str">
+        <f>VLOOKUP(E113,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="2"/>
+      <c r="A114" s="1">
+        <v>0.79964345825999994</v>
+      </c>
+      <c r="B114" s="1">
+        <v>1.7319236064300001</v>
+      </c>
+      <c r="C114" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D114" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E114" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F114" s="2" t="str">
+        <f>VLOOKUP(E114,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="4"/>
-      <c r="F115" s="2"/>
+      <c r="A115" s="1">
+        <v>2.4730978297409996</v>
+      </c>
+      <c r="B115" s="1">
+        <v>0.76652335999999999</v>
+      </c>
+      <c r="C115" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D115" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E115" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F115" s="2" t="str">
+        <f>VLOOKUP(E115,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="4"/>
-      <c r="F116" s="2"/>
+      <c r="A116" s="1">
+        <v>1.503025668234</v>
+      </c>
+      <c r="B116" s="1">
+        <v>0.87327723432000004</v>
+      </c>
+      <c r="C116" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D116" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E116" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F116" s="2" t="str">
+        <f>VLOOKUP(E116,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="2"/>
+      <c r="A117" s="1">
+        <v>0.48758095312500005</v>
+      </c>
+      <c r="B117" s="1">
+        <v>1.7231430775000001</v>
+      </c>
+      <c r="C117" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D117" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E117" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-2</v>
+      </c>
+      <c r="F117" s="2" t="str">
+        <f>VLOOKUP(E117,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="4"/>
-      <c r="F118" s="2"/>
+      <c r="A118" s="1">
+        <v>1.2189923812500001</v>
+      </c>
+      <c r="B118" s="1">
+        <v>0.49232564062500001</v>
+      </c>
+      <c r="C118" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D118" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E118" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-0</v>
+      </c>
+      <c r="F118" s="2" t="str">
+        <f>VLOOKUP(E118,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="4"/>
-      <c r="F119" s="2"/>
+      <c r="A119" s="1">
+        <v>1.7748458785799999</v>
+      </c>
+      <c r="B119" s="1">
+        <v>0.83811753305199987</v>
+      </c>
+      <c r="C119" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D119" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E119" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F119" s="2" t="str">
+        <f>VLOOKUP(E119,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="2"/>
+      <c r="A120" s="1">
+        <v>1.169119521372</v>
+      </c>
+      <c r="B120" s="1">
+        <v>0.92930218788499996</v>
+      </c>
+      <c r="C120" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D120" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E120" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F120" s="2" t="str">
+        <f>VLOOKUP(E120,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="2"/>
+      <c r="A121" s="1">
+        <v>1.393412922</v>
+      </c>
+      <c r="B121" s="1">
+        <v>1.7189497536300002</v>
+      </c>
+      <c r="C121" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D121" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E121" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F121" s="2" t="str">
+        <f>VLOOKUP(E121,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="2"/>
+      <c r="A122" s="1">
+        <v>1.482920701284</v>
+      </c>
+      <c r="B122" s="1">
+        <v>0.873198966252</v>
+      </c>
+      <c r="C122" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D122" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E122" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F122" s="2" t="str">
+        <f>VLOOKUP(E122,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="4"/>
+      <c r="A123" s="1">
+        <v>0.93459336164999995</v>
+      </c>
+      <c r="B123" s="1">
+        <v>0.55475783519999999</v>
+      </c>
+      <c r="C123" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D123" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E123" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F123" s="2" t="str">
+        <f>VLOOKUP(E123,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="4"/>
+      <c r="A124" s="1">
+        <v>1.5500930266800002</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0.89624342749999997</v>
+      </c>
+      <c r="C124" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D124" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E124" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F124" s="2" t="str">
+        <f>VLOOKUP(E124,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>

</xml_diff>

<commit_message>
updated fixtures for 26/10/2021
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -553,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F124"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1.028171600456</v>
+        <v>1.48682087775</v>
       </c>
       <c r="B1" s="1">
-        <v>2.2792454277119996</v>
+        <v>0.80225569060000002</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
@@ -572,27 +572,27 @@
       </c>
       <c r="D1" s="3">
         <f>ROUND(B1,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>VLOOKUP(E1,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.846070717106</v>
+        <v>0.9687647356800001</v>
       </c>
       <c r="B2" s="1">
-        <v>0.65846984070000003</v>
+        <v>0.72821966139999994</v>
       </c>
       <c r="C2" s="3">
         <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2" si="1">ROUND(B2,0)</f>
@@ -600,43 +600,43 @@
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(E2,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2.373594493248</v>
+        <v>0.73068719509500002</v>
       </c>
       <c r="B3" s="1">
-        <v>0.71839209613499999</v>
+        <v>0.73785232098899989</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
-        <v>2</v>
+        <f t="shared" ref="C3:C38" si="3">ROUND(A3,0)</f>
+        <v>1</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
+        <f t="shared" ref="D3:D38" si="4">ROUND(B3,0)</f>
         <v>1</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
-        <v>2-1</v>
+        <f t="shared" ref="E3:E38" si="5">CONCATENATE(C3,"-",D3)</f>
+        <v>1-1</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.1720964119939998</v>
+        <v>1.4999215201740002</v>
       </c>
       <c r="B4" s="1">
-        <v>0.67668433462799993</v>
+        <v>0.76826481186000006</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="3"/>
@@ -657,70 +657,70 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2.1504000000000003</v>
+        <v>1.1688722882100002</v>
       </c>
       <c r="B5" s="1">
-        <v>0.41510691334199995</v>
+        <v>1.064249740323</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-0</v>
+        <v>1-1</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>3.9822111093750006</v>
+        <v>0.75524824782</v>
       </c>
       <c r="B6" s="1">
-        <v>0.192266162928</v>
+        <v>1.3968769312680001</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>4-0</v>
+        <v>1-1</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.48766095000000004</v>
+        <v>0.80912312282999999</v>
       </c>
       <c r="B7" s="1">
-        <v>0.78766769250000013</v>
+        <v>1.5831971901199999</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-1</v>
+        <v>1-2</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -729,10 +729,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1.2800600006249998</v>
+        <v>1.4505966346079999</v>
       </c>
       <c r="B8" s="1">
-        <v>0.98462461499999998</v>
+        <v>1.835963642499</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="3"/>
@@ -740,23 +740,23 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1.5973612907219998</v>
+        <v>1.873352963808</v>
       </c>
       <c r="B9" s="1">
-        <v>0.67051402685999995</v>
+        <v>1.2592050871680001</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="3"/>
@@ -777,22 +777,22 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>0.53819084847999998</v>
+        <v>1.57612555008</v>
       </c>
       <c r="B10" s="1">
-        <v>0.17247217169699999</v>
+        <v>1.292990348844</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>2-1</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -801,14 +801,14 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.1090294416399997</v>
+        <v>0.99525171647999988</v>
       </c>
       <c r="B11" s="1">
-        <v>1.4948356808759999</v>
+        <v>0.80810078557800002</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="4"/>
@@ -816,23 +816,23 @@
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>VLOOKUP(E11,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2.9063513178</v>
+        <v>1.2714006102720004</v>
       </c>
       <c r="B12" s="1">
-        <v>0.5338934137350001</v>
+        <v>0.51846876127200003</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="4"/>
@@ -840,23 +840,23 @@
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-1</v>
+        <v>1-1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.7155712637</v>
+        <v>1.253318935232</v>
       </c>
       <c r="B13" s="1">
-        <v>0.61802941680000001</v>
+        <v>1.466605925064</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="4"/>
@@ -864,43 +864,43 @@
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>VLOOKUP(E13,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.4800474300950002</v>
+        <v>1.6049380432640001</v>
       </c>
       <c r="B14" s="1">
-        <v>1.8127529495999999</v>
+        <v>1.3852055962079999</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>2-1</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>VLOOKUP(E14,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.2809751669000002</v>
+        <v>1.1679102417959999</v>
       </c>
       <c r="B15" s="1">
-        <v>0.60988697840000006</v>
+        <v>1.1978832892950002</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
@@ -921,14 +921,14 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.2916529821200002</v>
+        <v>1.8185603337359999</v>
       </c>
       <c r="B16" s="1">
-        <v>0.72821966139999994</v>
+        <v>1.1179844039000002</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
@@ -936,19 +936,19 @@
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>VLOOKUP(E16,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>0.51670939500000002</v>
+        <v>1.479296305778</v>
       </c>
       <c r="B17" s="1">
-        <v>2.0164813669999999</v>
+        <v>1.7701322509000006</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="3"/>
@@ -969,10 +969,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.4117958693600003</v>
+        <v>1.3461931870019999</v>
       </c>
       <c r="B18" s="1">
-        <v>1.1096299591999998</v>
+        <v>1.3305401155300003</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="3"/>
@@ -993,10 +993,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.0908717108299999</v>
+        <v>1.1440164735999998</v>
       </c>
       <c r="B19" s="1">
-        <v>0.93125128751200004</v>
+        <v>2.1424397590890005</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="3"/>
@@ -1004,23 +1004,23 @@
       </c>
       <c r="D19" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F19" s="2" t="str">
         <f>VLOOKUP(E19,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.76918432519500013</v>
+        <v>1.3215743798400001</v>
       </c>
       <c r="B20" s="1">
-        <v>0.40243156778999994</v>
+        <v>0.78134358000000004</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="3"/>
@@ -1028,35 +1028,35 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>1-1</v>
       </c>
       <c r="F20" s="2" t="str">
         <f>VLOOKUP(E20,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1.4025073503209999</v>
+        <v>1.6572024471359996</v>
       </c>
       <c r="B21" s="1">
-        <v>1.3569378494</v>
+        <v>2.1817575746969999</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F21" s="2" t="str">
         <f>VLOOKUP(E21,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>0.77410948272500013</v>
+        <v>1.13487657704</v>
       </c>
       <c r="B22" s="1">
-        <v>1.0805812699919999</v>
+        <v>1.010057799321</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="3"/>
@@ -1089,14 +1089,14 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>0.31788389403000006</v>
+        <v>1.1119246247200001</v>
       </c>
       <c r="B23" s="1">
-        <v>2.1687451735679999</v>
+        <v>1.8849530429500003</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="4"/>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-2</v>
+        <v>1-2</v>
       </c>
       <c r="F23" s="2" t="str">
         <f>VLOOKUP(E23,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1113,10 +1113,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1.1191654803499997</v>
+        <v>0.63944233016400009</v>
       </c>
       <c r="B24" s="1">
-        <v>1.8636306285239999</v>
+        <v>1.4157597969900002</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="3"/>
@@ -1124,23 +1124,23 @@
       </c>
       <c r="D24" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F24" s="2" t="str">
         <f>VLOOKUP(E24,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1.438798474872</v>
+        <v>1.1990361810240002</v>
       </c>
       <c r="B25" s="1">
-        <v>0.53030836900799994</v>
+        <v>0.35570640170000006</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="3"/>
@@ -1148,59 +1148,59 @@
       </c>
       <c r="D25" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F25" s="2" t="str">
         <f>VLOOKUP(E25,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>0.42968221328799988</v>
+        <v>1.4688012959799999</v>
       </c>
       <c r="B26" s="1">
-        <v>1.567561804875</v>
+        <v>0.79864189019999998</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-2</v>
+        <v>1-1</v>
       </c>
       <c r="F26" s="2" t="str">
         <f>VLOOKUP(E26,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1.3519993487399997</v>
+        <v>1.6426236534400001</v>
       </c>
       <c r="B27" s="1">
-        <v>0.40397483095199993</v>
+        <v>1.2763902459780001</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>2-1</v>
       </c>
       <c r="F27" s="2" t="str">
         <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1209,10 +1209,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>0.80930070586199998</v>
+        <v>0.98566419336</v>
       </c>
       <c r="B28" s="1">
-        <v>1.122224530392</v>
+        <v>0.37258625216400004</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="3"/>
@@ -1220,23 +1220,23 @@
       </c>
       <c r="D28" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F28" s="2" t="str">
         <f>VLOOKUP(E28,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>2.2049410759199999</v>
+        <v>2.1384307929599999</v>
       </c>
       <c r="B29" s="1">
-        <v>0.99416580956</v>
+        <v>1.295657369208</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="3"/>
@@ -1257,14 +1257,14 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1.116180661122</v>
+        <v>1.6720240767999999</v>
       </c>
       <c r="B30" s="1">
-        <v>1.1667946057499998</v>
+        <v>0.84833693897400009</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="4"/>
@@ -1272,23 +1272,23 @@
       </c>
       <c r="E30" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F30" s="2" t="str">
         <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>1.4686613967239999</v>
+        <v>0.31429024</v>
       </c>
       <c r="B31" s="1">
-        <v>0.696118291</v>
+        <v>1.0025579399040001</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="4"/>
@@ -1296,43 +1296,43 @@
       </c>
       <c r="E31" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-1</v>
       </c>
       <c r="F31" s="2" t="str">
         <f>VLOOKUP(E31,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>1.7293495913279999</v>
+        <v>2.7343250880000003</v>
       </c>
       <c r="B32" s="1">
-        <v>2.1750187035840001</v>
+        <v>0.48993772009199998</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E32" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>3-0</v>
       </c>
       <c r="F32" s="2" t="str">
         <f>VLOOKUP(E32,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>0.74300035663999997</v>
+        <v>1.1943029119999999</v>
       </c>
       <c r="B33" s="1">
-        <v>2.4241023559260002</v>
+        <v>1.7148141642480002</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="3"/>
@@ -1353,14 +1353,14 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1.4933000000000001</v>
+        <v>1.9485994879999999</v>
       </c>
       <c r="B34" s="1">
-        <v>0.57666515579999988</v>
+        <v>1.4969450181840001</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="3">
         <f t="shared" si="4"/>
@@ -1368,19 +1368,19 @@
       </c>
       <c r="E34" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F34" s="2" t="str">
         <f>VLOOKUP(E34,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>2.56</v>
+        <v>2.5520367488</v>
       </c>
       <c r="B35" s="1">
-        <v>0.77837795833200008</v>
+        <v>1.151678718756</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="3"/>
@@ -1401,10 +1401,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>2.3039999999999998</v>
+        <v>2.05342956896</v>
       </c>
       <c r="B36" s="1">
-        <v>0.38918897916600004</v>
+        <v>1.3676257412730002</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" si="3"/>
@@ -1412,11 +1412,11 @@
       </c>
       <c r="D36" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-0</v>
+        <v>2-1</v>
       </c>
       <c r="F36" s="2" t="str">
         <f>VLOOKUP(E36,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1425,14 +1425,14 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>1.4336000000000002</v>
+        <v>1.5059039087299999</v>
       </c>
       <c r="B37" s="1">
-        <v>1.210896827442</v>
+        <v>0.82987574202299996</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" s="3">
         <f t="shared" si="4"/>
@@ -1440,19 +1440,19 @@
       </c>
       <c r="E37" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F37" s="2" t="str">
         <f>VLOOKUP(E37,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>0.63497936249999998</v>
+        <v>0.99672290409599984</v>
       </c>
       <c r="B38" s="1">
-        <v>0.71796794874999992</v>
+        <v>0.64350221422499998</v>
       </c>
       <c r="C38" s="3">
         <f t="shared" si="3"/>
@@ -1472,2068 +1472,690 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>0.10159269750000001</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1.3127794874999998</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E39" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-1</v>
-      </c>
-      <c r="F39" s="2" t="str">
-        <f>VLOOKUP(E39,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>0.91428428437500009</v>
-      </c>
-      <c r="B40" s="1">
-        <v>3.6923656412499994</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="E40" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-4</v>
-      </c>
-      <c r="F40" s="2" t="str">
-        <f>VLOOKUP(E40,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>0.73951911607500009</v>
-      </c>
-      <c r="B41" s="1">
-        <v>2.2627073396200004</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E41" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F41" s="2" t="str">
-        <f>VLOOKUP(E41,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>1.7748458785800001</v>
-      </c>
-      <c r="B42" s="1">
-        <v>2.8159229097840002</v>
-      </c>
-      <c r="C42" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E42" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-3</v>
-      </c>
-      <c r="F42" s="2" t="str">
-        <f>VLOOKUP(E42,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>0.98602548810000012</v>
-      </c>
-      <c r="B43" s="1">
-        <v>0.33520701238399997</v>
-      </c>
-      <c r="C43" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F43" s="2" t="str">
-        <f>VLOOKUP(E43,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>1.6787997481799999</v>
-      </c>
-      <c r="B44" s="1">
-        <v>1.1325463211800002</v>
-      </c>
-      <c r="C44" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E44" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F44" s="2" t="str">
-        <f>VLOOKUP(E44,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>1.678680051458</v>
-      </c>
-      <c r="B45" s="1">
-        <v>0.75509552909000011</v>
-      </c>
-      <c r="C45" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D45" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E45" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F45" s="2" t="str">
-        <f>VLOOKUP(E45,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>1.805259643808</v>
-      </c>
-      <c r="B46" s="1">
-        <v>0.26137457735400005</v>
-      </c>
-      <c r="C46" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D46" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-0</v>
-      </c>
-      <c r="F46" s="2" t="str">
-        <f>VLOOKUP(E46,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>2.7233259780440005</v>
-      </c>
-      <c r="B47" s="1">
-        <v>1.6464468283199998</v>
-      </c>
-      <c r="C47" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D47" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E47" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-2</v>
-      </c>
-      <c r="F47" s="2" t="str">
-        <f>VLOOKUP(E47,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>1.2965115266400002</v>
-      </c>
-      <c r="B48" s="1">
-        <v>1.1177587564920002</v>
-      </c>
-      <c r="C48" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D48" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E48" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F48" s="2" t="str">
-        <f>VLOOKUP(E48,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>1.6123089311999999</v>
-      </c>
-      <c r="B49" s="1">
-        <v>1.3882318760880001</v>
-      </c>
-      <c r="C49" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D49" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E49" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F49" s="2" t="str">
-        <f>VLOOKUP(E49,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>0.7414291009959999</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1.1642277894539999</v>
-      </c>
-      <c r="C50" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D50" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E50" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F50" s="2" t="str">
-        <f>VLOOKUP(E50,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>0.9226503815999999</v>
-      </c>
-      <c r="B51" s="1">
-        <v>1.207417708188</v>
-      </c>
-      <c r="C51" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D51" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E51" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F51" s="2" t="str">
-        <f>VLOOKUP(E51,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>0.82026330303600004</v>
-      </c>
-      <c r="B52" s="1">
-        <v>0.63879919791299988</v>
-      </c>
-      <c r="C52" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D52" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E52" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F52" s="2" t="str">
-        <f>VLOOKUP(E52,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>0.95684422093199994</v>
-      </c>
-      <c r="B53" s="1">
-        <v>0.51102824781300005</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E53" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F53" s="2" t="str">
-        <f>VLOOKUP(E53,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>1.3562972816400001</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1.1865764756550001</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E54" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F54" s="2" t="str">
-        <f>VLOOKUP(E54,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>0.72658782945</v>
-      </c>
-      <c r="B55" s="1">
-        <v>0.66732177109500013</v>
-      </c>
-      <c r="C55" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E55" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F55" s="2" t="str">
-        <f>VLOOKUP(E55,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>2.32508105424</v>
-      </c>
-      <c r="B56" s="1">
-        <v>1.1567590639650001</v>
-      </c>
-      <c r="C56" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E56" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F56" s="2" t="str">
-        <f>VLOOKUP(E56,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>1.2520064977200003</v>
-      </c>
-      <c r="B57" s="1">
-        <v>0.48258936080000009</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E57" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F57" s="2" t="str">
-        <f>VLOOKUP(E57,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>0.91349916761999994</v>
-      </c>
-      <c r="B58" s="1">
-        <v>0.82151119040000009</v>
-      </c>
-      <c r="C58" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D58" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E58" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F58" s="2" t="str">
-        <f>VLOOKUP(E58,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>1.5777920184000001</v>
-      </c>
-      <c r="B59" s="1">
-        <v>0.99750440640000015</v>
-      </c>
-      <c r="C59" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D59" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E59" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F59" s="2" t="str">
-        <f>VLOOKUP(E59,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>0.50477333291000004</v>
-      </c>
-      <c r="B60" s="1">
-        <v>2.3720853752959998</v>
-      </c>
-      <c r="C60" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D60" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E60" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F60" s="2" t="str">
-        <f>VLOOKUP(E60,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>1.8691604797249999</v>
-      </c>
-      <c r="B61" s="1">
-        <v>0.81399955718399986</v>
-      </c>
-      <c r="C61" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D61" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E61" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F61" s="2" t="str">
-        <f>VLOOKUP(E61,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>1.2561091726259999</v>
-      </c>
-      <c r="B62" s="1">
-        <v>0.39072445420799995</v>
-      </c>
-      <c r="C62" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D62" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E62" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-0</v>
-      </c>
-      <c r="F62" s="2" t="str">
-        <f>VLOOKUP(E62,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>2.8038240526449996</v>
-      </c>
-      <c r="B63" s="1">
-        <v>6.9746629680000005E-2</v>
-      </c>
-      <c r="C63" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D63" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E63" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-0</v>
-      </c>
-      <c r="F63" s="2" t="str">
-        <f>VLOOKUP(E63,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>1.480532169303</v>
-      </c>
-      <c r="B64" s="1">
-        <v>1.1707183490309998</v>
-      </c>
-      <c r="C64" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D64" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E64" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F64" s="2" t="str">
-        <f>VLOOKUP(E64,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>1.1514931229190002</v>
-      </c>
-      <c r="B65" s="1">
-        <v>1.0968041897759999</v>
-      </c>
-      <c r="C65" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D65" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E65" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F65" s="2" t="str">
-        <f>VLOOKUP(E65,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>1.3099478295929998</v>
-      </c>
-      <c r="B66" s="1">
-        <v>1.381139323884</v>
-      </c>
-      <c r="C66" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D66" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E66" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F66" s="2" t="str">
-        <f>VLOOKUP(E66,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>1.0791801044389999</v>
-      </c>
-      <c r="B67" s="1">
-        <v>0.94956258301200003</v>
-      </c>
-      <c r="C67" s="3">
-        <f t="shared" ref="C67:C124" si="6">ROUND(A67,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D67" s="3">
-        <f t="shared" ref="D67:D124" si="7">ROUND(B67,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E67" s="4" t="str">
-        <f t="shared" ref="E67:E124" si="8">CONCATENATE(C67,"-",D67)</f>
-        <v>1-1</v>
-      </c>
-      <c r="F67" s="2" t="str">
-        <f>VLOOKUP(E67,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>2.0773970160960005</v>
-      </c>
-      <c r="B68" s="1">
-        <v>0.78732947943000009</v>
-      </c>
-      <c r="C68" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D68" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E68" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F68" s="2" t="str">
-        <f>VLOOKUP(E68,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="4"/>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>1.1960651382159999</v>
-      </c>
-      <c r="B69" s="1">
-        <v>2.430830713158</v>
-      </c>
-      <c r="C69" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D69" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E69" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F69" s="2" t="str">
-        <f>VLOOKUP(E69,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="4"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>1.2801801120930001</v>
-      </c>
-      <c r="B70" s="1">
-        <v>1.0363143692500001</v>
-      </c>
-      <c r="C70" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D70" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E70" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F70" s="2" t="str">
-        <f>VLOOKUP(E70,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>0.71060202932399985</v>
-      </c>
-      <c r="B71" s="1">
-        <v>1.0735623703199999</v>
-      </c>
-      <c r="C71" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D71" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E71" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F71" s="2" t="str">
-        <f>VLOOKUP(E71,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>1.8939146966639997</v>
-      </c>
-      <c r="B72" s="1">
-        <v>0.42790147236499992</v>
-      </c>
-      <c r="C72" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D72" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E72" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F72" s="2" t="str">
-        <f>VLOOKUP(E72,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>2.3643019607039997</v>
-      </c>
-      <c r="B73" s="1">
-        <v>0.48488956326600002</v>
-      </c>
-      <c r="C73" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D73" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E73" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F73" s="2" t="str">
-        <f>VLOOKUP(E73,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>3.1901778939200005</v>
-      </c>
-      <c r="B74" s="1">
-        <v>1.251727786464</v>
-      </c>
-      <c r="C74" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D74" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E74" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F74" s="2" t="str">
-        <f>VLOOKUP(E74,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>1.1145378078720001</v>
-      </c>
-      <c r="B75" s="1">
-        <v>1.1334273085319999</v>
-      </c>
-      <c r="C75" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D75" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E75" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F75" s="2" t="str">
-        <f>VLOOKUP(E75,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>1.4267243221920003</v>
-      </c>
-      <c r="B76" s="1">
-        <v>1.3332290239260001</v>
-      </c>
-      <c r="C76" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D76" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E76" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F76" s="2" t="str">
-        <f>VLOOKUP(E76,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>2.1751043474079998</v>
-      </c>
-      <c r="B77" s="1">
-        <v>1.0504728374130001</v>
-      </c>
-      <c r="C77" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D77" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E77" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F77" s="2" t="str">
-        <f>VLOOKUP(E77,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>2.1646501306080004</v>
-      </c>
-      <c r="B78" s="1">
-        <v>1.3852055962080001</v>
-      </c>
-      <c r="C78" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D78" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E78" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F78" s="2" t="str">
-        <f>VLOOKUP(E78,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>1.70672</v>
-      </c>
-      <c r="B79" s="1">
-        <v>1.383863040936</v>
-      </c>
-      <c r="C79" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D79" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E79" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F79" s="2" t="str">
-        <f>VLOOKUP(E79,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="B80" s="1">
-        <v>1.2455007372419999</v>
-      </c>
-      <c r="C80" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D80" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E80" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F80" s="2" t="str">
-        <f>VLOOKUP(E80,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>1.70672</v>
-      </c>
-      <c r="B81" s="1">
-        <v>1.3837963744439998</v>
-      </c>
-      <c r="C81" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D81" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E81" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F81" s="2" t="str">
-        <f>VLOOKUP(E81,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>1.98098761875</v>
-      </c>
-      <c r="B82" s="1">
-        <v>0.16413076874999999</v>
-      </c>
-      <c r="C82" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D82" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E82" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F82" s="2" t="str">
-        <f>VLOOKUP(E82,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>1.23256519432</v>
-      </c>
-      <c r="B83" s="1">
-        <v>1.3968292210559998</v>
-      </c>
-      <c r="C83" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D83" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E83" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F83" s="2" t="str">
-        <f>VLOOKUP(E83,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>1.2941334524850001</v>
-      </c>
-      <c r="B84" s="1">
-        <v>0.29329613682</v>
-      </c>
-      <c r="C84" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D84" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E84" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F84" s="2" t="str">
-        <f>VLOOKUP(E84,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>0.88742293929000005</v>
-      </c>
-      <c r="B85" s="1">
-        <v>0.60336062347200015</v>
-      </c>
-      <c r="C85" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D85" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E85" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F85" s="2" t="str">
-        <f>VLOOKUP(E85,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>2.4044475544199999</v>
-      </c>
-      <c r="B86" s="1">
-        <v>1.1247461169400002</v>
-      </c>
-      <c r="C86" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D86" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E86" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F86" s="2" t="str">
-        <f>VLOOKUP(E86,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>2.5279996207999997</v>
-      </c>
-      <c r="B87" s="1">
-        <v>0.23962923565000002</v>
-      </c>
-      <c r="C87" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D87" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E87" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-0</v>
-      </c>
-      <c r="F87" s="2" t="str">
-        <f>VLOOKUP(E87,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>1.0191998471200001</v>
-      </c>
-      <c r="B88" s="1">
-        <v>0.39600274031999999</v>
-      </c>
-      <c r="C88" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D88" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E88" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F88" s="2" t="str">
-        <f>VLOOKUP(E88,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>1.7312372384189998</v>
-      </c>
-      <c r="B89" s="1">
-        <v>0.63895775656000009</v>
-      </c>
-      <c r="C89" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D89" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E89" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F89" s="2" t="str">
-        <f>VLOOKUP(E89,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>0.65949990107499989</v>
-      </c>
-      <c r="B90" s="1">
-        <v>1.9007404257600002</v>
-      </c>
-      <c r="C90" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D90" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E90" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F90" s="2" t="str">
-        <f>VLOOKUP(E90,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>2.475821794572</v>
-      </c>
-      <c r="B91" s="1">
-        <v>2.1952624377599999</v>
-      </c>
-      <c r="C91" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D91" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E91" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-2</v>
-      </c>
-      <c r="F91" s="2" t="str">
-        <f>VLOOKUP(E91,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>2.4758317987800003</v>
-      </c>
-      <c r="B92" s="1">
-        <v>1.1432325224339999</v>
-      </c>
-      <c r="C92" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D92" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E92" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F92" s="2" t="str">
-        <f>VLOOKUP(E92,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>3.5075158844960006</v>
-      </c>
-      <c r="B93" s="1">
-        <v>1.7247462019200002</v>
-      </c>
-      <c r="C93" s="3">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="D93" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E93" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>4-2</v>
-      </c>
-      <c r="F93" s="2" t="str">
-        <f>VLOOKUP(E93,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>2.5520367488</v>
-      </c>
-      <c r="B94" s="1">
-        <v>1.066960241376</v>
-      </c>
-      <c r="C94" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D94" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E94" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F94" s="2" t="str">
-        <f>VLOOKUP(E94,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <v>0.64536643599999999</v>
-      </c>
-      <c r="B95" s="1">
-        <v>0.55044581529600001</v>
-      </c>
-      <c r="C95" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D95" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E95" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F95" s="2" t="str">
-        <f>VLOOKUP(E95,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>1.1314448639999999</v>
-      </c>
-      <c r="B96" s="1">
-        <v>1.4289118027140002</v>
-      </c>
-      <c r="C96" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D96" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E96" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F96" s="2" t="str">
-        <f>VLOOKUP(E96,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>1.8755270072000001</v>
-      </c>
-      <c r="B97" s="1">
-        <v>1.5719022692520002</v>
-      </c>
-      <c r="C97" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D97" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E97" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-2</v>
-      </c>
-      <c r="F97" s="2" t="str">
-        <f>VLOOKUP(E97,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>1.8949201436000001</v>
-      </c>
-      <c r="B98" s="1">
-        <v>2.4937552012320001</v>
-      </c>
-      <c r="C98" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D98" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E98" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-2</v>
-      </c>
-      <c r="F98" s="2" t="str">
-        <f>VLOOKUP(E98,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>1.1314448640000001</v>
-      </c>
-      <c r="B99" s="1">
-        <v>0.58972357843199996</v>
-      </c>
-      <c r="C99" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D99" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E99" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F99" s="2" t="str">
-        <f>VLOOKUP(E99,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>1.82162623104</v>
-      </c>
-      <c r="B100" s="1">
-        <v>0.83835835314000007</v>
-      </c>
-      <c r="C100" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D100" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E100" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F100" s="2" t="str">
-        <f>VLOOKUP(E100,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>2.1025902768639999</v>
-      </c>
-      <c r="B101" s="1">
-        <v>1.2763902459780001</v>
-      </c>
-      <c r="C101" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D101" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E101" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F101" s="2" t="str">
-        <f>VLOOKUP(E101,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>1.4331634944</v>
-      </c>
-      <c r="B102" s="1">
-        <v>1.4969450181840003</v>
-      </c>
-      <c r="C102" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D102" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E102" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F102" s="2" t="str">
-        <f>VLOOKUP(E102,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>1.6866065108099999</v>
-      </c>
-      <c r="B103" s="1">
-        <v>1.272488582949</v>
-      </c>
-      <c r="C103" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D103" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E103" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F103" s="2" t="str">
-        <f>VLOOKUP(E103,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>1.230217173592</v>
-      </c>
-      <c r="B104" s="1">
-        <v>1.0731737656259999</v>
-      </c>
-      <c r="C104" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D104" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E104" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F104" s="2" t="str">
-        <f>VLOOKUP(E104,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>1.5379492479520003</v>
-      </c>
-      <c r="B105" s="1">
-        <v>0.23004715695600003</v>
-      </c>
-      <c r="C105" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D105" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E105" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F105" s="2" t="str">
-        <f>VLOOKUP(E105,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>1.31811006828</v>
-      </c>
-      <c r="B106" s="1">
-        <v>0.71869076571599999</v>
-      </c>
-      <c r="C106" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D106" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E106" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F106" s="2" t="str">
-        <f>VLOOKUP(E106,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>1.5378575789519999</v>
-      </c>
-      <c r="B107" s="1">
-        <v>0.70427514478499997</v>
-      </c>
-      <c r="C107" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D107" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E107" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F107" s="2" t="str">
-        <f>VLOOKUP(E107,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="2"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <v>1.7574356473799999</v>
-      </c>
-      <c r="B108" s="1">
-        <v>1.5331625209259998</v>
-      </c>
-      <c r="C108" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D108" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E108" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-2</v>
-      </c>
-      <c r="F108" s="2" t="str">
-        <f>VLOOKUP(E108,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="2"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <v>1.3278876734799998</v>
-      </c>
-      <c r="B109" s="1">
-        <v>0.53658688281299993</v>
-      </c>
-      <c r="C109" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D109" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E109" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F109" s="2" t="str">
-        <f>VLOOKUP(E109,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>1.8568074097500002</v>
-      </c>
-      <c r="B110" s="1">
-        <v>1.4812617872000002</v>
-      </c>
-      <c r="C110" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D110" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E110" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F110" s="2" t="str">
-        <f>VLOOKUP(E110,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>2.2429925756699998</v>
-      </c>
-      <c r="B111" s="1">
-        <v>0.44652509032799997</v>
-      </c>
-      <c r="C111" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D111" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E111" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F111" s="2" t="str">
-        <f>VLOOKUP(E111,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>2.46611020948</v>
-      </c>
-      <c r="B112" s="1">
-        <v>0.88726605491599997</v>
-      </c>
-      <c r="C112" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D112" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E112" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F112" s="2" t="str">
-        <f>VLOOKUP(E112,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>1.854696380652</v>
-      </c>
-      <c r="B113" s="1">
-        <v>0.79601866614599992</v>
-      </c>
-      <c r="C113" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D113" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E113" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F113" s="2" t="str">
-        <f>VLOOKUP(E113,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <v>0.79964345825999994</v>
-      </c>
-      <c r="B114" s="1">
-        <v>1.7319236064300001</v>
-      </c>
-      <c r="C114" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D114" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E114" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F114" s="2" t="str">
-        <f>VLOOKUP(E114,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="2"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <v>2.4730978297409996</v>
-      </c>
-      <c r="B115" s="1">
-        <v>0.76652335999999999</v>
-      </c>
-      <c r="C115" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D115" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E115" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F115" s="2" t="str">
-        <f>VLOOKUP(E115,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>1.503025668234</v>
-      </c>
-      <c r="B116" s="1">
-        <v>0.87327723432000004</v>
-      </c>
-      <c r="C116" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D116" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E116" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F116" s="2" t="str">
-        <f>VLOOKUP(E116,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>0.48758095312500005</v>
-      </c>
-      <c r="B117" s="1">
-        <v>1.7231430775000001</v>
-      </c>
-      <c r="C117" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D117" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E117" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-2</v>
-      </c>
-      <c r="F117" s="2" t="str">
-        <f>VLOOKUP(E117,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>1.2189923812500001</v>
-      </c>
-      <c r="B118" s="1">
-        <v>0.49232564062500001</v>
-      </c>
-      <c r="C118" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D118" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E118" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F118" s="2" t="str">
-        <f>VLOOKUP(E118,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="2"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>1.7748458785799999</v>
-      </c>
-      <c r="B119" s="1">
-        <v>0.83811753305199987</v>
-      </c>
-      <c r="C119" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D119" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E119" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F119" s="2" t="str">
-        <f>VLOOKUP(E119,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="2"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>1.169119521372</v>
-      </c>
-      <c r="B120" s="1">
-        <v>0.92930218788499996</v>
-      </c>
-      <c r="C120" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D120" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E120" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F120" s="2" t="str">
-        <f>VLOOKUP(E120,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="2"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>1.393412922</v>
-      </c>
-      <c r="B121" s="1">
-        <v>1.7189497536300002</v>
-      </c>
-      <c r="C121" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D121" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E121" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F121" s="2" t="str">
-        <f>VLOOKUP(E121,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>1.482920701284</v>
-      </c>
-      <c r="B122" s="1">
-        <v>0.873198966252</v>
-      </c>
-      <c r="C122" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D122" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E122" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F122" s="2" t="str">
-        <f>VLOOKUP(E122,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="2"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
-        <v>0.93459336164999995</v>
-      </c>
-      <c r="B123" s="1">
-        <v>0.55475783519999999</v>
-      </c>
-      <c r="C123" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D123" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E123" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F123" s="2" t="str">
-        <f>VLOOKUP(E123,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>1.5500930266800002</v>
-      </c>
-      <c r="B124" s="1">
-        <v>0.89624342749999997</v>
-      </c>
-      <c r="C124" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D124" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E124" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F124" s="2" t="str">
-        <f>VLOOKUP(E124,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="2"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>

</xml_diff>

<commit_message>
updated odds for fixtures 29/10/2021
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -553,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F38"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1.48682087775</v>
+        <v>1.2466857032279999</v>
       </c>
       <c r="B1" s="1">
-        <v>0.80225569060000002</v>
+        <v>0.77122205631999996</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
@@ -585,10 +585,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.9687647356800001</v>
+        <v>0.92895543587000007</v>
       </c>
       <c r="B2" s="1">
-        <v>0.72821966139999994</v>
+        <v>1.9954619178780002</v>
       </c>
       <c r="C2" s="3">
         <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
@@ -596,47 +596,47 @@
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2" si="1">ROUND(B2,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(E2,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.73068719509500002</v>
+        <v>1.98307226052</v>
       </c>
       <c r="B3" s="1">
-        <v>0.73785232098899989</v>
+        <v>0.36493978900399998</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C38" si="3">ROUND(A3,0)</f>
-        <v>1</v>
+        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
+        <v>2</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D38" si="4">ROUND(B3,0)</f>
-        <v>1</v>
+        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
+        <v>0</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3:E38" si="5">CONCATENATE(C3,"-",D3)</f>
-        <v>1-1</v>
+        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
+        <v>2-0</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.4999215201740002</v>
+        <v>0.93286148792399992</v>
       </c>
       <c r="B4" s="1">
-        <v>0.76826481186000006</v>
+        <v>2.6489385264900003</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="3"/>
@@ -644,35 +644,35 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-3</v>
       </c>
       <c r="F4" s="2" t="str">
         <f>VLOOKUP(E4,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1.1688722882100002</v>
+        <v>0.44591448283200003</v>
       </c>
       <c r="B5" s="1">
-        <v>1.064249740323</v>
+        <v>0.19552982910000002</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-0</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -681,10 +681,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.75524824782</v>
+        <v>0.95544735897600008</v>
       </c>
       <c r="B6" s="1">
-        <v>1.3968769312680001</v>
+        <v>0.73318686349999995</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="3"/>
@@ -705,10 +705,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.80912312282999999</v>
+        <v>1.4706117648000001</v>
       </c>
       <c r="B7" s="1">
-        <v>1.5831971901199999</v>
+        <v>1.3437224155</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="3"/>
@@ -716,23 +716,23 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1.4505966346079999</v>
+        <v>0.57187957499999997</v>
       </c>
       <c r="B8" s="1">
-        <v>1.835963642499</v>
+        <v>0.56850788050000001</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="3"/>
@@ -740,27 +740,27 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1.873352963808</v>
+        <v>1.0349082791999999</v>
       </c>
       <c r="B9" s="1">
-        <v>1.2592050871680001</v>
+        <v>0.77525620200000001</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="4"/>
@@ -768,19 +768,19 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>VLOOKUP(E9,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1.57612555008</v>
+        <v>1.8007682379959997</v>
       </c>
       <c r="B10" s="1">
-        <v>1.292990348844</v>
+        <v>1.6388274258000002</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="3"/>
@@ -788,27 +788,27 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>2-2</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0.99525171647999988</v>
+        <v>1.9908924147200002</v>
       </c>
       <c r="B11" s="1">
-        <v>0.80810078557800002</v>
+        <v>1.1377013652399999</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="4"/>
@@ -816,23 +816,23 @@
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>VLOOKUP(E11,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.2714006102720004</v>
+        <v>1.9801434777600002</v>
       </c>
       <c r="B12" s="1">
-        <v>0.51846876127200003</v>
+        <v>0.957904065759</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="4"/>
@@ -840,31 +840,31 @@
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.253318935232</v>
+        <v>0.42623656459999998</v>
       </c>
       <c r="B13" s="1">
-        <v>1.466605925064</v>
+        <v>0.38561102815999998</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-0</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>VLOOKUP(E13,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -873,34 +873,34 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.6049380432640001</v>
+        <v>0.5893787801999999</v>
       </c>
       <c r="B14" s="1">
-        <v>1.3852055962079999</v>
+        <v>1.9887362860800002</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>VLOOKUP(E14,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.1679102417959999</v>
+        <v>1.39725896184</v>
       </c>
       <c r="B15" s="1">
-        <v>1.1978832892950002</v>
+        <v>1.22131007691</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
@@ -921,10 +921,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.8185603337359999</v>
+        <v>1.5187307543999999</v>
       </c>
       <c r="B16" s="1">
-        <v>1.1179844039000002</v>
+        <v>1.0713103746600001</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="3"/>
@@ -945,34 +945,34 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1.479296305778</v>
+        <v>1.9220068940199999</v>
       </c>
       <c r="B17" s="1">
-        <v>1.7701322509000006</v>
+        <v>0.76330395472800006</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>2-1</v>
       </c>
       <c r="F17" s="2" t="str">
         <f>VLOOKUP(E17,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.3461931870019999</v>
+        <v>1.38859192944</v>
       </c>
       <c r="B18" s="1">
-        <v>1.3305401155300003</v>
+        <v>1.0285679584830001</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="3"/>
@@ -993,10 +993,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.1440164735999998</v>
+        <v>1.4411644744200001</v>
       </c>
       <c r="B19" s="1">
-        <v>2.1424397590890005</v>
+        <v>1.12897326528</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="3"/>
@@ -1004,23 +1004,23 @@
       </c>
       <c r="D19" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F19" s="2" t="str">
         <f>VLOOKUP(E19,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1.3215743798400001</v>
+        <v>0.92655216195000012</v>
       </c>
       <c r="B20" s="1">
-        <v>0.78134358000000004</v>
+        <v>2.0321572109000003</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="3"/>
@@ -1028,59 +1028,59 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F20" s="2" t="str">
         <f>VLOOKUP(E20,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1.6572024471359996</v>
+        <v>0.52021689609599997</v>
       </c>
       <c r="B21" s="1">
-        <v>2.1817575746969999</v>
+        <v>0.22813242080000001</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>1-0</v>
       </c>
       <c r="F21" s="2" t="str">
         <f>VLOOKUP(E21,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.13487657704</v>
+        <v>1.9152835436800004</v>
       </c>
       <c r="B22" s="1">
-        <v>1.010057799321</v>
+        <v>1.637489765625</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F22" s="2" t="str">
         <f>VLOOKUP(E22,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1089,14 +1089,14 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1.1119246247200001</v>
+        <v>1.8460168117159999</v>
       </c>
       <c r="B23" s="1">
-        <v>1.8849530429500003</v>
+        <v>1.62675277632</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="4"/>
@@ -1104,19 +1104,19 @@
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>2-2</v>
       </c>
       <c r="F23" s="2" t="str">
         <f>VLOOKUP(E23,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>0.63944233016400009</v>
+        <v>0.58600652849199997</v>
       </c>
       <c r="B24" s="1">
-        <v>1.4157597969900002</v>
+        <v>0.67478041152000001</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="3"/>
@@ -1137,10 +1137,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1.1990361810240002</v>
+        <v>1.0868657409119999</v>
       </c>
       <c r="B25" s="1">
-        <v>0.35570640170000006</v>
+        <v>0.77122205631999996</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="3"/>
@@ -1148,23 +1148,23 @@
       </c>
       <c r="D25" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>1-1</v>
       </c>
       <c r="F25" s="2" t="str">
         <f>VLOOKUP(E25,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1.4688012959799999</v>
+        <v>0.50345913046799995</v>
       </c>
       <c r="B26" s="1">
-        <v>0.79864189019999998</v>
+        <v>1.208509562385</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="3"/>
@@ -1185,14 +1185,14 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1.6426236534400001</v>
+        <v>0.83909855077999995</v>
       </c>
       <c r="B27" s="1">
-        <v>1.2763902459780001</v>
+        <v>0.55776595164999998</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" si="4"/>
@@ -1200,31 +1200,31 @@
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F27" s="2" t="str">
         <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>0.98566419336</v>
+        <v>2.1600432000000001</v>
       </c>
       <c r="B28" s="1">
-        <v>0.37258625216400004</v>
+        <v>1.2378935636279997</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>2-1</v>
       </c>
       <c r="F28" s="2" t="str">
         <f>VLOOKUP(E28,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1233,62 +1233,62 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>2.1384307929599999</v>
+        <v>0.7500150000000001</v>
       </c>
       <c r="B29" s="1">
-        <v>1.295657369208</v>
+        <v>2.5263324440640003</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-3</v>
       </c>
       <c r="F29" s="2" t="str">
         <f>VLOOKUP(E29,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1.6720240767999999</v>
+        <v>0.54001080000000001</v>
       </c>
       <c r="B30" s="1">
-        <v>0.84833693897400009</v>
+        <v>1.6673920798499997</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F30" s="2" t="str">
         <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>0.31429024</v>
+        <v>1.8646226395499998</v>
       </c>
       <c r="B31" s="1">
-        <v>1.0025579399040001</v>
+        <v>0.95344784799000004</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="4"/>
@@ -1296,43 +1296,43 @@
       </c>
       <c r="E31" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-1</v>
+        <v>2-1</v>
       </c>
       <c r="F31" s="2" t="str">
         <f>VLOOKUP(E31,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>2.7343250880000003</v>
+        <v>1.189057243902</v>
       </c>
       <c r="B32" s="1">
-        <v>0.48993772009199998</v>
+        <v>1.12690135228</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-0</v>
+        <v>1-1</v>
       </c>
       <c r="F32" s="2" t="str">
         <f>VLOOKUP(E32,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>1.1943029119999999</v>
+        <v>1.229541016088</v>
       </c>
       <c r="B33" s="1">
-        <v>1.7148141642480002</v>
+        <v>0.91560109871999995</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="3"/>
@@ -1340,51 +1340,51 @@
       </c>
       <c r="D33" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F33" s="2" t="str">
         <f>VLOOKUP(E33,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1.9485994879999999</v>
+        <v>1.3467790774619999</v>
       </c>
       <c r="B34" s="1">
-        <v>1.4969450181840001</v>
+        <v>1.50383137905</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F34" s="2" t="str">
         <f>VLOOKUP(E34,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>2.5520367488</v>
+        <v>0.81364254191999996</v>
       </c>
       <c r="B35" s="1">
-        <v>1.151678718756</v>
+        <v>1.2861456779849998</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="3">
         <f t="shared" si="4"/>
@@ -1392,23 +1392,23 @@
       </c>
       <c r="E35" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-1</v>
+        <v>1-1</v>
       </c>
       <c r="F35" s="2" t="str">
         <f>VLOOKUP(E35,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>2.05342956896</v>
+        <v>1.4141568552479999</v>
       </c>
       <c r="B36" s="1">
-        <v>1.3676257412730002</v>
+        <v>0.70847516707500002</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" s="3">
         <f t="shared" si="4"/>
@@ -1416,19 +1416,19 @@
       </c>
       <c r="E36" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F36" s="2" t="str">
         <f>VLOOKUP(E36,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>1.5059039087299999</v>
+        <v>1.7399758616940002</v>
       </c>
       <c r="B37" s="1">
-        <v>0.82987574202299996</v>
+        <v>0.87742645425600008</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" si="3"/>
@@ -1449,609 +1449,1779 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>0.99672290409599984</v>
+        <v>2.5309535238540004</v>
       </c>
       <c r="B38" s="1">
-        <v>0.64350221422499998</v>
+        <v>1.5953738548</v>
       </c>
       <c r="C38" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D38" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>3-2</v>
       </c>
       <c r="F38" s="2" t="str">
         <f>VLOOKUP(E38,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1.09819515824</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3.1048364814000005</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E39" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-3</v>
+      </c>
+      <c r="F39" s="2" t="str">
+        <f>VLOOKUP(E39,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>0.20591159216999999</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.41113325024</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-1</v>
+      </c>
+      <c r="F40" s="2" t="str">
+        <f>VLOOKUP(E40,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>1.5853625874600001</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.98785327232999998</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F41" s="2" t="str">
+        <f>VLOOKUP(E41,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>0.47646111174</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.58064682251999999</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-1</v>
+      </c>
+      <c r="F42" s="2" t="str">
+        <f>VLOOKUP(E42,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>3.2485381632000001</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.36662914469999996</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-0</v>
+      </c>
+      <c r="F43" s="2" t="str">
+        <f>VLOOKUP(E43,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2.6009178084000002</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.7983468065999999</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F44" s="2" t="str">
+        <f>VLOOKUP(E44,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>1.0623354060800001</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1.4436481200000002</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F45" s="2" t="str">
+        <f>VLOOKUP(E45,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
         <v>X</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="2"/>
-    </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="2"/>
+      <c r="A46" s="1">
+        <v>2.0656021848160004</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1.637489765625</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E46" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-2</v>
+      </c>
+      <c r="F46" s="2" t="str">
+        <f>VLOOKUP(E46,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="2"/>
+      <c r="A47" s="1">
+        <v>1.9123608811520003</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.67369578937499985</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E47" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F47" s="2" t="str">
+        <f>VLOOKUP(E47,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="2"/>
+      <c r="A48" s="1">
+        <v>0.56336574528000005</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1.8245885962499999</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E48" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F48" s="2" t="str">
+        <f>VLOOKUP(E48,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="2"/>
+      <c r="A49" s="1">
+        <v>0.70810566480000003</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1.7636424414999998</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E49" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F49" s="2" t="str">
+        <f>VLOOKUP(E49,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="2"/>
+      <c r="A50" s="1">
+        <v>1.4161113288</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.50388236350000004</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F50" s="2" t="str">
+        <f>VLOOKUP(E50,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="2"/>
+      <c r="A51" s="1">
+        <v>2.0060854946999997</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.4470549092499998</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F51" s="2" t="str">
+        <f>VLOOKUP(E51,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="2"/>
+      <c r="A52" s="1">
+        <v>0.9781052466900001</v>
+      </c>
+      <c r="B52" s="1">
+        <v>4.0304469490899999</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E52" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-4</v>
+      </c>
+      <c r="F52" s="2" t="str">
+        <f>VLOOKUP(E52,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="2"/>
+      <c r="A53" s="1">
+        <v>0.85596709224000012</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1.2645143385349999</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F53" s="2" t="str">
+        <f>VLOOKUP(E53,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="2"/>
+      <c r="A54" s="1">
+        <v>1.301119197312</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1.751433145245</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E54" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F54" s="2" t="str">
+        <f>VLOOKUP(E54,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="2"/>
+      <c r="A55" s="1">
+        <v>1.77139646208</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.86851852032999988</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F55" s="2" t="str">
+        <f>VLOOKUP(E55,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="2"/>
+      <c r="A56" s="1">
+        <v>0.90834476927999996</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.68236187148999994</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E56" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F56" s="2" t="str">
+        <f>VLOOKUP(E56,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="2"/>
+      <c r="A57" s="1">
+        <v>2.1573782000640001</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.62258951565499998</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F57" s="2" t="str">
+        <f>VLOOKUP(E57,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="2"/>
+      <c r="A58" s="1">
+        <v>1.294609192632</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.65071861002000009</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E58" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F58" s="2" t="str">
+        <f>VLOOKUP(E58,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="2"/>
+      <c r="A59" s="1">
+        <v>1.43845465848</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1.6732978549499999</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E59" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F59" s="2" t="str">
+        <f>VLOOKUP(E59,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="2"/>
+      <c r="A60" s="1">
+        <v>1.5628248127659998</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1.32213781206</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E60" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F60" s="2" t="str">
+        <f>VLOOKUP(E60,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="2"/>
+      <c r="A61" s="1">
+        <v>1.1508387244199998</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1.7351718511999998</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E61" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F61" s="2" t="str">
+        <f>VLOOKUP(E61,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="2"/>
+      <c r="A62" s="1">
+        <v>0.86307279508800006</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1.5803701972949999</v>
+      </c>
+      <c r="C62" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E62" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F62" s="2" t="str">
+        <f>VLOOKUP(E62,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="2"/>
+      <c r="A63" s="1">
+        <v>2.2400447999999997</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1.2378935636279997</v>
+      </c>
+      <c r="C63" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F63" s="2" t="str">
+        <f>VLOOKUP(E63,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="2"/>
+      <c r="A64" s="1">
+        <v>1.3500270000000003</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1.7053794002339999</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D64" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E64" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F64" s="2" t="str">
+        <f>VLOOKUP(E64,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="2"/>
+      <c r="A65" s="1">
+        <v>1.4400287999999999</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0.9094656789179999</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D65" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F65" s="2" t="str">
+        <f>VLOOKUP(E65,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="2"/>
+      <c r="A66" s="1">
+        <v>0.8899287366419999</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.71844229214999999</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D66" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E66" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F66" s="2" t="str">
+        <f>VLOOKUP(E66,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="2"/>
+      <c r="A67" s="1">
+        <v>1.194495558102</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.85459197885600002</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" ref="C67:C111" si="6">ROUND(A67,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D67" s="3">
+        <f t="shared" ref="D67:D111" si="7">ROUND(B67,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E67" s="4" t="str">
+        <f t="shared" ref="E67:E111" si="8">CONCATENATE(C67,"-",D67)</f>
+        <v>1-1</v>
+      </c>
+      <c r="F67" s="2" t="str">
+        <f>VLOOKUP(E67,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="4"/>
+      <c r="A68" s="1">
+        <v>0.87315871034699988</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1.2135014561999999</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F68" s="2" t="str">
+        <f>VLOOKUP(E68,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="4"/>
+      <c r="A69" s="1">
+        <v>0.70256629627799994</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.70430084516000002</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E69" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F69" s="2" t="str">
+        <f>VLOOKUP(E69,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="2"/>
+      <c r="A70" s="1">
+        <v>0.32788427063699999</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0.72310086772000004</v>
+      </c>
+      <c r="C70" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-1</v>
+      </c>
+      <c r="F70" s="2" t="str">
+        <f>VLOOKUP(E70,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="2"/>
+      <c r="A71" s="1">
+        <v>1.2591554046799998</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1.720373290008</v>
+      </c>
+      <c r="C71" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E71" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F71" s="2" t="str">
+        <f>VLOOKUP(E71,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="2"/>
+      <c r="A72" s="1">
+        <v>0.50368502027999995</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1.0948193670120001</v>
+      </c>
+      <c r="C72" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E72" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F72" s="2" t="str">
+        <f>VLOOKUP(E72,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="2"/>
+      <c r="A73" s="1">
+        <v>2.9745333937200003</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.54740968350600006</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E73" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F73" s="2" t="str">
+        <f>VLOOKUP(E73,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="2"/>
+      <c r="A74" s="1">
+        <v>1.4138890211840001</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1.642162382672</v>
+      </c>
+      <c r="C74" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D74" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E74" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F74" s="2" t="str">
+        <f>VLOOKUP(E74,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="2"/>
+      <c r="A75" s="1">
+        <v>0.73456009972799985</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1.1175114381389999</v>
+      </c>
+      <c r="C75" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E75" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F75" s="2" t="str">
+        <f>VLOOKUP(E75,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="2"/>
+      <c r="A76" s="1">
+        <v>1.3675629098250002</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1.142775509796</v>
+      </c>
+      <c r="C76" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E76" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F76" s="2" t="str">
+        <f>VLOOKUP(E76,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="2"/>
+      <c r="A77" s="1">
+        <v>0.92310543</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.92308021796700002</v>
+      </c>
+      <c r="C77" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E77" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F77" s="2" t="str">
+        <f>VLOOKUP(E77,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="2"/>
+      <c r="A78" s="1">
+        <v>1.4118589850040002</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1.0549107261120001</v>
+      </c>
+      <c r="C78" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E78" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F78" s="2" t="str">
+        <f>VLOOKUP(E78,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="2"/>
+      <c r="A79" s="1">
+        <v>1.509865215354</v>
+      </c>
+      <c r="B79" s="1">
+        <v>1.2088074280350001</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E79" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F79" s="2" t="str">
+        <f>VLOOKUP(E79,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="2"/>
+      <c r="A80" s="1">
+        <v>1.7376536614320002</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.73035121324800001</v>
+      </c>
+      <c r="C80" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D80" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E80" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F80" s="2" t="str">
+        <f>VLOOKUP(E80,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="2"/>
+      <c r="A81" s="1">
+        <v>0.58832586072000015</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0.59341036076400011</v>
+      </c>
+      <c r="C81" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E81" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F81" s="2" t="str">
+        <f>VLOOKUP(E81,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="2"/>
+      <c r="A82" s="1">
+        <v>0.93686139783000011</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.74222279332500007</v>
+      </c>
+      <c r="C82" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D82" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E82" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F82" s="2" t="str">
+        <f>VLOOKUP(E82,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="2"/>
+      <c r="A83" s="1">
+        <v>1.3179611031839999</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1.491604296245</v>
+      </c>
+      <c r="C83" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E83" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F83" s="2" t="str">
+        <f>VLOOKUP(E83,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="2"/>
+      <c r="A84" s="1">
+        <v>1.6217681383079998</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1.4329147793400001</v>
+      </c>
+      <c r="C84" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E84" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F84" s="2" t="str">
+        <f>VLOOKUP(E84,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="2"/>
+      <c r="A85" s="1">
+        <v>1.495995181326</v>
+      </c>
+      <c r="B85" s="1">
+        <v>1.0984610212500001</v>
+      </c>
+      <c r="C85" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E85" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F85" s="2" t="str">
+        <f>VLOOKUP(E85,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="2"/>
+      <c r="A86" s="1">
+        <v>3.217069320192</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.95717582901600007</v>
+      </c>
+      <c r="C86" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E86" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F86" s="2" t="str">
+        <f>VLOOKUP(E86,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="2"/>
+      <c r="A87" s="1">
+        <v>2.2597659448140002</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1.243107332808</v>
+      </c>
+      <c r="C87" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D87" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E87" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F87" s="2" t="str">
+        <f>VLOOKUP(E87,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="2"/>
+      <c r="A88" s="1">
+        <v>1.0358215430639999</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1.8346507671360002</v>
+      </c>
+      <c r="C88" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D88" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E88" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F88" s="2" t="str">
+        <f>VLOOKUP(E88,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="2"/>
+      <c r="A89" s="1">
+        <v>1.4687716147020002</v>
+      </c>
+      <c r="B89" s="1">
+        <v>1.196442893448</v>
+      </c>
+      <c r="C89" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D89" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E89" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F89" s="2" t="str">
+        <f>VLOOKUP(E89,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="2"/>
+      <c r="A90" s="1">
+        <v>2.8398273423660001</v>
+      </c>
+      <c r="B90" s="1">
+        <v>1.2307312597800002</v>
+      </c>
+      <c r="C90" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E90" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F90" s="2" t="str">
+        <f>VLOOKUP(E90,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="2"/>
+      <c r="A91" s="1">
+        <v>2.2522320305100005</v>
+      </c>
+      <c r="B91" s="1">
+        <v>1.0370221715040002</v>
+      </c>
+      <c r="C91" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E91" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F91" s="2" t="str">
+        <f>VLOOKUP(E91,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="2"/>
+      <c r="A92" s="1">
+        <v>2.2647441726800004</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.19752398607000002</v>
+      </c>
+      <c r="C92" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E92" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F92" s="2" t="str">
+        <f>VLOOKUP(E92,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="2"/>
+      <c r="A93" s="1">
+        <v>0.88244967911999994</v>
+      </c>
+      <c r="B93" s="1">
+        <v>4.2338497471499998</v>
+      </c>
+      <c r="C93" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="E93" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-4</v>
+      </c>
+      <c r="F93" s="2" t="str">
+        <f>VLOOKUP(E93,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="2"/>
+      <c r="A94" s="1">
+        <v>0.92655216195000012</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.70560829080000009</v>
+      </c>
+      <c r="C94" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E94" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F94" s="2" t="str">
+        <f>VLOOKUP(E94,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="2"/>
+      <c r="A95" s="1">
+        <v>2.0063794544640001</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.85539657839999994</v>
+      </c>
+      <c r="C95" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E95" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F95" s="2" t="str">
+        <f>VLOOKUP(E95,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="2"/>
+      <c r="A96" s="1">
+        <v>2.3408760291840003</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0.25663230679999999</v>
+      </c>
+      <c r="C96" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E96" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F96" s="2" t="str">
+        <f>VLOOKUP(E96,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="2"/>
+      <c r="A97" s="1">
+        <v>1.0589462991359999</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1.283161534</v>
+      </c>
+      <c r="C97" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E97" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F97" s="2" t="str">
+        <f>VLOOKUP(E97,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="2"/>
+      <c r="A98" s="1">
+        <v>1.5935221612160002</v>
+      </c>
+      <c r="B98" s="1">
+        <v>1.3232917293749997</v>
+      </c>
+      <c r="C98" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E98" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F98" s="2" t="str">
+        <f>VLOOKUP(E98,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="2"/>
+      <c r="A99" s="1">
+        <v>1.126745779632</v>
+      </c>
+      <c r="B99" s="1">
+        <v>1.1227929824999998</v>
+      </c>
+      <c r="C99" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E99" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F99" s="2" t="str">
+        <f>VLOOKUP(E99,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="2"/>
+      <c r="A100" s="1">
+        <v>1.0816342326400004</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.16839894749999998</v>
+      </c>
+      <c r="C100" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D100" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E100" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-0</v>
+      </c>
+      <c r="F100" s="2" t="str">
+        <f>VLOOKUP(E100,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="2"/>
+      <c r="A101" s="1">
+        <v>1.3571664110999999</v>
+      </c>
+      <c r="B101" s="1">
+        <v>1.4728484485000002</v>
+      </c>
+      <c r="C101" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E101" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F101" s="2" t="str">
+        <f>VLOOKUP(E101,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="4"/>
-      <c r="F102" s="2"/>
+      <c r="A102" s="1">
+        <v>0.49928454809999995</v>
+      </c>
+      <c r="B102" s="1">
+        <v>1.5116470905000001</v>
+      </c>
+      <c r="C102" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E102" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-2</v>
+      </c>
+      <c r="F102" s="2" t="str">
+        <f>VLOOKUP(E102,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="2"/>
+      <c r="A103" s="1">
+        <v>0.85582709107999999</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.63219716574000007</v>
+      </c>
+      <c r="C103" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D103" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E103" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F103" s="2" t="str">
+        <f>VLOOKUP(E103,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="2"/>
+      <c r="A104" s="1">
+        <v>1.4672378721000003</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1.896711504275</v>
+      </c>
+      <c r="C104" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D104" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E104" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F104" s="2" t="str">
+        <f>VLOOKUP(E104,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="2"/>
+      <c r="A105" s="1">
+        <v>1.3448197153300001</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.92193753450000004</v>
+      </c>
+      <c r="C105" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D105" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E105" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F105" s="2" t="str">
+        <f>VLOOKUP(E105,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="2"/>
+      <c r="A106" s="1">
+        <v>1.6133713052159999</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.47890828098099991</v>
+      </c>
+      <c r="C106" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D106" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E106" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F106" s="2" t="str">
+        <f>VLOOKUP(E106,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="2"/>
+      <c r="A107" s="1">
+        <v>1.5089801955840003</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.51089050199099995</v>
+      </c>
+      <c r="C107" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D107" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E107" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F107" s="2" t="str">
+        <f>VLOOKUP(E107,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="2"/>
+      <c r="A108" s="1">
+        <v>0.99917924620799992</v>
+      </c>
+      <c r="B108" s="1">
+        <v>1.1384215442200001</v>
+      </c>
+      <c r="C108" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D108" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E108" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F108" s="2" t="str">
+        <f>VLOOKUP(E108,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="2"/>
+      <c r="A109" s="1">
+        <v>1.0433371557120001</v>
+      </c>
+      <c r="B109" s="1">
+        <v>1.3648686044140002</v>
+      </c>
+      <c r="C109" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D109" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E109" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F109" s="2" t="str">
+        <f>VLOOKUP(E109,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="2"/>
+      <c r="A110" s="1">
+        <v>0.92729413862400023</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1.1049332142050001</v>
+      </c>
+      <c r="C110" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D110" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E110" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F110" s="2" t="str">
+        <f>VLOOKUP(E110,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="2"/>
+      <c r="A111" s="1">
+        <v>2.3397315102720002</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0.68414575908899999</v>
+      </c>
+      <c r="C111" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D111" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E111" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F111" s="2" t="str">
+        <f>VLOOKUP(E111,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>

</xml_diff>

<commit_message>
updated fixtures for 02/11/2021
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -553,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F111"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1.2466857032279999</v>
+        <v>0.96034919639999994</v>
       </c>
       <c r="B1" s="1">
-        <v>0.77122205631999996</v>
+        <v>2.6137049112900002</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
@@ -572,23 +572,23 @@
       </c>
       <c r="D1" s="3">
         <f>ROUND(B1,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>1-1</v>
+        <v>1-3</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>VLOOKUP(E1,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.92895543587000007</v>
+        <v>0.99148183876799989</v>
       </c>
       <c r="B2" s="1">
-        <v>1.9954619178780002</v>
+        <v>1.6456127328300001</v>
       </c>
       <c r="C2" s="3">
         <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
@@ -608,135 +608,135 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1.98307226052</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.36493978900399998</v>
-      </c>
-      <c r="C3" s="3">
-        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
+      <c r="A3" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B3" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C3" s="3" t="e">
+        <f t="shared" ref="C3:C28" si="3">ROUND(A3,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D3" s="3" t="e">
+        <f t="shared" ref="D3:D28" si="4">ROUND(B3,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="4" t="e">
+        <f t="shared" ref="E3:E28" si="5">CONCATENATE(C3,"-",D3)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F3" s="2" t="e">
+        <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C4" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D4" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F4" s="2" t="e">
+        <f>VLOOKUP(E4,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F5" s="2" t="e">
+        <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.805822247456</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.62959891708800009</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
-        <v>2-0</v>
-      </c>
-      <c r="F3" s="2" t="str">
-        <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0.93286148792399992</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2.6489385264900003</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="D6" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.6483615188479999</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.38322355881600001</v>
+      </c>
+      <c r="C7" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-3</v>
-      </c>
-      <c r="F4" s="2" t="str">
-        <f>VLOOKUP(E4,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.44591448283200003</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.19552982910000002</v>
-      </c>
-      <c r="C5" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="D7" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E5" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-0</v>
-      </c>
-      <c r="F5" s="2" t="str">
-        <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.95544735897600008</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.73318686349999995</v>
-      </c>
-      <c r="C6" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F6" s="2" t="str">
-        <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1.4706117648000001</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1.3437224155</v>
-      </c>
-      <c r="C7" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.57187957499999997</v>
+        <v>1.5990601420799999</v>
       </c>
       <c r="B8" s="1">
-        <v>0.56850788050000001</v>
+        <v>1.4952533088640001</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="4"/>
@@ -744,19 +744,19 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1.0349082791999999</v>
+        <v>0.89447572684800003</v>
       </c>
       <c r="B9" s="1">
-        <v>0.77525620200000001</v>
+        <v>1.1836630386560001</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="3"/>
@@ -777,22 +777,22 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1.8007682379959997</v>
+        <v>1.115309880384</v>
       </c>
       <c r="B10" s="1">
-        <v>1.6388274258000002</v>
+        <v>1.1934788307200002</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -801,10 +801,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1.9908924147200002</v>
+        <v>2.0257112851200003</v>
       </c>
       <c r="B11" s="1">
-        <v>1.1377013652399999</v>
+        <v>0.47036755064800007</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="3"/>
@@ -812,11 +812,11 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>2-0</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>VLOOKUP(E11,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -825,14 +825,14 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.9801434777600002</v>
+        <v>1.1576232575999998</v>
       </c>
       <c r="B12" s="1">
-        <v>0.957904065759</v>
+        <v>0.60178616080000014</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="4"/>
@@ -840,31 +840,31 @@
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.42623656459999998</v>
+        <v>0.670864147104</v>
       </c>
       <c r="B13" s="1">
-        <v>0.38561102815999998</v>
+        <v>1.311597744048</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>0-0</v>
+        <v>1-1</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>VLOOKUP(E13,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -873,14 +873,14 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>0.5893787801999999</v>
+        <v>1.7359653205439998</v>
       </c>
       <c r="B14" s="1">
-        <v>1.9887362860800002</v>
+        <v>1.6395339442079999</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="4"/>
@@ -888,43 +888,43 @@
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>2-2</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>VLOOKUP(E14,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.39725896184</v>
+        <v>2.3985902131199999</v>
       </c>
       <c r="B15" s="1">
-        <v>1.22131007691</v>
+        <v>0.49184106456000004</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F15" s="2" t="str">
         <f>VLOOKUP(E15,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.5187307543999999</v>
+        <v>2.1078892262400002</v>
       </c>
       <c r="B16" s="1">
-        <v>1.0713103746600001</v>
+        <v>1.4298227654210001</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="3"/>
@@ -945,10 +945,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1.9220068940199999</v>
+        <v>2.0438694777599999</v>
       </c>
       <c r="B17" s="1">
-        <v>0.76330395472800006</v>
+        <v>1.1493748773999997</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="3"/>
@@ -969,10 +969,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.38859192944</v>
+        <v>1.065775196928</v>
       </c>
       <c r="B18" s="1">
-        <v>1.0285679584830001</v>
+        <v>0.77065458436199985</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="3"/>
@@ -993,34 +993,34 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.4411644744200001</v>
+        <v>2.5673801429539997</v>
       </c>
       <c r="B19" s="1">
-        <v>1.12897326528</v>
+        <v>0.34672568990399999</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>3-0</v>
       </c>
       <c r="F19" s="2" t="str">
         <f>VLOOKUP(E19,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.92655216195000012</v>
+        <v>1.331816063092</v>
       </c>
       <c r="B20" s="1">
-        <v>2.0321572109000003</v>
+        <v>0.90164746062000001</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="3"/>
@@ -1028,35 +1028,35 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F20" s="2" t="str">
         <f>VLOOKUP(E20,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>0.52021689609599997</v>
+        <v>1.7534902655700002</v>
       </c>
       <c r="B21" s="1">
-        <v>0.22813242080000001</v>
+        <v>0.98966531101499999</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>2-1</v>
       </c>
       <c r="F21" s="2" t="str">
         <f>VLOOKUP(E21,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1065,22 +1065,22 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.9152835436800004</v>
+        <v>1.483040598876</v>
       </c>
       <c r="B22" s="1">
-        <v>1.637489765625</v>
+        <v>1.0049384181000001</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
       <c r="F22" s="2" t="str">
         <f>VLOOKUP(E22,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1089,10 +1089,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1.8460168117159999</v>
+        <v>2.0287658921760001</v>
       </c>
       <c r="B23" s="1">
-        <v>1.62675277632</v>
+        <v>0.15966602799999999</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="3"/>
@@ -1100,23 +1100,23 @@
       </c>
       <c r="D23" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>2-0</v>
       </c>
       <c r="F23" s="2" t="str">
         <f>VLOOKUP(E23,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>0.58600652849199997</v>
+        <v>1.0900137231360001</v>
       </c>
       <c r="B24" s="1">
-        <v>0.67478041152000001</v>
+        <v>2.1017997758080003</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="3"/>
@@ -1124,27 +1124,27 @@
       </c>
       <c r="D24" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F24" s="2" t="str">
         <f>VLOOKUP(E24,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1.0868657409119999</v>
+        <v>1.9026045953279997</v>
       </c>
       <c r="B25" s="1">
-        <v>0.77122205631999996</v>
+        <v>0.91957490191199986</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" si="4"/>
@@ -1152,23 +1152,23 @@
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F25" s="2" t="str">
         <f>VLOOKUP(E25,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>0.50345913046799995</v>
+        <v>1.5223269704719999</v>
       </c>
       <c r="B26" s="1">
-        <v>1.208509562385</v>
+        <v>1.1973014367600001</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="4"/>
@@ -1176,19 +1176,19 @@
       </c>
       <c r="E26" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F26" s="2" t="str">
         <f>VLOOKUP(E26,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>0.83909855077999995</v>
+        <v>1.287909994104</v>
       </c>
       <c r="B27" s="1">
-        <v>0.55776595164999998</v>
+        <v>0.49594011642500002</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="3"/>
@@ -1196,27 +1196,27 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F27" s="2" t="str">
         <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>2.1600432000000001</v>
+        <v>1.286519338512</v>
       </c>
       <c r="B28" s="1">
-        <v>1.2378935636279997</v>
+        <v>0.77350797810000005</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="4"/>
@@ -1224,2004 +1224,674 @@
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F28" s="2" t="str">
         <f>VLOOKUP(E28,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>0.7500150000000001</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2.5263324440640003</v>
-      </c>
-      <c r="C29" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E29" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-3</v>
-      </c>
-      <c r="F29" s="2" t="str">
-        <f>VLOOKUP(E29,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>0.54001080000000001</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1.6673920798499997</v>
-      </c>
-      <c r="C30" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E30" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F30" s="2" t="str">
-        <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>1.8646226395499998</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.95344784799000004</v>
-      </c>
-      <c r="C31" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E31" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F31" s="2" t="str">
-        <f>VLOOKUP(E31,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>1.189057243902</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1.12690135228</v>
-      </c>
-      <c r="C32" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F32" s="2" t="str">
-        <f>VLOOKUP(E32,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>1.229541016088</v>
-      </c>
-      <c r="B33" s="1">
-        <v>0.91560109871999995</v>
-      </c>
-      <c r="C33" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E33" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F33" s="2" t="str">
-        <f>VLOOKUP(E33,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>1.3467790774619999</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1.50383137905</v>
-      </c>
-      <c r="C34" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E34" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F34" s="2" t="str">
-        <f>VLOOKUP(E34,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>0.81364254191999996</v>
-      </c>
-      <c r="B35" s="1">
-        <v>1.2861456779849998</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F35" s="2" t="str">
-        <f>VLOOKUP(E35,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>1.4141568552479999</v>
-      </c>
-      <c r="B36" s="1">
-        <v>0.70847516707500002</v>
-      </c>
-      <c r="C36" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E36" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F36" s="2" t="str">
-        <f>VLOOKUP(E36,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>1.7399758616940002</v>
-      </c>
-      <c r="B37" s="1">
-        <v>0.87742645425600008</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E37" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F37" s="2" t="str">
-        <f>VLOOKUP(E37,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>2.5309535238540004</v>
-      </c>
-      <c r="B38" s="1">
-        <v>1.5953738548</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E38" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-2</v>
-      </c>
-      <c r="F38" s="2" t="str">
-        <f>VLOOKUP(E38,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>1.09819515824</v>
-      </c>
-      <c r="B39" s="1">
-        <v>3.1048364814000005</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E39" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-3</v>
-      </c>
-      <c r="F39" s="2" t="str">
-        <f>VLOOKUP(E39,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>0.20591159216999999</v>
-      </c>
-      <c r="B40" s="1">
-        <v>1.41113325024</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E40" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-1</v>
-      </c>
-      <c r="F40" s="2" t="str">
-        <f>VLOOKUP(E40,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>1.5853625874600001</v>
-      </c>
-      <c r="B41" s="1">
-        <v>0.98785327232999998</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E41" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F41" s="2" t="str">
-        <f>VLOOKUP(E41,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>0.47646111174</v>
-      </c>
-      <c r="B42" s="1">
-        <v>0.58064682251999999</v>
-      </c>
-      <c r="C42" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E42" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>0-1</v>
-      </c>
-      <c r="F42" s="2" t="str">
-        <f>VLOOKUP(E42,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>3.2485381632000001</v>
-      </c>
-      <c r="B43" s="1">
-        <v>0.36662914469999996</v>
-      </c>
-      <c r="C43" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-0</v>
-      </c>
-      <c r="F43" s="2" t="str">
-        <f>VLOOKUP(E43,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>2.6009178084000002</v>
-      </c>
-      <c r="B44" s="1">
-        <v>0.7983468065999999</v>
-      </c>
-      <c r="C44" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E44" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>3-1</v>
-      </c>
-      <c r="F44" s="2" t="str">
-        <f>VLOOKUP(E44,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>1.0623354060800001</v>
-      </c>
-      <c r="B45" s="1">
-        <v>1.4436481200000002</v>
-      </c>
-      <c r="C45" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D45" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E45" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F45" s="2" t="str">
-        <f>VLOOKUP(E45,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>2.0656021848160004</v>
-      </c>
-      <c r="B46" s="1">
-        <v>1.637489765625</v>
-      </c>
-      <c r="C46" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D46" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E46" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-2</v>
-      </c>
-      <c r="F46" s="2" t="str">
-        <f>VLOOKUP(E46,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>1.9123608811520003</v>
-      </c>
-      <c r="B47" s="1">
-        <v>0.67369578937499985</v>
-      </c>
-      <c r="C47" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D47" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E47" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F47" s="2" t="str">
-        <f>VLOOKUP(E47,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>0.56336574528000005</v>
-      </c>
-      <c r="B48" s="1">
-        <v>1.8245885962499999</v>
-      </c>
-      <c r="C48" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D48" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E48" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F48" s="2" t="str">
-        <f>VLOOKUP(E48,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>0.70810566480000003</v>
-      </c>
-      <c r="B49" s="1">
-        <v>1.7636424414999998</v>
-      </c>
-      <c r="C49" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D49" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E49" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F49" s="2" t="str">
-        <f>VLOOKUP(E49,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>1.4161113288</v>
-      </c>
-      <c r="B50" s="1">
-        <v>0.50388236350000004</v>
-      </c>
-      <c r="C50" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D50" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E50" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F50" s="2" t="str">
-        <f>VLOOKUP(E50,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>2.0060854946999997</v>
-      </c>
-      <c r="B51" s="1">
-        <v>1.4470549092499998</v>
-      </c>
-      <c r="C51" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D51" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E51" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F51" s="2" t="str">
-        <f>VLOOKUP(E51,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>0.9781052466900001</v>
-      </c>
-      <c r="B52" s="1">
-        <v>4.0304469490899999</v>
-      </c>
-      <c r="C52" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D52" s="3">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="E52" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-4</v>
-      </c>
-      <c r="F52" s="2" t="str">
-        <f>VLOOKUP(E52,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>0.85596709224000012</v>
-      </c>
-      <c r="B53" s="1">
-        <v>1.2645143385349999</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E53" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F53" s="2" t="str">
-        <f>VLOOKUP(E53,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>1.301119197312</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1.751433145245</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E54" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F54" s="2" t="str">
-        <f>VLOOKUP(E54,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>1.77139646208</v>
-      </c>
-      <c r="B55" s="1">
-        <v>0.86851852032999988</v>
-      </c>
-      <c r="C55" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E55" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F55" s="2" t="str">
-        <f>VLOOKUP(E55,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>0.90834476927999996</v>
-      </c>
-      <c r="B56" s="1">
-        <v>0.68236187148999994</v>
-      </c>
-      <c r="C56" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E56" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F56" s="2" t="str">
-        <f>VLOOKUP(E56,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>2.1573782000640001</v>
-      </c>
-      <c r="B57" s="1">
-        <v>0.62258951565499998</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E57" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F57" s="2" t="str">
-        <f>VLOOKUP(E57,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>1.294609192632</v>
-      </c>
-      <c r="B58" s="1">
-        <v>0.65071861002000009</v>
-      </c>
-      <c r="C58" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D58" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E58" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F58" s="2" t="str">
-        <f>VLOOKUP(E58,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>1.43845465848</v>
-      </c>
-      <c r="B59" s="1">
-        <v>1.6732978549499999</v>
-      </c>
-      <c r="C59" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D59" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E59" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F59" s="2" t="str">
-        <f>VLOOKUP(E59,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>1.5628248127659998</v>
-      </c>
-      <c r="B60" s="1">
-        <v>1.32213781206</v>
-      </c>
-      <c r="C60" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D60" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E60" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F60" s="2" t="str">
-        <f>VLOOKUP(E60,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>1.1508387244199998</v>
-      </c>
-      <c r="B61" s="1">
-        <v>1.7351718511999998</v>
-      </c>
-      <c r="C61" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D61" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E61" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F61" s="2" t="str">
-        <f>VLOOKUP(E61,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>0.86307279508800006</v>
-      </c>
-      <c r="B62" s="1">
-        <v>1.5803701972949999</v>
-      </c>
-      <c r="C62" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D62" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E62" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F62" s="2" t="str">
-        <f>VLOOKUP(E62,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>2.2400447999999997</v>
-      </c>
-      <c r="B63" s="1">
-        <v>1.2378935636279997</v>
-      </c>
-      <c r="C63" s="3">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D63" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E63" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>2-1</v>
-      </c>
-      <c r="F63" s="2" t="str">
-        <f>VLOOKUP(E63,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>1.3500270000000003</v>
-      </c>
-      <c r="B64" s="1">
-        <v>1.7053794002339999</v>
-      </c>
-      <c r="C64" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D64" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E64" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-2</v>
-      </c>
-      <c r="F64" s="2" t="str">
-        <f>VLOOKUP(E64,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>1.4400287999999999</v>
-      </c>
-      <c r="B65" s="1">
-        <v>0.9094656789179999</v>
-      </c>
-      <c r="C65" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D65" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E65" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F65" s="2" t="str">
-        <f>VLOOKUP(E65,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>0.8899287366419999</v>
-      </c>
-      <c r="B66" s="1">
-        <v>0.71844229214999999</v>
-      </c>
-      <c r="C66" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D66" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E66" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>1-1</v>
-      </c>
-      <c r="F66" s="2" t="str">
-        <f>VLOOKUP(E66,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>1.194495558102</v>
-      </c>
-      <c r="B67" s="1">
-        <v>0.85459197885600002</v>
-      </c>
-      <c r="C67" s="3">
-        <f t="shared" ref="C67:C111" si="6">ROUND(A67,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D67" s="3">
-        <f t="shared" ref="D67:D111" si="7">ROUND(B67,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E67" s="4" t="str">
-        <f t="shared" ref="E67:E111" si="8">CONCATENATE(C67,"-",D67)</f>
-        <v>1-1</v>
-      </c>
-      <c r="F67" s="2" t="str">
-        <f>VLOOKUP(E67,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>0.87315871034699988</v>
-      </c>
-      <c r="B68" s="1">
-        <v>1.2135014561999999</v>
-      </c>
-      <c r="C68" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D68" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E68" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F68" s="2" t="str">
-        <f>VLOOKUP(E68,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="4"/>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>0.70256629627799994</v>
-      </c>
-      <c r="B69" s="1">
-        <v>0.70430084516000002</v>
-      </c>
-      <c r="C69" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D69" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E69" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F69" s="2" t="str">
-        <f>VLOOKUP(E69,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="4"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>0.32788427063699999</v>
-      </c>
-      <c r="B70" s="1">
-        <v>0.72310086772000004</v>
-      </c>
-      <c r="C70" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D70" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E70" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-1</v>
-      </c>
-      <c r="F70" s="2" t="str">
-        <f>VLOOKUP(E70,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>1.2591554046799998</v>
-      </c>
-      <c r="B71" s="1">
-        <v>1.720373290008</v>
-      </c>
-      <c r="C71" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D71" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E71" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F71" s="2" t="str">
-        <f>VLOOKUP(E71,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>0.50368502027999995</v>
-      </c>
-      <c r="B72" s="1">
-        <v>1.0948193670120001</v>
-      </c>
-      <c r="C72" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D72" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E72" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F72" s="2" t="str">
-        <f>VLOOKUP(E72,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>2.9745333937200003</v>
-      </c>
-      <c r="B73" s="1">
-        <v>0.54740968350600006</v>
-      </c>
-      <c r="C73" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D73" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E73" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F73" s="2" t="str">
-        <f>VLOOKUP(E73,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>1.4138890211840001</v>
-      </c>
-      <c r="B74" s="1">
-        <v>1.642162382672</v>
-      </c>
-      <c r="C74" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D74" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E74" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F74" s="2" t="str">
-        <f>VLOOKUP(E74,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>0.73456009972799985</v>
-      </c>
-      <c r="B75" s="1">
-        <v>1.1175114381389999</v>
-      </c>
-      <c r="C75" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D75" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E75" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F75" s="2" t="str">
-        <f>VLOOKUP(E75,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>1.3675629098250002</v>
-      </c>
-      <c r="B76" s="1">
-        <v>1.142775509796</v>
-      </c>
-      <c r="C76" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D76" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E76" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F76" s="2" t="str">
-        <f>VLOOKUP(E76,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>0.92310543</v>
-      </c>
-      <c r="B77" s="1">
-        <v>0.92308021796700002</v>
-      </c>
-      <c r="C77" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D77" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E77" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F77" s="2" t="str">
-        <f>VLOOKUP(E77,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>1.4118589850040002</v>
-      </c>
-      <c r="B78" s="1">
-        <v>1.0549107261120001</v>
-      </c>
-      <c r="C78" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D78" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E78" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F78" s="2" t="str">
-        <f>VLOOKUP(E78,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>1.509865215354</v>
-      </c>
-      <c r="B79" s="1">
-        <v>1.2088074280350001</v>
-      </c>
-      <c r="C79" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D79" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E79" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F79" s="2" t="str">
-        <f>VLOOKUP(E79,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>1.7376536614320002</v>
-      </c>
-      <c r="B80" s="1">
-        <v>0.73035121324800001</v>
-      </c>
-      <c r="C80" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D80" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E80" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F80" s="2" t="str">
-        <f>VLOOKUP(E80,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>0.58832586072000015</v>
-      </c>
-      <c r="B81" s="1">
-        <v>0.59341036076400011</v>
-      </c>
-      <c r="C81" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D81" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E81" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F81" s="2" t="str">
-        <f>VLOOKUP(E81,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>0.93686139783000011</v>
-      </c>
-      <c r="B82" s="1">
-        <v>0.74222279332500007</v>
-      </c>
-      <c r="C82" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D82" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E82" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F82" s="2" t="str">
-        <f>VLOOKUP(E82,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>1.3179611031839999</v>
-      </c>
-      <c r="B83" s="1">
-        <v>1.491604296245</v>
-      </c>
-      <c r="C83" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D83" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E83" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F83" s="2" t="str">
-        <f>VLOOKUP(E83,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>1.6217681383079998</v>
-      </c>
-      <c r="B84" s="1">
-        <v>1.4329147793400001</v>
-      </c>
-      <c r="C84" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D84" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E84" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F84" s="2" t="str">
-        <f>VLOOKUP(E84,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>1.495995181326</v>
-      </c>
-      <c r="B85" s="1">
-        <v>1.0984610212500001</v>
-      </c>
-      <c r="C85" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D85" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E85" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F85" s="2" t="str">
-        <f>VLOOKUP(E85,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>3.217069320192</v>
-      </c>
-      <c r="B86" s="1">
-        <v>0.95717582901600007</v>
-      </c>
-      <c r="C86" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D86" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E86" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F86" s="2" t="str">
-        <f>VLOOKUP(E86,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>2.2597659448140002</v>
-      </c>
-      <c r="B87" s="1">
-        <v>1.243107332808</v>
-      </c>
-      <c r="C87" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D87" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E87" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F87" s="2" t="str">
-        <f>VLOOKUP(E87,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>1.0358215430639999</v>
-      </c>
-      <c r="B88" s="1">
-        <v>1.8346507671360002</v>
-      </c>
-      <c r="C88" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D88" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E88" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F88" s="2" t="str">
-        <f>VLOOKUP(E88,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>1.4687716147020002</v>
-      </c>
-      <c r="B89" s="1">
-        <v>1.196442893448</v>
-      </c>
-      <c r="C89" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D89" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E89" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F89" s="2" t="str">
-        <f>VLOOKUP(E89,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>2.8398273423660001</v>
-      </c>
-      <c r="B90" s="1">
-        <v>1.2307312597800002</v>
-      </c>
-      <c r="C90" s="3">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="D90" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E90" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>3-1</v>
-      </c>
-      <c r="F90" s="2" t="str">
-        <f>VLOOKUP(E90,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>2.2522320305100005</v>
-      </c>
-      <c r="B91" s="1">
-        <v>1.0370221715040002</v>
-      </c>
-      <c r="C91" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D91" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E91" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F91" s="2" t="str">
-        <f>VLOOKUP(E91,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>2.2647441726800004</v>
-      </c>
-      <c r="B92" s="1">
-        <v>0.19752398607000002</v>
-      </c>
-      <c r="C92" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D92" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E92" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F92" s="2" t="str">
-        <f>VLOOKUP(E92,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>0.88244967911999994</v>
-      </c>
-      <c r="B93" s="1">
-        <v>4.2338497471499998</v>
-      </c>
-      <c r="C93" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D93" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="E93" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-4</v>
-      </c>
-      <c r="F93" s="2" t="str">
-        <f>VLOOKUP(E93,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>0.92655216195000012</v>
-      </c>
-      <c r="B94" s="1">
-        <v>0.70560829080000009</v>
-      </c>
-      <c r="C94" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D94" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E94" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F94" s="2" t="str">
-        <f>VLOOKUP(E94,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <v>2.0063794544640001</v>
-      </c>
-      <c r="B95" s="1">
-        <v>0.85539657839999994</v>
-      </c>
-      <c r="C95" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D95" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E95" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F95" s="2" t="str">
-        <f>VLOOKUP(E95,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>2.3408760291840003</v>
-      </c>
-      <c r="B96" s="1">
-        <v>0.25663230679999999</v>
-      </c>
-      <c r="C96" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D96" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E96" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F96" s="2" t="str">
-        <f>VLOOKUP(E96,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>1.0589462991359999</v>
-      </c>
-      <c r="B97" s="1">
-        <v>1.283161534</v>
-      </c>
-      <c r="C97" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D97" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E97" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F97" s="2" t="str">
-        <f>VLOOKUP(E97,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>1.5935221612160002</v>
-      </c>
-      <c r="B98" s="1">
-        <v>1.3232917293749997</v>
-      </c>
-      <c r="C98" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D98" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E98" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F98" s="2" t="str">
-        <f>VLOOKUP(E98,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>1.126745779632</v>
-      </c>
-      <c r="B99" s="1">
-        <v>1.1227929824999998</v>
-      </c>
-      <c r="C99" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D99" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E99" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F99" s="2" t="str">
-        <f>VLOOKUP(E99,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>1.0816342326400004</v>
-      </c>
-      <c r="B100" s="1">
-        <v>0.16839894749999998</v>
-      </c>
-      <c r="C100" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D100" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E100" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-0</v>
-      </c>
-      <c r="F100" s="2" t="str">
-        <f>VLOOKUP(E100,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>1.3571664110999999</v>
-      </c>
-      <c r="B101" s="1">
-        <v>1.4728484485000002</v>
-      </c>
-      <c r="C101" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D101" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E101" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F101" s="2" t="str">
-        <f>VLOOKUP(E101,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>0.49928454809999995</v>
-      </c>
-      <c r="B102" s="1">
-        <v>1.5116470905000001</v>
-      </c>
-      <c r="C102" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D102" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E102" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>0-2</v>
-      </c>
-      <c r="F102" s="2" t="str">
-        <f>VLOOKUP(E102,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>0.85582709107999999</v>
-      </c>
-      <c r="B103" s="1">
-        <v>0.63219716574000007</v>
-      </c>
-      <c r="C103" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D103" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E103" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F103" s="2" t="str">
-        <f>VLOOKUP(E103,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>1.4672378721000003</v>
-      </c>
-      <c r="B104" s="1">
-        <v>1.896711504275</v>
-      </c>
-      <c r="C104" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D104" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E104" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-2</v>
-      </c>
-      <c r="F104" s="2" t="str">
-        <f>VLOOKUP(E104,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>1.3448197153300001</v>
-      </c>
-      <c r="B105" s="1">
-        <v>0.92193753450000004</v>
-      </c>
-      <c r="C105" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D105" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E105" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F105" s="2" t="str">
-        <f>VLOOKUP(E105,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>1.6133713052159999</v>
-      </c>
-      <c r="B106" s="1">
-        <v>0.47890828098099991</v>
-      </c>
-      <c r="C106" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D106" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E106" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-0</v>
-      </c>
-      <c r="F106" s="2" t="str">
-        <f>VLOOKUP(E106,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>1.5089801955840003</v>
-      </c>
-      <c r="B107" s="1">
-        <v>0.51089050199099995</v>
-      </c>
-      <c r="C107" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D107" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E107" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F107" s="2" t="str">
-        <f>VLOOKUP(E107,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="2"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <v>0.99917924620799992</v>
-      </c>
-      <c r="B108" s="1">
-        <v>1.1384215442200001</v>
-      </c>
-      <c r="C108" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D108" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E108" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F108" s="2" t="str">
-        <f>VLOOKUP(E108,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="2"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <v>1.0433371557120001</v>
-      </c>
-      <c r="B109" s="1">
-        <v>1.3648686044140002</v>
-      </c>
-      <c r="C109" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D109" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E109" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F109" s="2" t="str">
-        <f>VLOOKUP(E109,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>0.92729413862400023</v>
-      </c>
-      <c r="B110" s="1">
-        <v>1.1049332142050001</v>
-      </c>
-      <c r="C110" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D110" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E110" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>1-1</v>
-      </c>
-      <c r="F110" s="2" t="str">
-        <f>VLOOKUP(E110,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>2.3397315102720002</v>
-      </c>
-      <c r="B111" s="1">
-        <v>0.68414575908899999</v>
-      </c>
-      <c r="C111" s="3">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="D111" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="E111" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v>2-1</v>
-      </c>
-      <c r="F111" s="2" t="str">
-        <f>VLOOKUP(E111,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>

</xml_diff>

<commit_message>
updated odds for newleagues
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitboyzorro5\FDAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magut\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CDAF96-4357-4E4F-9DF3-D4EC747F5BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11280"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="score_newleagues" sheetId="1" r:id="rId1"/>
     <sheet name="cs_lookupnewleagues" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -204,7 +211,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -550,45 +557,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F28"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0.96034919639999994</v>
+        <v>2.5573193907519998</v>
       </c>
       <c r="B1" s="1">
-        <v>2.6137049112900002</v>
+        <v>1.32213781206</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3">
         <f>ROUND(B1,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" s="4" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>1-3</v>
+        <v>3-1</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>VLOOKUP(E1,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.99148183876799989</v>
+        <v>1.432205761536</v>
       </c>
       <c r="B2" s="1">
-        <v>1.6456127328300001</v>
+        <v>1.231621787004</v>
       </c>
       <c r="C2" s="3">
         <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
@@ -596,95 +603,95 @@
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2" si="1">ROUND(B2,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(E2,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B3" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C3" s="3" t="e">
-        <f t="shared" ref="C3:C28" si="3">ROUND(A3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D3" s="3" t="e">
-        <f t="shared" ref="D3:D28" si="4">ROUND(B3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E3" s="4" t="e">
-        <f t="shared" ref="E3:E28" si="5">CONCATENATE(C3,"-",D3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F3" s="2" t="e">
+      <c r="A3" s="1">
+        <v>1.3424170728499998</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.62858652910200008</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
+        <v>1-1</v>
+      </c>
+      <c r="F3" s="2" t="str">
         <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>X</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B4" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C4" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D4" s="3" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E4" s="4" t="e">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F4" s="2" t="e">
+      <c r="A4" s="1">
+        <v>0.5680506373919999</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.971375253398</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F4" s="2" t="str">
         <f>VLOOKUP(E4,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B5" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C5" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D5" s="3" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E5" s="4" t="e">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F5" s="2" t="e">
+      <c r="A5" s="1">
+        <v>0.99148183876799989</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.43994114</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F5" s="2" t="str">
         <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>X</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1.805822247456</v>
+        <v>1.72935737029</v>
       </c>
       <c r="B6" s="1">
-        <v>0.62959891708800009</v>
+        <v>0.13544159142000001</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="3"/>
@@ -692,11 +699,11 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>2-0</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -705,10 +712,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1.6483615188479999</v>
+        <v>1.64715939652</v>
       </c>
       <c r="B7" s="1">
-        <v>0.38322355881600001</v>
+        <v>0.67736795898000002</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="3"/>
@@ -716,11 +723,11 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-0</v>
+        <v>2-1</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -729,14 +736,14 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1.5990601420799999</v>
+        <v>1.30054224024</v>
       </c>
       <c r="B8" s="1">
-        <v>1.4952533088640001</v>
+        <v>0.66533067199999996</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="4"/>
@@ -744,23 +751,23 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0.89447572684800003</v>
+        <v>0.27862333876800005</v>
       </c>
       <c r="B9" s="1">
-        <v>1.1836630386560001</v>
+        <v>1.0265292271999999</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="4"/>
@@ -768,31 +775,31 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-1</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>VLOOKUP(E9,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1.115309880384</v>
+        <v>1.9333750591399999</v>
       </c>
       <c r="B10" s="1">
-        <v>1.1934788307200002</v>
+        <v>2.2311638094599999</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -801,38 +808,38 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.0257112851200003</v>
+        <v>1.074066144368</v>
       </c>
       <c r="B11" s="1">
-        <v>0.47036755064800007</v>
+        <v>1.0796797686399999</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-0</v>
+        <v>1-1</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>VLOOKUP(E11,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.1576232575999998</v>
+        <v>1.8413419590719999</v>
       </c>
       <c r="B12" s="1">
-        <v>0.60178616080000014</v>
+        <v>1.4178625545499999</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="4"/>
@@ -840,19 +847,19 @@
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.670864147104</v>
+        <v>1.36395700672</v>
       </c>
       <c r="B13" s="1">
-        <v>1.311597744048</v>
+        <v>0.154209966955</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="3"/>
@@ -860,35 +867,35 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-0</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>VLOOKUP(E13,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.7359653205439998</v>
+        <v>0.81842753915999988</v>
       </c>
       <c r="B14" s="1">
-        <v>1.6395339442079999</v>
+        <v>0.99162835976000008</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>VLOOKUP(E14,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -897,10 +904,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2.3985902131199999</v>
+        <v>2.4000480000000004</v>
       </c>
       <c r="B15" s="1">
-        <v>0.49184106456000004</v>
+        <v>0.43308365587199993</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
@@ -921,14 +928,14 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2.1078892262400002</v>
+        <v>0.45000900000000005</v>
       </c>
       <c r="B16" s="1">
-        <v>1.4298227654210001</v>
+        <v>1.3894628447699999</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
@@ -936,19 +943,19 @@
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>0-1</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>VLOOKUP(E16,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2.0438694777599999</v>
+        <v>1.6714834290000002</v>
       </c>
       <c r="B17" s="1">
-        <v>1.1493748773999997</v>
+        <v>1.78655698935</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="3"/>
@@ -956,23 +963,23 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>2-2</v>
       </c>
       <c r="F17" s="2" t="str">
         <f>VLOOKUP(E17,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.065775196928</v>
+        <v>1.3872334512189999</v>
       </c>
       <c r="B18" s="1">
-        <v>0.77065458436199985</v>
+        <v>0.98600118320000008</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="3"/>
@@ -993,38 +1000,38 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>2.5673801429539997</v>
+        <v>1.3578189662400002</v>
       </c>
       <c r="B19" s="1">
-        <v>0.34672568990399999</v>
+        <v>1.28943334245</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>3-0</v>
+        <v>1-1</v>
       </c>
       <c r="F19" s="2" t="str">
         <f>VLOOKUP(E19,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1.331816063092</v>
+        <v>1.9967862639779999</v>
       </c>
       <c r="B20" s="1">
-        <v>0.90164746062000001</v>
+        <v>0.68772800579999993</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="4"/>
@@ -1032,67 +1039,67 @@
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F20" s="2" t="str">
         <f>VLOOKUP(E20,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1.7534902655700002</v>
+        <v>0.71285565542400009</v>
       </c>
       <c r="B21" s="1">
-        <v>0.98966531101499999</v>
+        <v>1.5678168346880001</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F21" s="2" t="str">
         <f>VLOOKUP(E21,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.483040598876</v>
+        <v>2.316687132672</v>
       </c>
       <c r="B22" s="1">
-        <v>1.0049384181000001</v>
+        <v>0.45290625093599995</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F22" s="2" t="str">
         <f>VLOOKUP(E22,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>2.0287658921760001</v>
+        <v>1.861806760416</v>
       </c>
       <c r="B23" s="1">
-        <v>0.15966602799999999</v>
+        <v>0.55739904127200002</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="3"/>
@@ -1100,11 +1107,11 @@
       </c>
       <c r="D23" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-0</v>
+        <v>2-1</v>
       </c>
       <c r="F23" s="2" t="str">
         <f>VLOOKUP(E23,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
@@ -1113,58 +1120,58 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1.0900137231360001</v>
+        <v>1.8136310742270001</v>
       </c>
       <c r="B24" s="1">
-        <v>2.1017997758080003</v>
+        <v>0.94240372000000006</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>2-1</v>
       </c>
       <c r="F24" s="2" t="str">
         <f>VLOOKUP(E24,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1.9026045953279997</v>
+        <v>1.2099642904799999</v>
       </c>
       <c r="B25" s="1">
-        <v>0.91957490191199986</v>
+        <v>1.5977278232300001</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F25" s="2" t="str">
         <f>VLOOKUP(E25,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1.5223269704719999</v>
+        <v>1.8397642764599997</v>
       </c>
       <c r="B26" s="1">
-        <v>1.1973014367600001</v>
+        <v>0.66485130183999996</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="3"/>
@@ -1185,10 +1192,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1.287909994104</v>
+        <v>0.96407436211800002</v>
       </c>
       <c r="B27" s="1">
-        <v>0.49594011642500002</v>
+        <v>1.9372158707000002</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="3"/>
@@ -1196,27 +1203,27 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>1-2</v>
       </c>
       <c r="F27" s="2" t="str">
         <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1.286519338512</v>
+        <v>1.6872301275900001</v>
       </c>
       <c r="B28" s="1">
-        <v>0.77350797810000005</v>
+        <v>1.0028254711200002</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="4"/>
@@ -1224,730 +1231,2172 @@
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F28" s="2" t="str">
         <f>VLOOKUP(E28,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1.8529543235500001</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.57242562075</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E29" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-2</v>
+      </c>
+      <c r="F29" s="2" t="str">
+        <f>VLOOKUP(E29,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
         <v>X</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="2"/>
-    </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="2"/>
+      <c r="A30" s="1">
+        <v>1.8529243234799999</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.98780994144000012</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F30" s="2" t="str">
+        <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="2"/>
+      <c r="A31" s="1">
+        <v>2.4913469248400002</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.56447329915</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F31" s="2" t="str">
+        <f>VLOOKUP(E31,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="2"/>
+      <c r="A32" s="1">
+        <v>0.61773477651000008</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3.8103397694900001</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E32" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-4</v>
+      </c>
+      <c r="F32" s="2" t="str">
+        <f>VLOOKUP(E32,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="2"/>
+      <c r="A33" s="1">
+        <v>0.17340563203199999</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.3306613439999999</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E33" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>0-1</v>
+      </c>
+      <c r="F33" s="2" t="str">
+        <f>VLOOKUP(E33,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="2"/>
+      <c r="A34" s="1">
+        <v>0.52021689609599997</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.3991984032</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-0</v>
+      </c>
+      <c r="F34" s="2" t="str">
+        <f>VLOOKUP(E34,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="2"/>
+      <c r="A35" s="1">
+        <v>1.2619599397679999</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.89826105249999999</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f>VLOOKUP(E35,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="2"/>
+      <c r="A36" s="1">
+        <v>1.1266314966400002</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1.563890225625</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F36" s="2" t="str">
+        <f>VLOOKUP(E36,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="2"/>
+      <c r="A37" s="1">
+        <v>2.3437541774720008</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.70179561374999988</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F37" s="2" t="str">
+        <f>VLOOKUP(E37,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="2"/>
+      <c r="A38" s="1">
+        <v>1.4872095721600003</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.0105836850000001</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F38" s="2" t="str">
+        <f>VLOOKUP(E38,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="2"/>
+      <c r="A39" s="1">
+        <v>1.7635774193999998</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.2164574224999998</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F39" s="2" t="str">
+        <f>VLOOKUP(E39,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="2"/>
+      <c r="A40" s="1">
+        <v>1.67071869</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.90815401224999992</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F40" s="2" t="str">
+        <f>VLOOKUP(E40,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="2"/>
+      <c r="A41" s="1">
+        <v>1.4077112616</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.62017829299999994</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F41" s="2" t="str">
+        <f>VLOOKUP(E41,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="2"/>
+      <c r="A42" s="1">
+        <v>1.5282969478400001</v>
+      </c>
+      <c r="B42" s="1">
+        <v>3.7319205089599996</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E42" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-4</v>
+      </c>
+      <c r="F42" s="2" t="str">
+        <f>VLOOKUP(E42,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="2"/>
+      <c r="A43" s="1">
+        <v>2.5470449121000001</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1.7562143569349997</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E43" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-2</v>
+      </c>
+      <c r="F43" s="2" t="str">
+        <f>VLOOKUP(E43,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="2"/>
+      <c r="A44" s="1">
+        <v>0.5524185882599999</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.35691421108499999</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-0</v>
+      </c>
+      <c r="F44" s="2" t="str">
+        <f>VLOOKUP(E44,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="2"/>
+      <c r="A45" s="1">
+        <v>1.074066144368</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.60597399635499993</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F45" s="2" t="str">
+        <f>VLOOKUP(E45,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="2"/>
+      <c r="A46" s="1">
+        <v>2.4551226120959999</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.41642991076500002</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-0</v>
+      </c>
+      <c r="F46" s="2" t="str">
+        <f>VLOOKUP(E46,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="2"/>
+      <c r="A47" s="1">
+        <v>2.4551226120959999</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.53540131445999994</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E47" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F47" s="2" t="str">
+        <f>VLOOKUP(E47,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="2"/>
+      <c r="A48" s="1">
+        <v>0.83335000000000004</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2.9474989624800001</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E48" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-3</v>
+      </c>
+      <c r="F48" s="2" t="str">
+        <f>VLOOKUP(E48,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="2"/>
+      <c r="A49" s="1">
+        <v>1.285775715</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1.2630924147959999</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F49" s="2" t="str">
+        <f>VLOOKUP(E49,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="2"/>
+      <c r="A50" s="1">
+        <v>1.1428228560000002</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1.0827496188719998</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F50" s="2" t="str">
+        <f>VLOOKUP(E50,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="2"/>
+      <c r="A51" s="1">
+        <v>1.112474251911</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.54936065923200006</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F51" s="2" t="str">
+        <f>VLOOKUP(E51,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="2"/>
+      <c r="A52" s="1">
+        <v>2.5095224817739998</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.60362725579199994</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E52" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F52" s="2" t="str">
+        <f>VLOOKUP(E52,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="2"/>
+      <c r="A53" s="1">
+        <v>1.6758884948299997</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1.1919636514500001</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F53" s="2" t="str">
+        <f>VLOOKUP(E53,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="2"/>
+      <c r="A54" s="1">
+        <v>0.75666370110100001</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.95344784799000004</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E54" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F54" s="2" t="str">
+        <f>VLOOKUP(E54,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="2"/>
+      <c r="A55" s="1">
+        <v>1.409117164125</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.92969063895400006</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F55" s="2" t="str">
+        <f>VLOOKUP(E55,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="2"/>
+      <c r="A56" s="1">
+        <v>0.77293006728299996</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.85459197885600002</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E56" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F56" s="2" t="str">
+        <f>VLOOKUP(E56,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="2"/>
+      <c r="A57" s="1">
+        <v>1.32204817368</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1.4368170865560002</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F57" s="2" t="str">
+        <f>VLOOKUP(E57,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="2"/>
+      <c r="A58" s="1">
+        <v>1.2275518780800001</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.70381245022200001</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E58" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F58" s="2" t="str">
+        <f>VLOOKUP(E58,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="2"/>
+      <c r="A59" s="1">
+        <v>0.50368502027999995</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1.2512221337280001</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E59" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F59" s="2" t="str">
+        <f>VLOOKUP(E59,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="2"/>
+      <c r="A60" s="1">
+        <v>1.6324707096319997</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.93841660029600005</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E60" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F60" s="2" t="str">
+        <f>VLOOKUP(E60,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="2"/>
+      <c r="A61" s="1">
+        <v>0.74206071340799995</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1.8098034434280001</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E61" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F61" s="2" t="str">
+        <f>VLOOKUP(E61,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="2"/>
+      <c r="A62" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B62" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C62" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D62" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E62" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F62" s="2" t="e">
+        <f>VLOOKUP(E62,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="2"/>
+      <c r="A63" s="1">
+        <v>2.1478888538200005</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1.6071280599660001</v>
+      </c>
+      <c r="C63" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E63" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-2</v>
+      </c>
+      <c r="F63" s="2" t="str">
+        <f>VLOOKUP(E63,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="2"/>
+      <c r="A64" s="1">
+        <v>2.0087514323999995</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0.83811537213600018</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D64" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E64" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F64" s="2" t="str">
+        <f>VLOOKUP(E64,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="2"/>
+      <c r="A65" s="1">
+        <v>1.6928915604479999</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1.1148980823720001</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D65" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F65" s="2" t="str">
+        <f>VLOOKUP(E65,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="2"/>
+      <c r="A66" s="1">
+        <v>0.628951682304</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.64929373689600001</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D66" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E66" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F66" s="2" t="str">
+        <f>VLOOKUP(E66,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="2"/>
+      <c r="A67" s="1">
+        <v>0.69503864102400004</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1.5050411606240002</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" ref="C67:C118" si="6">ROUND(A67,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D67" s="3">
+        <f t="shared" ref="D67:D118" si="7">ROUND(B67,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E67" s="4" t="str">
+        <f t="shared" ref="E67:E118" si="8">CONCATENATE(C67,"-",D67)</f>
+        <v>1-2</v>
+      </c>
+      <c r="F67" s="2" t="str">
+        <f>VLOOKUP(E67,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="4"/>
+      <c r="A68" s="1">
+        <v>0.424709723712</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1.1252398629919997</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-1</v>
+      </c>
+      <c r="F68" s="2" t="str">
+        <f>VLOOKUP(E68,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="4"/>
+      <c r="A69" s="1">
+        <v>2.6444800051200001</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.49183738702399993</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E69" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-0</v>
+      </c>
+      <c r="F69" s="2" t="str">
+        <f>VLOOKUP(E69,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="2"/>
+      <c r="A70" s="1">
+        <v>0.58136892998400003</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0.96401415084000008</v>
+      </c>
+      <c r="C70" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F70" s="2" t="str">
+        <f>VLOOKUP(E70,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="2"/>
+      <c r="A71" s="1">
+        <v>1.069220984832</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1.720990009956</v>
+      </c>
+      <c r="C71" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E71" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F71" s="2" t="str">
+        <f>VLOOKUP(E71,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="2"/>
+      <c r="A72" s="1">
+        <v>1.6693740658710001</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1.2927640445000002</v>
+      </c>
+      <c r="C72" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E72" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F72" s="2" t="str">
+        <f>VLOOKUP(E72,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="2"/>
+      <c r="A73" s="1">
+        <v>1.8607376594879996</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1.0529268704799999</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E73" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F73" s="2" t="str">
+        <f>VLOOKUP(E73,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="2"/>
+      <c r="A74" s="1">
+        <v>0.80162900292599992</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1.190852098485</v>
+      </c>
+      <c r="C74" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D74" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E74" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F74" s="2" t="str">
+        <f>VLOOKUP(E74,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="2"/>
+      <c r="A75" s="1">
+        <v>0.92685719235599995</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.75150502328000002</v>
+      </c>
+      <c r="C75" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E75" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F75" s="2" t="str">
+        <f>VLOOKUP(E75,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="2"/>
+      <c r="A76" s="1">
+        <v>0.97932551976000026</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1.2535318389000001</v>
+      </c>
+      <c r="C76" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E76" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F76" s="2" t="str">
+        <f>VLOOKUP(E76,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="2"/>
+      <c r="A77" s="1">
+        <v>1.5591785863500003</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1.7093767504000001</v>
+      </c>
+      <c r="C77" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E77" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F77" s="2" t="str">
+        <f>VLOOKUP(E77,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="2"/>
+      <c r="A78" s="1">
+        <v>3.9936625397759999</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1.1312772163440001</v>
+      </c>
+      <c r="C78" s="3">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E78" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>4-1</v>
+      </c>
+      <c r="F78" s="2" t="str">
+        <f>VLOOKUP(E78,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="2"/>
+      <c r="A79" s="1">
+        <v>1.9885700317980002</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0.99455859448000028</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E79" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F79" s="2" t="str">
+        <f>VLOOKUP(E79,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="2"/>
+      <c r="A80" s="1">
+        <v>1.3557795680939999</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.6152906310320001</v>
+      </c>
+      <c r="C80" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D80" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E80" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F80" s="2" t="str">
+        <f>VLOOKUP(E80,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="2"/>
+      <c r="A81" s="1">
+        <v>1.280457093006</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1.0940277876000002</v>
+      </c>
+      <c r="C81" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E81" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F81" s="2" t="str">
+        <f>VLOOKUP(E81,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="2"/>
+      <c r="A82" s="1">
+        <v>1.54428693846</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.84674328245000008</v>
+      </c>
+      <c r="C82" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D82" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E82" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F82" s="2" t="str">
+        <f>VLOOKUP(E82,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="2"/>
+      <c r="A83" s="1">
+        <v>1.5441036029000001</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1.0583499376800001</v>
+      </c>
+      <c r="C83" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E83" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F83" s="2" t="str">
+        <f>VLOOKUP(E83,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="2"/>
+      <c r="A84" s="1">
+        <v>1.1323518488400002</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1.81445703264</v>
+      </c>
+      <c r="C84" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E84" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F84" s="2" t="str">
+        <f>VLOOKUP(E84,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="2"/>
+      <c r="A85" s="1">
+        <v>2.3667635417760002</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.239499042</v>
+      </c>
+      <c r="C85" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E85" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F85" s="2" t="str">
+        <f>VLOOKUP(E85,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="2"/>
+      <c r="A86" s="1">
+        <v>0.74315747030400003</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1.5683270599999999</v>
+      </c>
+      <c r="C86" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E86" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F86" s="2" t="str">
+        <f>VLOOKUP(E86,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="2"/>
+      <c r="A87" s="1">
+        <v>1.1147362054560002</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.57026438559999992</v>
+      </c>
+      <c r="C87" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D87" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E87" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F87" s="2" t="str">
+        <f>VLOOKUP(E87,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="2"/>
+      <c r="A88" s="1">
+        <v>0.51507344494399998</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1.8245885962499999</v>
+      </c>
+      <c r="C88" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D88" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E88" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F88" s="2" t="str">
+        <f>VLOOKUP(E88,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="2"/>
+      <c r="A89" s="1">
+        <v>1.216846011264</v>
+      </c>
+      <c r="B89" s="1">
+        <v>1.6841894737499998</v>
+      </c>
+      <c r="C89" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D89" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E89" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F89" s="2" t="str">
+        <f>VLOOKUP(E89,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="2"/>
+      <c r="A90" s="1">
+        <v>0.67595889920000019</v>
+      </c>
+      <c r="B90" s="1">
+        <v>1.146301171875</v>
+      </c>
+      <c r="C90" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E90" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F90" s="2" t="str">
+        <f>VLOOKUP(E90,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="2"/>
+      <c r="A91" s="1">
+        <v>0.93897068817600016</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.982493859375</v>
+      </c>
+      <c r="C91" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E91" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F91" s="2" t="str">
+        <f>VLOOKUP(E91,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="2"/>
+      <c r="A92" s="1">
+        <v>2.3965127612999999</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.21464248725000001</v>
+      </c>
+      <c r="C92" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E92" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-0</v>
+      </c>
+      <c r="F92" s="2" t="str">
+        <f>VLOOKUP(E92,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="2"/>
+      <c r="A93" s="1">
+        <v>2.9412042974999997</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.954125581</v>
+      </c>
+      <c r="C93" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E93" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F93" s="2" t="str">
+        <f>VLOOKUP(E93,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="2"/>
+      <c r="A94" s="1">
+        <v>3.2371732350000002</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.61654528750000004</v>
+      </c>
+      <c r="C94" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E94" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F94" s="2" t="str">
+        <f>VLOOKUP(E94,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="2"/>
+      <c r="A95" s="1">
+        <v>0.95530764239999999</v>
+      </c>
+      <c r="B95" s="1">
+        <v>1.8782669502499998</v>
+      </c>
+      <c r="C95" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E95" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F95" s="2" t="str">
+        <f>VLOOKUP(E95,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="2"/>
+      <c r="A96" s="1">
+        <v>1.2492372123</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1.2329828815000001</v>
+      </c>
+      <c r="C96" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E96" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F96" s="2" t="str">
+        <f>VLOOKUP(E96,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="2"/>
+      <c r="A97" s="1">
+        <v>2.1791791635900002</v>
+      </c>
+      <c r="B97" s="1">
+        <v>2.8536233281799999</v>
+      </c>
+      <c r="C97" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E97" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-3</v>
+      </c>
+      <c r="F97" s="2" t="str">
+        <f>VLOOKUP(E97,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="2"/>
+      <c r="A98" s="1">
+        <v>4.3302763558599997</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.64026495623999991</v>
+      </c>
+      <c r="C98" s="3">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E98" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>4-1</v>
+      </c>
+      <c r="F98" s="2" t="str">
+        <f>VLOOKUP(E98,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="2"/>
+      <c r="A99" s="1">
+        <v>1.3041936636300002</v>
+      </c>
+      <c r="B99" s="1">
+        <v>2.2127900885000003</v>
+      </c>
+      <c r="C99" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E99" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F99" s="2" t="str">
+        <f>VLOOKUP(E99,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="2"/>
+      <c r="A100" s="1">
+        <v>2.0438694777599999</v>
+      </c>
+      <c r="B100" s="1">
+        <v>1.4558281790600001</v>
+      </c>
+      <c r="C100" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D100" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E100" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F100" s="2" t="str">
+        <f>VLOOKUP(E100,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="2"/>
+      <c r="A101" s="1">
+        <v>2.4933920171519999</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.97828531358499993</v>
+      </c>
+      <c r="C101" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E101" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F101" s="2" t="str">
+        <f>VLOOKUP(E101,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="4"/>
-      <c r="F102" s="2"/>
+      <c r="A102" s="1">
+        <v>0.88817044070400009</v>
+      </c>
+      <c r="B102" s="1">
+        <v>1.7733935608379998</v>
+      </c>
+      <c r="C102" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E102" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F102" s="2" t="str">
+        <f>VLOOKUP(E102,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="2"/>
+      <c r="A103" s="1">
+        <v>1.689106284672</v>
+      </c>
+      <c r="B103" s="1">
+        <v>1.1049332142050001</v>
+      </c>
+      <c r="C103" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D103" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E103" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F103" s="2" t="str">
+        <f>VLOOKUP(E103,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="2"/>
+      <c r="A104" s="1">
+        <v>1.3200310679040002</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.52340619416999989</v>
+      </c>
+      <c r="C104" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D104" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E104" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F104" s="2" t="str">
+        <f>VLOOKUP(E104,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="2"/>
+      <c r="A105" s="1">
+        <v>2.043831979008</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.90307490367199994</v>
+      </c>
+      <c r="C105" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D105" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E105" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F105" s="2" t="str">
+        <f>VLOOKUP(E105,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="2"/>
+      <c r="A106" s="1">
+        <v>1.9587848094720002</v>
+      </c>
+      <c r="B106" s="1">
+        <v>1.7240998160960002</v>
+      </c>
+      <c r="C106" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D106" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E106" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F106" s="2" t="str">
+        <f>VLOOKUP(E106,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="2"/>
+      <c r="A107" s="1">
+        <v>1.4146779179520002</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.69787492555999997</v>
+      </c>
+      <c r="C107" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D107" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E107" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F107" s="2" t="str">
+        <f>VLOOKUP(E107,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="2"/>
+      <c r="A108" s="1">
+        <v>1.6606947302400001</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.97490614600999992</v>
+      </c>
+      <c r="C108" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D108" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E108" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F108" s="2" t="str">
+        <f>VLOOKUP(E108,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="2"/>
+      <c r="A109" s="1">
+        <v>2.0993301319680002</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.56194688357299993</v>
+      </c>
+      <c r="C109" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D109" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E109" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F109" s="2" t="str">
+        <f>VLOOKUP(E109,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="2"/>
+      <c r="A110" s="1">
+        <v>1.9302857579520001</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1.6523060737539998</v>
+      </c>
+      <c r="C110" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D110" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E110" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F110" s="2" t="str">
+        <f>VLOOKUP(E110,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="2"/>
+      <c r="A111" s="1">
+        <v>2.4981168599040005</v>
+      </c>
+      <c r="B111" s="1">
+        <v>1.3135498598880002</v>
+      </c>
+      <c r="C111" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D111" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E111" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-1</v>
+      </c>
+      <c r="F111" s="2" t="str">
+        <f>VLOOKUP(E111,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="2"/>
+      <c r="A112" s="1">
+        <v>0.96521787648000001</v>
+      </c>
+      <c r="B112" s="1">
+        <v>1.3135498598880002</v>
+      </c>
+      <c r="C112" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D112" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E112" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F112" s="2" t="str">
+        <f>VLOOKUP(E112,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="2"/>
+      <c r="A113" s="1">
+        <v>1.8187278647999998</v>
+      </c>
+      <c r="B113" s="1">
+        <v>1.5424441126400001</v>
+      </c>
+      <c r="C113" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D113" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E113" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>2-2</v>
+      </c>
+      <c r="F113" s="2" t="str">
+        <f>VLOOKUP(E113,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="2"/>
+      <c r="A114" s="1">
+        <v>0.75950805902999985</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0.62467986613999993</v>
+      </c>
+      <c r="C114" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D114" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E114" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-1</v>
+      </c>
+      <c r="F114" s="2" t="str">
+        <f>VLOOKUP(E114,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="4"/>
-      <c r="F115" s="2"/>
+      <c r="A115" s="1">
+        <v>0.49540480572000001</v>
+      </c>
+      <c r="B115" s="1">
+        <v>3.489032209146</v>
+      </c>
+      <c r="C115" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D115" s="3">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E115" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-3</v>
+      </c>
+      <c r="F115" s="2" t="str">
+        <f>VLOOKUP(E115,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="4"/>
-      <c r="F116" s="2"/>
+      <c r="A116" s="1">
+        <v>2.6111913864299998</v>
+      </c>
+      <c r="B116" s="1">
+        <v>0.72997441349999992</v>
+      </c>
+      <c r="C116" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D116" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E116" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>3-1</v>
+      </c>
+      <c r="F116" s="2" t="str">
+        <f>VLOOKUP(E116,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="2"/>
+      <c r="A117" s="1">
+        <v>0.43348074566400002</v>
+      </c>
+      <c r="B117" s="1">
+        <v>3.3266533599999999</v>
+      </c>
+      <c r="C117" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D117" s="3">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E117" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>0-3</v>
+      </c>
+      <c r="F117" s="2" t="str">
+        <f>VLOOKUP(E117,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="4"/>
-      <c r="F118" s="2"/>
+      <c r="A118" s="1">
+        <v>0.82862788238999996</v>
+      </c>
+      <c r="B118" s="1">
+        <v>2.0228638526549996</v>
+      </c>
+      <c r="C118" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D118" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E118" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>1-2</v>
+      </c>
+      <c r="F118" s="2" t="str">
+        <f>VLOOKUP(E118,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
@@ -3340,7 +4789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">

</xml_diff>

<commit_message>
updated myodds new leagues
</commit_message>
<xml_diff>
--- a/CS generator_newleagues.xlsx
+++ b/CS generator_newleagues.xlsx
@@ -559,22 +559,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F354"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1.03372565156</v>
+        <v>2.0599788175540001</v>
       </c>
       <c r="B1" s="1">
-        <v>1.5401279323979999</v>
+        <v>1.5264174314880001</v>
       </c>
       <c r="C1" s="3">
         <f>ROUND(A1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3">
         <f>ROUND(B1,0)</f>
@@ -582,23 +582,23 @@
       </c>
       <c r="E1" s="4" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>1-2</v>
+        <v>2-2</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>VLOOKUP(E1,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.1133508908899998</v>
+        <v>1.7114861604490001</v>
       </c>
       <c r="B2" s="1">
-        <v>1.017778188546</v>
+        <v>0.96461101573199992</v>
       </c>
       <c r="C2" s="3">
         <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2" si="1">ROUND(B2,0)</f>
@@ -606,43 +606,43 @@
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(E2,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.9741937326999999</v>
+        <v>0.51698056208400012</v>
       </c>
       <c r="B3" s="1">
-        <v>0.74644191963600004</v>
+        <v>0.89010434368800007</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C13" si="3">ROUND(A3,0)</f>
-        <v>2</v>
+        <f t="shared" ref="C3:C30" si="3">ROUND(A3,0)</f>
+        <v>1</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D13" si="4">ROUND(B3,0)</f>
+        <f t="shared" ref="D3:D30" si="4">ROUND(B3,0)</f>
         <v>1</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3:E13" si="5">CONCATENATE(C3,"-",D3)</f>
-        <v>2-1</v>
+        <f t="shared" ref="E3:E30" si="5">CONCATENATE(C3,"-",D3)</f>
+        <v>1-1</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>VLOOKUP(E3,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.1670730600320001</v>
+        <v>0.98688561606599989</v>
       </c>
       <c r="B4" s="1">
-        <v>0.61976074371199996</v>
+        <v>1.7802086873760001</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="3"/>
@@ -650,23 +650,23 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F4" s="2" t="str">
         <f>VLOOKUP(E4,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1.0268935946939999</v>
+        <v>0.64134129805199991</v>
       </c>
       <c r="B5" s="1">
-        <v>0.39011255738400002</v>
+        <v>1.5216906450899998</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="3"/>
@@ -674,27 +674,27 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-0</v>
+        <v>1-2</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>VLOOKUP(E5,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1.5920174054729999</v>
+        <v>1.4637469359799999</v>
       </c>
       <c r="B6" s="1">
-        <v>1.2665392987499999</v>
+        <v>1.3737490213680001</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="4"/>
@@ -702,47 +702,47 @@
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>VLOOKUP(E6,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1.8216237263399999</v>
+        <v>0.959790776304</v>
       </c>
       <c r="B7" s="1">
-        <v>1.1919636514500001</v>
+        <v>1.510991259516</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>VLOOKUP(E7,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.64061688199999989</v>
+        <v>2.2513192303710001</v>
       </c>
       <c r="B8" s="1">
-        <v>1.3559182060799999</v>
+        <v>1.3737934663200002</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="4"/>
@@ -750,23 +750,23 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>VLOOKUP(E8,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0.84231069648000012</v>
+        <v>0.48245252276400002</v>
       </c>
       <c r="B9" s="1">
-        <v>1.056469949304</v>
+        <v>0.70089542107200009</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="4"/>
@@ -774,19 +774,19 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>0-1</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>VLOOKUP(E9,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>0.59448576686400001</v>
+        <v>0.62656977042000006</v>
       </c>
       <c r="B10" s="1">
-        <v>1.5169611611220002</v>
+        <v>0.20226280620000001</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="3"/>
@@ -794,23 +794,23 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>1-0</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(E10,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0.81075726323899999</v>
+        <v>0.82703289779400002</v>
       </c>
       <c r="B11" s="1">
-        <v>1.12685794452</v>
+        <v>1.1571516472319998</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="3"/>
@@ -831,14 +831,14 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.2459762286289999</v>
+        <v>1.9249130937119998</v>
       </c>
       <c r="B12" s="1">
-        <v>0.55218066261600007</v>
+        <v>1.2062852598640001</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="4"/>
@@ -846,23 +846,23 @@
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>VLOOKUP(E12,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.92009871788999997</v>
+        <v>1.9249130937119998</v>
       </c>
       <c r="B13" s="1">
-        <v>1.5042416022479999</v>
+        <v>1.85703242322</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="4"/>
@@ -870,148 +870,420 @@
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>2-2</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>VLOOKUP(E13,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2.9459542338900002</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.89496863024999995</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F14" s="2" t="str">
+        <f>VLOOKUP(E14,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.92586149883000002</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.75017223417500001</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F15" s="2" t="str">
+        <f>VLOOKUP(E15,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.6272850838399999</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.2146574247649999</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2"/>
+      <c r="D16" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F16" s="2" t="str">
+        <f>VLOOKUP(E16,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="2"/>
+      <c r="A17" s="1">
+        <v>0.71096279747600011</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0303117660260002</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F17" s="2" t="str">
+        <f>VLOOKUP(E17,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="1">
+        <v>2.7810414022230003</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.76320871574400007</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F18" s="2" t="str">
+        <f>VLOOKUP(E18,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="2"/>
+      <c r="A19" s="1">
+        <v>1.0067565649699999</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.780820336736</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-2</v>
+      </c>
+      <c r="F19" s="2" t="str">
+        <f>VLOOKUP(E19,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="1">
+        <v>1.7230218683160001</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.89010434368800007</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F20" s="2" t="str">
+        <f>VLOOKUP(E20,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="2"/>
+      <c r="A21" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B21" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C21" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D21" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E21" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F21" s="2" t="e">
+        <f>VLOOKUP(E21,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="2"/>
+      <c r="A22" s="1">
+        <v>3.5669301409279996</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.85704829972800012</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>4-1</v>
+      </c>
+      <c r="F22" s="2" t="str">
+        <f>VLOOKUP(E22,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="2"/>
+      <c r="A23" s="1">
+        <v>1.6559624088</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.85704829972800012</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F23" s="2" t="str">
+        <f>VLOOKUP(E23,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="2"/>
+      <c r="A24" s="1">
+        <v>0.93432694555199991</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3.0474013594560003</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E24" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-3</v>
+      </c>
+      <c r="F24" s="2" t="str">
+        <f>VLOOKUP(E24,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="2"/>
+      <c r="A25" s="1">
+        <v>0.67779683625599996</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.74582254012500016</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F25" s="2" t="str">
+        <f>VLOOKUP(E25,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="2"/>
+      <c r="A26" s="1">
+        <v>2.1087672397919999</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.403944597575</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-1</v>
+      </c>
+      <c r="F26" s="2" t="str">
+        <f>VLOOKUP(E26,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="2"/>
+      <c r="A27" s="1">
+        <v>2.6717770378050001</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.0176116209920001</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>3-1</v>
+      </c>
+      <c r="F27" s="2" t="str">
+        <f>VLOOKUP(E27,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="2"/>
+      <c r="A28" s="1">
+        <v>2.0935957716360001</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.44500217160000005</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>2-0</v>
+      </c>
+      <c r="F28" s="2" t="str">
+        <f>VLOOKUP(E28,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="2"/>
+      <c r="A29" s="1">
+        <v>1.0592530249949998</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.97139950687999999</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F29" s="2" t="str">
+        <f>VLOOKUP(E29,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="2"/>
+      <c r="A30" s="1">
+        <v>0.73647826441199993</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.250357644795</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1-1</v>
+      </c>
+      <c r="F30" s="2" t="str">
+        <f>VLOOKUP(E30,cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>

</xml_diff>